<commit_message>
0.0.28-SNAPSHOT fix auto row height
</commit_message>
<xml_diff>
--- a/src/test/resources/ceping.xlsx
+++ b/src/test/resources/ceping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E611D32-6215-FA4A-AB45-6FA8D82EA613}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BA6A47-A071-E94E-B9DA-1D4245BF1B99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
@@ -2115,6 +2115,147 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2151,149 +2292,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2304,13 +2313,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2326,33 +2353,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6913,7 +6913,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7006,7 +7006,7 @@
       <c r="F6" s="82"/>
       <c r="G6" s="82"/>
     </row>
-    <row r="7" spans="1:7" s="35" customFormat="1" ht="40" customHeight="1">
+    <row r="7" spans="1:7" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A7" s="74"/>
       <c r="B7" s="37" t="s">
         <v>89</v>
@@ -7049,7 +7049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="40" t="s">
         <v>15</v>
       </c>
@@ -7554,162 +7554,162 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="92">
+      <c r="C5" s="139">
         <v>1.2</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="94"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="141"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="97"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="144"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="89"/>
-      <c r="B7" s="98" t="s">
+      <c r="A7" s="136"/>
+      <c r="B7" s="145" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="99"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="136"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="81"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="89"/>
-      <c r="B10" s="99"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="146"/>
       <c r="C10" s="81"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="100"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A11" s="89"/>
-      <c r="B11" s="99"/>
+      <c r="A11" s="136"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="81"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="134"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="89"/>
-      <c r="B12" s="99"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="81"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="131"/>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A13" s="89"/>
-      <c r="B13" s="99"/>
+      <c r="A13" s="136"/>
+      <c r="B13" s="146"/>
       <c r="C13" s="81"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="131"/>
+      <c r="G13" s="131"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A14" s="89"/>
-      <c r="B14" s="99"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="146"/>
       <c r="C14" s="81"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="134"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="99"/>
+      <c r="A15" s="136"/>
+      <c r="B15" s="146"/>
       <c r="C15" s="81"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
+      <c r="G15" s="134"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A16" s="89"/>
-      <c r="B16" s="99"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="146"/>
       <c r="C16" s="81"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="103"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="134"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A17" s="89"/>
-      <c r="B17" s="99"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="146"/>
       <c r="C17" s="81"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="134"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A18" s="89"/>
-      <c r="B18" s="99"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="146"/>
       <c r="C18" s="81"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="131"/>
+      <c r="G18" s="131"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A19" s="89"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="90" t="s">
+      <c r="A19" s="136"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
+      <c r="F19" s="131"/>
+      <c r="G19" s="131"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A20" s="89"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="131"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
       <c r="A21" s="75" t="s">
@@ -7742,548 +7742,548 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="109"/>
-      <c r="D23" s="110" t="s">
+      <c r="C23" s="130"/>
+      <c r="D23" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="111"/>
+      <c r="E23" s="112"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="106"/>
-      <c r="B24" s="112" t="s">
+      <c r="A24" s="127"/>
+      <c r="B24" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="113"/>
-      <c r="D24" s="110" t="s">
+      <c r="C24" s="121"/>
+      <c r="D24" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="111"/>
-      <c r="F24" s="118">
+      <c r="E24" s="112"/>
+      <c r="F24" s="97">
         <v>2</v>
       </c>
-      <c r="G24" s="121" t="s">
+      <c r="G24" s="88" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="106"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="110" t="s">
+      <c r="A25" s="127"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="111"/>
+      <c r="E25" s="112"/>
       <c r="F25" s="119"/>
-      <c r="G25" s="122"/>
+      <c r="G25" s="89"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="106"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="110" t="s">
+      <c r="A26" s="127"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="111"/>
+      <c r="E26" s="112"/>
       <c r="F26" s="119"/>
-      <c r="G26" s="122"/>
+      <c r="G26" s="89"/>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="106"/>
-      <c r="B27" s="114"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="110" t="s">
+      <c r="A27" s="127"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="111"/>
+      <c r="E27" s="112"/>
       <c r="F27" s="119"/>
-      <c r="G27" s="122"/>
+      <c r="G27" s="89"/>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="106"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="117"/>
-      <c r="D28" s="110" t="s">
+      <c r="A28" s="127"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="125"/>
+      <c r="D28" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="111"/>
-      <c r="F28" s="120"/>
-      <c r="G28" s="122"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="106"/>
-      <c r="B29" s="124" t="s">
+      <c r="A29" s="127"/>
+      <c r="B29" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="110" t="s">
+      <c r="C29" s="114"/>
+      <c r="D29" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="111"/>
-      <c r="F29" s="118">
+      <c r="E29" s="112"/>
+      <c r="F29" s="97">
         <v>2</v>
       </c>
-      <c r="G29" s="122"/>
+      <c r="G29" s="89"/>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="106"/>
-      <c r="B30" s="128"/>
-      <c r="C30" s="129"/>
-      <c r="D30" s="110" t="s">
+      <c r="A30" s="127"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="111"/>
+      <c r="E30" s="112"/>
       <c r="F30" s="119"/>
-      <c r="G30" s="122"/>
+      <c r="G30" s="89"/>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="106"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="129"/>
-      <c r="D31" s="110" t="s">
+      <c r="A31" s="127"/>
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="111"/>
+      <c r="E31" s="112"/>
       <c r="F31" s="119"/>
-      <c r="G31" s="122"/>
+      <c r="G31" s="89"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="106"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="129"/>
-      <c r="D32" s="110" t="s">
+      <c r="A32" s="127"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="111"/>
+      <c r="E32" s="112"/>
       <c r="F32" s="119"/>
-      <c r="G32" s="122"/>
+      <c r="G32" s="89"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="106"/>
-      <c r="B33" s="126"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="110" t="s">
+      <c r="A33" s="127"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="111"/>
-      <c r="F33" s="120"/>
-      <c r="G33" s="123"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="106"/>
-      <c r="B34" s="124" t="s">
+      <c r="A34" s="127"/>
+      <c r="B34" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="125"/>
-      <c r="D34" s="110" t="s">
+      <c r="C34" s="114"/>
+      <c r="D34" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="111"/>
-      <c r="F34" s="118">
+      <c r="E34" s="112"/>
+      <c r="F34" s="97">
         <v>0</v>
       </c>
-      <c r="G34" s="121" t="s">
+      <c r="G34" s="88" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="106"/>
-      <c r="B35" s="126"/>
-      <c r="C35" s="127"/>
-      <c r="D35" s="110" t="s">
+      <c r="A35" s="127"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="111"/>
-      <c r="F35" s="120"/>
-      <c r="G35" s="123"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="90"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="106"/>
-      <c r="B36" s="112" t="s">
+      <c r="A36" s="127"/>
+      <c r="B36" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="113"/>
-      <c r="D36" s="110" t="s">
+      <c r="C36" s="121"/>
+      <c r="D36" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="111"/>
-      <c r="F36" s="118">
+      <c r="E36" s="112"/>
+      <c r="F36" s="97">
         <v>2</v>
       </c>
-      <c r="G36" s="121" t="s">
+      <c r="G36" s="88" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="106"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="115"/>
-      <c r="D37" s="110" t="s">
+      <c r="A37" s="127"/>
+      <c r="B37" s="122"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="111"/>
+      <c r="E37" s="112"/>
       <c r="F37" s="119"/>
-      <c r="G37" s="122"/>
+      <c r="G37" s="89"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="106"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="110" t="s">
+      <c r="A38" s="127"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="111"/>
+      <c r="E38" s="112"/>
       <c r="F38" s="119"/>
-      <c r="G38" s="122"/>
+      <c r="G38" s="89"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="106"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="115"/>
-      <c r="D39" s="110" t="s">
+      <c r="A39" s="127"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="123"/>
+      <c r="D39" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="111"/>
+      <c r="E39" s="112"/>
       <c r="F39" s="119"/>
-      <c r="G39" s="122"/>
+      <c r="G39" s="89"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="106"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="117"/>
-      <c r="D40" s="110" t="s">
+      <c r="A40" s="127"/>
+      <c r="B40" s="124"/>
+      <c r="C40" s="125"/>
+      <c r="D40" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="111"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="122"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="89"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="106"/>
-      <c r="B41" s="124" t="s">
+      <c r="A41" s="127"/>
+      <c r="B41" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="125"/>
-      <c r="D41" s="110" t="s">
+      <c r="C41" s="114"/>
+      <c r="D41" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="111"/>
-      <c r="F41" s="118">
+      <c r="E41" s="112"/>
+      <c r="F41" s="97">
         <v>2</v>
       </c>
-      <c r="G41" s="122"/>
+      <c r="G41" s="89"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="106"/>
-      <c r="B42" s="128"/>
-      <c r="C42" s="129"/>
-      <c r="D42" s="110" t="s">
+      <c r="A42" s="127"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="111"/>
+      <c r="E42" s="112"/>
       <c r="F42" s="119"/>
-      <c r="G42" s="122"/>
+      <c r="G42" s="89"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="106"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="129"/>
-      <c r="D43" s="110" t="s">
+      <c r="A43" s="127"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
+      <c r="D43" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="111"/>
+      <c r="E43" s="112"/>
       <c r="F43" s="119"/>
-      <c r="G43" s="122"/>
+      <c r="G43" s="89"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="106"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="129"/>
-      <c r="D44" s="110" t="s">
+      <c r="A44" s="127"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="111"/>
+      <c r="E44" s="112"/>
       <c r="F44" s="119"/>
-      <c r="G44" s="122"/>
+      <c r="G44" s="89"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="106"/>
-      <c r="B45" s="126"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="110" t="s">
+      <c r="A45" s="127"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="111"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="122"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="89"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="106"/>
-      <c r="B46" s="124" t="s">
+      <c r="A46" s="127"/>
+      <c r="B46" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="125"/>
-      <c r="D46" s="110" t="s">
+      <c r="C46" s="114"/>
+      <c r="D46" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="111"/>
-      <c r="F46" s="118">
+      <c r="E46" s="112"/>
+      <c r="F46" s="97">
         <v>2</v>
       </c>
-      <c r="G46" s="122"/>
+      <c r="G46" s="89"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="106"/>
-      <c r="B47" s="128"/>
-      <c r="C47" s="129"/>
-      <c r="D47" s="110" t="s">
+      <c r="A47" s="127"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="118"/>
+      <c r="D47" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="111"/>
+      <c r="E47" s="112"/>
       <c r="F47" s="119"/>
-      <c r="G47" s="122"/>
+      <c r="G47" s="89"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="106"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="129"/>
-      <c r="D48" s="110" t="s">
+      <c r="A48" s="127"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="111"/>
+      <c r="E48" s="112"/>
       <c r="F48" s="119"/>
-      <c r="G48" s="122"/>
+      <c r="G48" s="89"/>
     </row>
     <row r="49" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="106"/>
-      <c r="B49" s="128"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="110" t="s">
+      <c r="A49" s="127"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="111"/>
+      <c r="E49" s="112"/>
       <c r="F49" s="119"/>
-      <c r="G49" s="122"/>
+      <c r="G49" s="89"/>
     </row>
     <row r="50" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="106"/>
-      <c r="B50" s="126"/>
-      <c r="C50" s="127"/>
-      <c r="D50" s="110" t="s">
+      <c r="A50" s="127"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="111"/>
-      <c r="F50" s="120"/>
-      <c r="G50" s="122"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="89"/>
     </row>
     <row r="51" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="106"/>
-      <c r="B51" s="124" t="s">
+      <c r="A51" s="127"/>
+      <c r="B51" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="125"/>
-      <c r="D51" s="110" t="s">
+      <c r="C51" s="114"/>
+      <c r="D51" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="111"/>
-      <c r="F51" s="118">
+      <c r="E51" s="112"/>
+      <c r="F51" s="97">
         <v>2</v>
       </c>
-      <c r="G51" s="122"/>
+      <c r="G51" s="89"/>
     </row>
     <row r="52" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A52" s="106"/>
-      <c r="B52" s="128"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="110" t="s">
+      <c r="A52" s="127"/>
+      <c r="B52" s="117"/>
+      <c r="C52" s="118"/>
+      <c r="D52" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="E52" s="111"/>
+      <c r="E52" s="112"/>
       <c r="F52" s="119"/>
-      <c r="G52" s="122"/>
+      <c r="G52" s="89"/>
     </row>
     <row r="53" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A53" s="106"/>
-      <c r="B53" s="128"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="110" t="s">
+      <c r="A53" s="127"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
+      <c r="D53" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E53" s="111"/>
+      <c r="E53" s="112"/>
       <c r="F53" s="119"/>
-      <c r="G53" s="122"/>
+      <c r="G53" s="89"/>
     </row>
     <row r="54" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A54" s="106"/>
-      <c r="B54" s="128"/>
-      <c r="C54" s="129"/>
-      <c r="D54" s="110" t="s">
+      <c r="A54" s="127"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="118"/>
+      <c r="D54" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="E54" s="111"/>
+      <c r="E54" s="112"/>
       <c r="F54" s="119"/>
-      <c r="G54" s="122"/>
+      <c r="G54" s="89"/>
     </row>
     <row r="55" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A55" s="106"/>
-      <c r="B55" s="126"/>
-      <c r="C55" s="127"/>
-      <c r="D55" s="110" t="s">
+      <c r="A55" s="127"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="E55" s="111"/>
-      <c r="F55" s="120"/>
-      <c r="G55" s="123"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="98"/>
+      <c r="G55" s="90"/>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A56" s="106"/>
-      <c r="B56" s="124" t="s">
+      <c r="A56" s="127"/>
+      <c r="B56" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="125"/>
-      <c r="D56" s="110" t="s">
+      <c r="C56" s="114"/>
+      <c r="D56" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="111"/>
-      <c r="F56" s="118">
+      <c r="E56" s="112"/>
+      <c r="F56" s="97">
         <v>0</v>
       </c>
-      <c r="G56" s="121" t="s">
+      <c r="G56" s="88" t="s">
         <v>34</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A57" s="106"/>
-      <c r="B57" s="126"/>
-      <c r="C57" s="127"/>
-      <c r="D57" s="110" t="s">
+      <c r="A57" s="127"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="116"/>
+      <c r="D57" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="111"/>
-      <c r="F57" s="120"/>
-      <c r="G57" s="123"/>
+      <c r="E57" s="112"/>
+      <c r="F57" s="98"/>
+      <c r="G57" s="90"/>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A58" s="106"/>
-      <c r="B58" s="124" t="s">
+      <c r="A58" s="127"/>
+      <c r="B58" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="125"/>
-      <c r="D58" s="110" t="s">
+      <c r="C58" s="114"/>
+      <c r="D58" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="111"/>
-      <c r="F58" s="118">
+      <c r="E58" s="112"/>
+      <c r="F58" s="97">
         <v>0</v>
       </c>
-      <c r="G58" s="121" t="s">
+      <c r="G58" s="88" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A59" s="106"/>
-      <c r="B59" s="126"/>
-      <c r="C59" s="127"/>
-      <c r="D59" s="110" t="s">
+      <c r="A59" s="127"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="116"/>
+      <c r="D59" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="111"/>
-      <c r="F59" s="120"/>
-      <c r="G59" s="122"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="98"/>
+      <c r="G59" s="89"/>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A60" s="106"/>
-      <c r="B60" s="124" t="s">
+      <c r="A60" s="127"/>
+      <c r="B60" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="125"/>
-      <c r="D60" s="110" t="s">
+      <c r="C60" s="114"/>
+      <c r="D60" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="111"/>
-      <c r="F60" s="118">
+      <c r="E60" s="112"/>
+      <c r="F60" s="97">
         <v>0</v>
       </c>
-      <c r="G60" s="122"/>
+      <c r="G60" s="89"/>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A61" s="106"/>
-      <c r="B61" s="128"/>
-      <c r="C61" s="129"/>
-      <c r="D61" s="110" t="s">
+      <c r="A61" s="127"/>
+      <c r="B61" s="117"/>
+      <c r="C61" s="118"/>
+      <c r="D61" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="111"/>
+      <c r="E61" s="112"/>
       <c r="F61" s="119"/>
-      <c r="G61" s="122"/>
+      <c r="G61" s="89"/>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A62" s="106"/>
-      <c r="B62" s="128"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="110" t="s">
+      <c r="A62" s="127"/>
+      <c r="B62" s="117"/>
+      <c r="C62" s="118"/>
+      <c r="D62" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="111"/>
+      <c r="E62" s="112"/>
       <c r="F62" s="119"/>
-      <c r="G62" s="122"/>
+      <c r="G62" s="89"/>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A63" s="106"/>
-      <c r="B63" s="128"/>
-      <c r="C63" s="129"/>
-      <c r="D63" s="110" t="s">
+      <c r="A63" s="127"/>
+      <c r="B63" s="117"/>
+      <c r="C63" s="118"/>
+      <c r="D63" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="111"/>
+      <c r="E63" s="112"/>
       <c r="F63" s="119"/>
-      <c r="G63" s="122"/>
+      <c r="G63" s="89"/>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A64" s="106"/>
-      <c r="B64" s="128"/>
-      <c r="C64" s="129"/>
-      <c r="D64" s="110" t="s">
+      <c r="A64" s="127"/>
+      <c r="B64" s="117"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="111"/>
+      <c r="E64" s="112"/>
       <c r="F64" s="119"/>
-      <c r="G64" s="122"/>
+      <c r="G64" s="89"/>
     </row>
     <row r="65" spans="1:7" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A65" s="107"/>
-      <c r="B65" s="126"/>
-      <c r="C65" s="127"/>
-      <c r="D65" s="110" t="s">
+      <c r="A65" s="128"/>
+      <c r="B65" s="115"/>
+      <c r="C65" s="116"/>
+      <c r="D65" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="111"/>
-      <c r="F65" s="120"/>
-      <c r="G65" s="123"/>
+      <c r="E65" s="112"/>
+      <c r="F65" s="98"/>
+      <c r="G65" s="90"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A66" s="130" t="s">
+      <c r="A66" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="131" t="s">
+      <c r="B66" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="131"/>
-      <c r="D66" s="131" t="s">
+      <c r="C66" s="100"/>
+      <c r="D66" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="131"/>
+      <c r="E66" s="100"/>
       <c r="F66" s="17">
         <v>0</v>
       </c>
@@ -8292,15 +8292,15 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A67" s="130"/>
-      <c r="B67" s="132" t="s">
+      <c r="A67" s="99"/>
+      <c r="B67" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="132"/>
-      <c r="D67" s="133" t="s">
+      <c r="C67" s="101"/>
+      <c r="D67" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E67" s="133"/>
+      <c r="E67" s="95"/>
       <c r="F67" s="26">
         <v>0</v>
       </c>
@@ -8309,127 +8309,180 @@
       </c>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A68" s="130"/>
-      <c r="B68" s="134" t="s">
+      <c r="A68" s="99"/>
+      <c r="B68" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="135"/>
-      <c r="D68" s="140" t="s">
+      <c r="C68" s="103"/>
+      <c r="D68" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="E68" s="141"/>
-      <c r="F68" s="143">
+      <c r="E68" s="92"/>
+      <c r="F68" s="108">
         <v>0</v>
       </c>
-      <c r="G68" s="121" t="s">
+      <c r="G68" s="88" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A69" s="130"/>
-      <c r="B69" s="136"/>
-      <c r="C69" s="137"/>
-      <c r="D69" s="140" t="s">
+      <c r="A69" s="99"/>
+      <c r="B69" s="104"/>
+      <c r="C69" s="105"/>
+      <c r="D69" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="E69" s="141"/>
-      <c r="F69" s="144"/>
-      <c r="G69" s="122"/>
+      <c r="E69" s="92"/>
+      <c r="F69" s="109"/>
+      <c r="G69" s="89"/>
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A70" s="130"/>
-      <c r="B70" s="136"/>
-      <c r="C70" s="137"/>
-      <c r="D70" s="140" t="s">
+      <c r="A70" s="99"/>
+      <c r="B70" s="104"/>
+      <c r="C70" s="105"/>
+      <c r="D70" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="E70" s="141"/>
-      <c r="F70" s="144"/>
-      <c r="G70" s="122"/>
+      <c r="E70" s="92"/>
+      <c r="F70" s="109"/>
+      <c r="G70" s="89"/>
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A71" s="130"/>
-      <c r="B71" s="138"/>
-      <c r="C71" s="139"/>
-      <c r="D71" s="140" t="s">
+      <c r="A71" s="99"/>
+      <c r="B71" s="106"/>
+      <c r="C71" s="107"/>
+      <c r="D71" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="E71" s="141"/>
-      <c r="F71" s="145"/>
-      <c r="G71" s="123"/>
+      <c r="E71" s="92"/>
+      <c r="F71" s="110"/>
+      <c r="G71" s="90"/>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A72" s="130"/>
-      <c r="B72" s="142" t="s">
+      <c r="A72" s="99"/>
+      <c r="B72" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="142"/>
-      <c r="D72" s="142" t="s">
+      <c r="C72" s="93"/>
+      <c r="D72" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="142"/>
-      <c r="F72" s="146">
+      <c r="E72" s="93"/>
+      <c r="F72" s="94">
         <v>0</v>
       </c>
-      <c r="G72" s="133" t="s">
+      <c r="G72" s="95" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A73" s="130"/>
-      <c r="B73" s="142"/>
-      <c r="C73" s="142"/>
-      <c r="D73" s="147" t="s">
+      <c r="A73" s="99"/>
+      <c r="B73" s="93"/>
+      <c r="C73" s="93"/>
+      <c r="D73" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="E73" s="147"/>
-      <c r="F73" s="146"/>
-      <c r="G73" s="133"/>
+      <c r="E73" s="96"/>
+      <c r="F73" s="94"/>
+      <c r="G73" s="95"/>
     </row>
     <row r="74" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A74" s="130"/>
-      <c r="B74" s="142"/>
-      <c r="C74" s="142"/>
-      <c r="D74" s="142" t="s">
+      <c r="A74" s="99"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="93"/>
+      <c r="D74" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="E74" s="142"/>
-      <c r="F74" s="146"/>
-      <c r="G74" s="133"/>
+      <c r="E74" s="93"/>
+      <c r="F74" s="94"/>
+      <c r="G74" s="95"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A75" s="130"/>
-      <c r="B75" s="142"/>
-      <c r="C75" s="142"/>
-      <c r="D75" s="142" t="s">
+      <c r="A75" s="99"/>
+      <c r="B75" s="93"/>
+      <c r="C75" s="93"/>
+      <c r="D75" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="142"/>
-      <c r="F75" s="146"/>
-      <c r="G75" s="133"/>
+      <c r="E75" s="93"/>
+      <c r="F75" s="94"/>
+      <c r="G75" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="B72:C75"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="A66:A75"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C71"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B7:B20"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="C8:C18"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:A65"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B24:C28"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="G24:G33"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:C40"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G36:G55"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B58:C59"/>
@@ -8454,79 +8507,26 @@
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="B56:C57"/>
     <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:C40"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="G36:G55"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:F45"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:A65"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B24:C28"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="G24:G33"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="C8:C18"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:A20"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B7:B20"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="A66:A75"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C71"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="B72:C75"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="D73:E73"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F66">
@@ -8664,19 +8664,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="92">
+      <c r="C5" s="139">
         <v>6</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="94"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="141"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -8688,13 +8688,13 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="151"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
-      <c r="G6" s="153"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="150"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -8739,17 +8739,17 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110" t="s">
+      <c r="C9" s="130"/>
+      <c r="D9" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="111"/>
+      <c r="E9" s="112"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
         <v>18</v>
@@ -8759,19 +8759,19 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="106"/>
-      <c r="B10" s="112" t="s">
+      <c r="A10" s="127"/>
+      <c r="B10" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="110" t="s">
+      <c r="C10" s="121"/>
+      <c r="D10" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="111"/>
-      <c r="F10" s="118">
+      <c r="E10" s="112"/>
+      <c r="F10" s="97">
         <v>2</v>
       </c>
-      <c r="G10" s="148" t="s">
+      <c r="G10" s="151" t="s">
         <v>21</v>
       </c>
       <c r="K10" s="4"/>
@@ -8780,79 +8780,79 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A11" s="106"/>
-      <c r="B11" s="114"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="110" t="s">
+      <c r="A11" s="127"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="111"/>
+      <c r="E11" s="112"/>
       <c r="F11" s="119"/>
-      <c r="G11" s="149"/>
+      <c r="G11" s="152"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="106"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="110" t="s">
+      <c r="A12" s="127"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="111"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="119"/>
-      <c r="G12" s="149"/>
+      <c r="G12" s="152"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="106"/>
-      <c r="B13" s="114"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="110" t="s">
+      <c r="A13" s="127"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="111"/>
+      <c r="E13" s="112"/>
       <c r="F13" s="119"/>
-      <c r="G13" s="149"/>
+      <c r="G13" s="152"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="106"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="110" t="s">
+      <c r="A14" s="127"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="111"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="149"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="152"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="106"/>
-      <c r="B15" s="124" t="s">
+      <c r="A15" s="127"/>
+      <c r="B15" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="125"/>
-      <c r="D15" s="110" t="s">
+      <c r="C15" s="114"/>
+      <c r="D15" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="111"/>
-      <c r="F15" s="118">
+      <c r="E15" s="112"/>
+      <c r="F15" s="97">
         <v>2</v>
       </c>
-      <c r="G15" s="149"/>
+      <c r="G15" s="152"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -8862,15 +8862,15 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A16" s="106"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="110" t="s">
+      <c r="A16" s="127"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="111"/>
+      <c r="E16" s="112"/>
       <c r="F16" s="119"/>
-      <c r="G16" s="149"/>
+      <c r="G16" s="152"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -8880,15 +8880,15 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="106"/>
-      <c r="B17" s="128"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="110" t="s">
+      <c r="A17" s="127"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="111"/>
+      <c r="E17" s="112"/>
       <c r="F17" s="119"/>
-      <c r="G17" s="149"/>
+      <c r="G17" s="152"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -8898,15 +8898,15 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A18" s="106"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="110" t="s">
+      <c r="A18" s="127"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="111"/>
+      <c r="E18" s="112"/>
       <c r="F18" s="119"/>
-      <c r="G18" s="149"/>
+      <c r="G18" s="152"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -8916,15 +8916,15 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A19" s="106"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="110" t="s">
+      <c r="A19" s="127"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="111"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="150"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="153"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -8934,19 +8934,19 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A20" s="106"/>
-      <c r="B20" s="124" t="s">
+      <c r="A20" s="127"/>
+      <c r="B20" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="125"/>
-      <c r="D20" s="110" t="s">
+      <c r="C20" s="114"/>
+      <c r="D20" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="111"/>
-      <c r="F20" s="118">
+      <c r="E20" s="112"/>
+      <c r="F20" s="97">
         <v>0</v>
       </c>
-      <c r="G20" s="148" t="s">
+      <c r="G20" s="151" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="4"/>
@@ -8955,34 +8955,34 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A21" s="106"/>
-      <c r="B21" s="126"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="110" t="s">
+      <c r="A21" s="127"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="150"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="153"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A22" s="106"/>
-      <c r="B22" s="112" t="s">
+      <c r="A22" s="127"/>
+      <c r="B22" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="113"/>
-      <c r="D22" s="110" t="s">
+      <c r="C22" s="121"/>
+      <c r="D22" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="111"/>
-      <c r="F22" s="118">
+      <c r="E22" s="112"/>
+      <c r="F22" s="97">
         <v>2</v>
       </c>
-      <c r="G22" s="121" t="s">
+      <c r="G22" s="88" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="4"/>
@@ -8991,79 +8991,79 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="106"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="110" t="s">
+      <c r="A23" s="127"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="111"/>
+      <c r="E23" s="112"/>
       <c r="F23" s="119"/>
-      <c r="G23" s="122"/>
+      <c r="G23" s="89"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="106"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="115"/>
-      <c r="D24" s="110" t="s">
+      <c r="A24" s="127"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="111"/>
+      <c r="E24" s="112"/>
       <c r="F24" s="119"/>
-      <c r="G24" s="122"/>
+      <c r="G24" s="89"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="106"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="110" t="s">
+      <c r="A25" s="127"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="111"/>
+      <c r="E25" s="112"/>
       <c r="F25" s="119"/>
-      <c r="G25" s="122"/>
+      <c r="G25" s="89"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="106"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="110" t="s">
+      <c r="A26" s="127"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="122"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="89"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="106"/>
-      <c r="B27" s="124" t="s">
+      <c r="A27" s="127"/>
+      <c r="B27" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="125"/>
-      <c r="D27" s="110" t="s">
+      <c r="C27" s="114"/>
+      <c r="D27" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="111"/>
-      <c r="F27" s="118">
+      <c r="E27" s="112"/>
+      <c r="F27" s="97">
         <v>2</v>
       </c>
-      <c r="G27" s="122"/>
+      <c r="G27" s="89"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
@@ -9073,15 +9073,15 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="106"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="129"/>
-      <c r="D28" s="110" t="s">
+      <c r="A28" s="127"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="111"/>
+      <c r="E28" s="112"/>
       <c r="F28" s="119"/>
-      <c r="G28" s="122"/>
+      <c r="G28" s="89"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -9090,15 +9090,15 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="106"/>
-      <c r="B29" s="128"/>
-      <c r="C29" s="129"/>
-      <c r="D29" s="110" t="s">
+      <c r="A29" s="127"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="111"/>
+      <c r="E29" s="112"/>
       <c r="F29" s="119"/>
-      <c r="G29" s="122"/>
+      <c r="G29" s="89"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -9107,15 +9107,15 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="106"/>
-      <c r="B30" s="128"/>
-      <c r="C30" s="129"/>
-      <c r="D30" s="110" t="s">
+      <c r="A30" s="127"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="111"/>
+      <c r="E30" s="112"/>
       <c r="F30" s="119"/>
-      <c r="G30" s="122"/>
+      <c r="G30" s="89"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -9124,15 +9124,15 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="106"/>
-      <c r="B31" s="126"/>
-      <c r="C31" s="127"/>
-      <c r="D31" s="110" t="s">
+      <c r="A31" s="127"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="111"/>
-      <c r="F31" s="120"/>
-      <c r="G31" s="122"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="89"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -9141,19 +9141,19 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="106"/>
-      <c r="B32" s="124" t="s">
+      <c r="A32" s="127"/>
+      <c r="B32" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="125"/>
-      <c r="D32" s="110" t="s">
+      <c r="C32" s="114"/>
+      <c r="D32" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="111"/>
-      <c r="F32" s="118">
+      <c r="E32" s="112"/>
+      <c r="F32" s="97">
         <v>2</v>
       </c>
-      <c r="G32" s="122" t="s">
+      <c r="G32" s="89" t="s">
         <v>49</v>
       </c>
       <c r="H32" s="19"/>
@@ -9165,15 +9165,15 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="106"/>
-      <c r="B33" s="128"/>
-      <c r="C33" s="129"/>
-      <c r="D33" s="110" t="s">
+      <c r="A33" s="127"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="111"/>
+      <c r="E33" s="112"/>
       <c r="F33" s="119"/>
-      <c r="G33" s="122"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -9183,15 +9183,15 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="106"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="129"/>
-      <c r="D34" s="110" t="s">
+      <c r="A34" s="127"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="111"/>
+      <c r="E34" s="112"/>
       <c r="F34" s="119"/>
-      <c r="G34" s="122"/>
+      <c r="G34" s="89"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -9201,15 +9201,15 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="106"/>
-      <c r="B35" s="128"/>
-      <c r="C35" s="129"/>
-      <c r="D35" s="110" t="s">
+      <c r="A35" s="127"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="111"/>
+      <c r="E35" s="112"/>
       <c r="F35" s="119"/>
-      <c r="G35" s="122"/>
+      <c r="G35" s="89"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -9219,15 +9219,15 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="106"/>
-      <c r="B36" s="126"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="110" t="s">
+      <c r="A36" s="127"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="111"/>
-      <c r="F36" s="120"/>
-      <c r="G36" s="122"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -9237,98 +9237,98 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="106"/>
-      <c r="B37" s="124" t="s">
+      <c r="A37" s="127"/>
+      <c r="B37" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="125"/>
-      <c r="D37" s="110" t="s">
+      <c r="C37" s="114"/>
+      <c r="D37" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="111"/>
-      <c r="F37" s="118">
+      <c r="E37" s="112"/>
+      <c r="F37" s="97">
         <v>2</v>
       </c>
-      <c r="G37" s="122"/>
+      <c r="G37" s="89"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="106"/>
-      <c r="B38" s="128"/>
-      <c r="C38" s="129"/>
-      <c r="D38" s="110" t="s">
+      <c r="A38" s="127"/>
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="111"/>
+      <c r="E38" s="112"/>
       <c r="F38" s="119"/>
-      <c r="G38" s="122"/>
+      <c r="G38" s="89"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="106"/>
-      <c r="B39" s="128"/>
-      <c r="C39" s="129"/>
-      <c r="D39" s="110" t="s">
+      <c r="A39" s="127"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="111"/>
+      <c r="E39" s="112"/>
       <c r="F39" s="119"/>
-      <c r="G39" s="122"/>
+      <c r="G39" s="89"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="106"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="110" t="s">
+      <c r="A40" s="127"/>
+      <c r="B40" s="117"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="111"/>
+      <c r="E40" s="112"/>
       <c r="F40" s="119"/>
-      <c r="G40" s="122"/>
+      <c r="G40" s="89"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="106"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="127"/>
-      <c r="D41" s="110" t="s">
+      <c r="A41" s="127"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="111"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="123"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="90"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="106"/>
-      <c r="B42" s="124" t="s">
+      <c r="A42" s="127"/>
+      <c r="B42" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="125"/>
-      <c r="D42" s="110" t="s">
+      <c r="C42" s="114"/>
+      <c r="D42" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="111"/>
-      <c r="F42" s="118">
+      <c r="E42" s="112"/>
+      <c r="F42" s="97">
         <v>0</v>
       </c>
-      <c r="G42" s="121" t="s">
+      <c r="G42" s="88" t="s">
         <v>34</v>
       </c>
       <c r="K42" s="21"/>
@@ -9338,34 +9338,34 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="106"/>
-      <c r="B43" s="126"/>
-      <c r="C43" s="127"/>
-      <c r="D43" s="110" t="s">
+      <c r="A43" s="127"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="111"/>
-      <c r="F43" s="120"/>
-      <c r="G43" s="123"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="90"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
     </row>
     <row r="44" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="106"/>
-      <c r="B44" s="124" t="s">
+      <c r="A44" s="127"/>
+      <c r="B44" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="125"/>
-      <c r="D44" s="110" t="s">
+      <c r="C44" s="114"/>
+      <c r="D44" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="111"/>
-      <c r="F44" s="118">
+      <c r="E44" s="112"/>
+      <c r="F44" s="97">
         <v>0</v>
       </c>
-      <c r="G44" s="121" t="s">
+      <c r="G44" s="88" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="8"/>
@@ -9377,15 +9377,15 @@
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="106"/>
-      <c r="B45" s="126"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="110" t="s">
+      <c r="A45" s="127"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="111"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="122"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -9395,111 +9395,111 @@
       <c r="N45" s="21"/>
     </row>
     <row r="46" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="106"/>
-      <c r="B46" s="124" t="s">
+      <c r="A46" s="127"/>
+      <c r="B46" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="125"/>
-      <c r="D46" s="110" t="s">
+      <c r="C46" s="114"/>
+      <c r="D46" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="111"/>
-      <c r="F46" s="118">
+      <c r="E46" s="112"/>
+      <c r="F46" s="97">
         <v>0</v>
       </c>
-      <c r="G46" s="122"/>
+      <c r="G46" s="89"/>
       <c r="K46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="106"/>
-      <c r="B47" s="128"/>
-      <c r="C47" s="129"/>
-      <c r="D47" s="110" t="s">
+      <c r="A47" s="127"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="118"/>
+      <c r="D47" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="111"/>
+      <c r="E47" s="112"/>
       <c r="F47" s="119"/>
-      <c r="G47" s="122"/>
+      <c r="G47" s="89"/>
       <c r="K47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="106"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="129"/>
-      <c r="D48" s="110" t="s">
+      <c r="A48" s="127"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="E48" s="111"/>
+      <c r="E48" s="112"/>
       <c r="F48" s="119"/>
-      <c r="G48" s="122"/>
+      <c r="G48" s="89"/>
       <c r="K48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
     </row>
     <row r="49" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="106"/>
-      <c r="B49" s="128"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="110" t="s">
+      <c r="A49" s="127"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="111"/>
+      <c r="E49" s="112"/>
       <c r="F49" s="119"/>
-      <c r="G49" s="122"/>
+      <c r="G49" s="89"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
     </row>
     <row r="50" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="106"/>
-      <c r="B50" s="128"/>
-      <c r="C50" s="129"/>
-      <c r="D50" s="110" t="s">
+      <c r="A50" s="127"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="111"/>
+      <c r="E50" s="112"/>
       <c r="F50" s="119"/>
-      <c r="G50" s="122"/>
+      <c r="G50" s="89"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
     </row>
     <row r="51" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="107"/>
-      <c r="B51" s="126"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="110" t="s">
+      <c r="A51" s="128"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="111"/>
-      <c r="F51" s="120"/>
-      <c r="G51" s="123"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="98"/>
+      <c r="G51" s="90"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
     </row>
     <row r="52" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A52" s="130" t="s">
+      <c r="A52" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="131" t="s">
+      <c r="B52" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="131"/>
-      <c r="D52" s="131" t="s">
+      <c r="C52" s="100"/>
+      <c r="D52" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="131"/>
+      <c r="E52" s="100"/>
       <c r="F52" s="17">
         <v>0</v>
       </c>
@@ -9511,15 +9511,15 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="1:16" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A53" s="130"/>
-      <c r="B53" s="132" t="s">
+      <c r="A53" s="99"/>
+      <c r="B53" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="132"/>
-      <c r="D53" s="133" t="s">
+      <c r="C53" s="101"/>
+      <c r="D53" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="133"/>
+      <c r="E53" s="95"/>
       <c r="F53" s="26">
         <v>0</v>
       </c>
@@ -9531,19 +9531,19 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="130"/>
-      <c r="B54" s="134" t="s">
+      <c r="A54" s="99"/>
+      <c r="B54" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="135"/>
-      <c r="D54" s="140" t="s">
+      <c r="C54" s="103"/>
+      <c r="D54" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="141"/>
-      <c r="F54" s="143">
+      <c r="E54" s="92"/>
+      <c r="F54" s="108">
         <v>0</v>
       </c>
-      <c r="G54" s="121" t="s">
+      <c r="G54" s="88" t="s">
         <v>79</v>
       </c>
       <c r="K54" s="4"/>
@@ -9552,30 +9552,30 @@
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="130"/>
-      <c r="B55" s="136"/>
-      <c r="C55" s="137"/>
-      <c r="D55" s="140" t="s">
+      <c r="A55" s="99"/>
+      <c r="B55" s="104"/>
+      <c r="C55" s="105"/>
+      <c r="D55" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="141"/>
-      <c r="F55" s="144"/>
-      <c r="G55" s="122"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="109"/>
+      <c r="G55" s="89"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="130"/>
-      <c r="B56" s="136"/>
-      <c r="C56" s="137"/>
-      <c r="D56" s="140" t="s">
+      <c r="A56" s="99"/>
+      <c r="B56" s="104"/>
+      <c r="C56" s="105"/>
+      <c r="D56" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="141"/>
-      <c r="F56" s="144"/>
-      <c r="G56" s="122"/>
+      <c r="E56" s="92"/>
+      <c r="F56" s="109"/>
+      <c r="G56" s="89"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -9583,15 +9583,15 @@
       <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="130"/>
-      <c r="B57" s="138"/>
-      <c r="C57" s="139"/>
-      <c r="D57" s="140" t="s">
+      <c r="A57" s="99"/>
+      <c r="B57" s="106"/>
+      <c r="C57" s="107"/>
+      <c r="D57" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="141"/>
-      <c r="F57" s="145"/>
-      <c r="G57" s="123"/>
+      <c r="E57" s="92"/>
+      <c r="F57" s="110"/>
+      <c r="G57" s="90"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="3"/>
@@ -9601,19 +9601,19 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="130"/>
-      <c r="B58" s="142" t="s">
+      <c r="A58" s="99"/>
+      <c r="B58" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="142"/>
-      <c r="D58" s="142" t="s">
+      <c r="C58" s="93"/>
+      <c r="D58" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="E58" s="142"/>
-      <c r="F58" s="146">
+      <c r="E58" s="93"/>
+      <c r="F58" s="94">
         <v>0</v>
       </c>
-      <c r="G58" s="133" t="s">
+      <c r="G58" s="95" t="s">
         <v>85</v>
       </c>
       <c r="K58" s="4"/>
@@ -9622,44 +9622,44 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="130"/>
-      <c r="B59" s="142"/>
-      <c r="C59" s="142"/>
-      <c r="D59" s="147" t="s">
+      <c r="A59" s="99"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="147"/>
-      <c r="F59" s="146"/>
-      <c r="G59" s="133"/>
+      <c r="E59" s="96"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="95"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="130"/>
-      <c r="B60" s="142"/>
-      <c r="C60" s="142"/>
-      <c r="D60" s="142" t="s">
+      <c r="A60" s="99"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="E60" s="142"/>
-      <c r="F60" s="146"/>
-      <c r="G60" s="133"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="95"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
     <row r="61" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="130"/>
-      <c r="B61" s="142"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="142" t="s">
+      <c r="A61" s="99"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="142"/>
-      <c r="F61" s="146"/>
-      <c r="G61" s="133"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="94"/>
+      <c r="G61" s="95"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -9677,15 +9677,74 @@
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B58:C61"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B54:C57"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="B44:C45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B46:C51"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:F51"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G32:G41"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C41"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G10:G19"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="G22:G31"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B27:C31"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A9:A51"/>
@@ -9710,74 +9769,15 @@
     <mergeCell ref="B42:C43"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G10:G19"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="G22:G31"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C31"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C41"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B44:C45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B46:C51"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:F51"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:A61"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B54:C57"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B58:C61"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F52">
@@ -9841,262 +9841,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:248" s="48" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="154" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="160" t="s">
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="161" t="s">
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="156" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="161"/>
-      <c r="P1" s="161"/>
-      <c r="Q1" s="161"/>
-      <c r="R1" s="161"/>
-      <c r="S1" s="161"/>
-      <c r="T1" s="161"/>
-      <c r="U1" s="161"/>
-      <c r="V1" s="161"/>
-      <c r="W1" s="161"/>
-      <c r="X1" s="161"/>
-      <c r="Y1" s="161"/>
-      <c r="Z1" s="161"/>
-      <c r="AA1" s="161"/>
-      <c r="AB1" s="161"/>
-      <c r="AC1" s="161"/>
-      <c r="AD1" s="161"/>
-      <c r="AE1" s="161"/>
-      <c r="AF1" s="161"/>
-      <c r="AG1" s="161"/>
-      <c r="AH1" s="161"/>
-      <c r="AI1" s="161"/>
-      <c r="AJ1" s="161"/>
-      <c r="AK1" s="161"/>
-      <c r="AL1" s="161"/>
-      <c r="AM1" s="161"/>
-      <c r="AN1" s="162" t="s">
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
+      <c r="Q1" s="156"/>
+      <c r="R1" s="156"/>
+      <c r="S1" s="156"/>
+      <c r="T1" s="156"/>
+      <c r="U1" s="156"/>
+      <c r="V1" s="156"/>
+      <c r="W1" s="156"/>
+      <c r="X1" s="156"/>
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="156"/>
+      <c r="AA1" s="156"/>
+      <c r="AB1" s="156"/>
+      <c r="AC1" s="156"/>
+      <c r="AD1" s="156"/>
+      <c r="AE1" s="156"/>
+      <c r="AF1" s="156"/>
+      <c r="AG1" s="156"/>
+      <c r="AH1" s="156"/>
+      <c r="AI1" s="156"/>
+      <c r="AJ1" s="156"/>
+      <c r="AK1" s="156"/>
+      <c r="AL1" s="156"/>
+      <c r="AM1" s="156"/>
+      <c r="AN1" s="157" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="162"/>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
-      <c r="AZ1" s="162"/>
-      <c r="BA1" s="162"/>
-      <c r="BB1" s="162"/>
-      <c r="BC1" s="162"/>
-      <c r="BD1" s="162"/>
-      <c r="BE1" s="162"/>
-      <c r="BF1" s="162"/>
-      <c r="BG1" s="162"/>
-      <c r="BH1" s="162"/>
-      <c r="BI1" s="162"/>
-      <c r="BJ1" s="162"/>
-      <c r="BK1" s="162"/>
-      <c r="BL1" s="162"/>
-      <c r="BM1" s="162"/>
-      <c r="BN1" s="162"/>
-      <c r="BO1" s="162"/>
-      <c r="BP1" s="162"/>
-      <c r="BQ1" s="162"/>
-      <c r="BR1" s="162"/>
-      <c r="BS1" s="162"/>
-      <c r="BT1" s="162"/>
-      <c r="BU1" s="162"/>
-      <c r="BV1" s="162"/>
-      <c r="BW1" s="162"/>
-      <c r="BX1" s="162"/>
-      <c r="BY1" s="162"/>
-      <c r="BZ1" s="162"/>
-      <c r="CA1" s="162"/>
-      <c r="CB1" s="162"/>
-      <c r="CC1" s="162"/>
-      <c r="CD1" s="162"/>
-      <c r="CE1" s="162"/>
-      <c r="CF1" s="162"/>
-      <c r="CG1" s="162"/>
-      <c r="CH1" s="162"/>
-      <c r="CI1" s="162"/>
-      <c r="CJ1" s="162"/>
-      <c r="CK1" s="162"/>
-      <c r="CL1" s="162"/>
-      <c r="CM1" s="162"/>
-      <c r="CN1" s="162"/>
-      <c r="CO1" s="162"/>
-      <c r="CP1" s="162"/>
-      <c r="CQ1" s="162"/>
-      <c r="CR1" s="162"/>
-      <c r="CS1" s="162"/>
-      <c r="CT1" s="162"/>
-      <c r="CU1" s="162"/>
-      <c r="CV1" s="162"/>
-      <c r="CW1" s="162"/>
-      <c r="CX1" s="162"/>
-      <c r="CY1" s="162"/>
-      <c r="CZ1" s="162"/>
-      <c r="DA1" s="162"/>
-      <c r="DB1" s="162"/>
-      <c r="DC1" s="162"/>
-      <c r="DD1" s="162"/>
-      <c r="DE1" s="162"/>
-      <c r="DF1" s="162"/>
-      <c r="DG1" s="162"/>
-      <c r="DH1" s="162"/>
-      <c r="DI1" s="162"/>
-      <c r="DJ1" s="162"/>
-      <c r="DK1" s="162"/>
-      <c r="DL1" s="162"/>
-      <c r="DM1" s="162"/>
-      <c r="DN1" s="162"/>
-      <c r="DO1" s="162"/>
-      <c r="DP1" s="162"/>
-      <c r="DQ1" s="162"/>
-      <c r="DR1" s="162"/>
-      <c r="DS1" s="162"/>
-      <c r="DT1" s="162"/>
-      <c r="DU1" s="162"/>
-      <c r="DV1" s="162"/>
-      <c r="DW1" s="162"/>
-      <c r="DX1" s="162"/>
-      <c r="DY1" s="162"/>
-      <c r="DZ1" s="162"/>
-      <c r="EA1" s="162"/>
-      <c r="EB1" s="162"/>
-      <c r="EC1" s="162"/>
-      <c r="ED1" s="162"/>
-      <c r="EE1" s="162"/>
-      <c r="EF1" s="162"/>
-      <c r="EG1" s="162"/>
-      <c r="EH1" s="162"/>
-      <c r="EI1" s="162"/>
-      <c r="EJ1" s="162"/>
-      <c r="EK1" s="162"/>
-      <c r="EL1" s="162"/>
-      <c r="EM1" s="162"/>
-      <c r="EN1" s="162"/>
-      <c r="EO1" s="162"/>
-      <c r="EP1" s="162"/>
-      <c r="EQ1" s="162"/>
-      <c r="ER1" s="162"/>
-      <c r="ES1" s="162"/>
-      <c r="ET1" s="162"/>
-      <c r="EU1" s="162"/>
-      <c r="EV1" s="162"/>
-      <c r="EW1" s="162"/>
-      <c r="EX1" s="162"/>
-      <c r="EY1" s="162"/>
-      <c r="EZ1" s="162"/>
-      <c r="FA1" s="162"/>
-      <c r="FB1" s="162"/>
-      <c r="FC1" s="162"/>
-      <c r="FD1" s="162"/>
-      <c r="FE1" s="162"/>
-      <c r="FF1" s="162"/>
-      <c r="FG1" s="162"/>
-      <c r="FH1" s="162"/>
-      <c r="FI1" s="162"/>
-      <c r="FJ1" s="162"/>
-      <c r="FK1" s="162"/>
-      <c r="FL1" s="162"/>
-      <c r="FM1" s="162"/>
-      <c r="FN1" s="162"/>
-      <c r="FO1" s="162"/>
-      <c r="FP1" s="162"/>
-      <c r="FQ1" s="162"/>
-      <c r="FR1" s="162"/>
-      <c r="FS1" s="162"/>
-      <c r="FT1" s="162"/>
-      <c r="FU1" s="162"/>
-      <c r="FV1" s="162"/>
-      <c r="FW1" s="162"/>
-      <c r="FX1" s="162"/>
-      <c r="FY1" s="162"/>
-      <c r="FZ1" s="162"/>
-      <c r="GA1" s="162"/>
-      <c r="GB1" s="162"/>
-      <c r="GC1" s="162"/>
-      <c r="GD1" s="162"/>
-      <c r="GE1" s="162"/>
-      <c r="GF1" s="162"/>
-      <c r="GG1" s="162"/>
-      <c r="GH1" s="162"/>
-      <c r="GI1" s="162"/>
-      <c r="GJ1" s="162"/>
-      <c r="GK1" s="162"/>
-      <c r="GL1" s="162"/>
-      <c r="GM1" s="162"/>
-      <c r="GN1" s="162"/>
-      <c r="GO1" s="162"/>
-      <c r="GP1" s="162"/>
-      <c r="GQ1" s="162"/>
-      <c r="GR1" s="162"/>
-      <c r="GS1" s="162"/>
-      <c r="GT1" s="162"/>
-      <c r="GU1" s="162"/>
-      <c r="GV1" s="162"/>
-      <c r="GW1" s="162"/>
-      <c r="GX1" s="162"/>
-      <c r="GY1" s="162"/>
-      <c r="GZ1" s="162"/>
-      <c r="HA1" s="162"/>
-      <c r="HB1" s="162"/>
-      <c r="HC1" s="162"/>
-      <c r="HD1" s="162"/>
-      <c r="HE1" s="162"/>
-      <c r="HF1" s="162"/>
-      <c r="HG1" s="162"/>
-      <c r="HH1" s="162"/>
-      <c r="HI1" s="162"/>
-      <c r="HJ1" s="162"/>
-      <c r="HK1" s="162"/>
-      <c r="HL1" s="162"/>
-      <c r="HM1" s="162"/>
-      <c r="HN1" s="162"/>
-      <c r="HO1" s="162"/>
-      <c r="HP1" s="162"/>
-      <c r="HQ1" s="162"/>
-      <c r="HR1" s="162"/>
-      <c r="HS1" s="162"/>
-      <c r="HT1" s="162"/>
-      <c r="HU1" s="162"/>
-      <c r="HV1" s="162"/>
-      <c r="HW1" s="162"/>
-      <c r="HX1" s="162"/>
-      <c r="HY1" s="162"/>
-      <c r="HZ1" s="162"/>
-      <c r="IA1" s="162"/>
-      <c r="IB1" s="162"/>
-      <c r="IC1" s="162"/>
-      <c r="ID1" s="162"/>
-      <c r="IE1" s="162"/>
-      <c r="IF1" s="162"/>
-      <c r="IG1" s="162"/>
-      <c r="IH1" s="162"/>
-      <c r="II1" s="162"/>
-      <c r="IJ1" s="162"/>
-      <c r="IK1" s="162"/>
-      <c r="IL1" s="162"/>
-      <c r="IM1" s="162"/>
-      <c r="IN1" s="162"/>
+      <c r="AO1" s="157"/>
+      <c r="AP1" s="157"/>
+      <c r="AQ1" s="157"/>
+      <c r="AR1" s="157"/>
+      <c r="AS1" s="157"/>
+      <c r="AT1" s="157"/>
+      <c r="AU1" s="157"/>
+      <c r="AV1" s="157"/>
+      <c r="AW1" s="157"/>
+      <c r="AX1" s="157"/>
+      <c r="AY1" s="157"/>
+      <c r="AZ1" s="157"/>
+      <c r="BA1" s="157"/>
+      <c r="BB1" s="157"/>
+      <c r="BC1" s="157"/>
+      <c r="BD1" s="157"/>
+      <c r="BE1" s="157"/>
+      <c r="BF1" s="157"/>
+      <c r="BG1" s="157"/>
+      <c r="BH1" s="157"/>
+      <c r="BI1" s="157"/>
+      <c r="BJ1" s="157"/>
+      <c r="BK1" s="157"/>
+      <c r="BL1" s="157"/>
+      <c r="BM1" s="157"/>
+      <c r="BN1" s="157"/>
+      <c r="BO1" s="157"/>
+      <c r="BP1" s="157"/>
+      <c r="BQ1" s="157"/>
+      <c r="BR1" s="157"/>
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="157"/>
+      <c r="BU1" s="157"/>
+      <c r="BV1" s="157"/>
+      <c r="BW1" s="157"/>
+      <c r="BX1" s="157"/>
+      <c r="BY1" s="157"/>
+      <c r="BZ1" s="157"/>
+      <c r="CA1" s="157"/>
+      <c r="CB1" s="157"/>
+      <c r="CC1" s="157"/>
+      <c r="CD1" s="157"/>
+      <c r="CE1" s="157"/>
+      <c r="CF1" s="157"/>
+      <c r="CG1" s="157"/>
+      <c r="CH1" s="157"/>
+      <c r="CI1" s="157"/>
+      <c r="CJ1" s="157"/>
+      <c r="CK1" s="157"/>
+      <c r="CL1" s="157"/>
+      <c r="CM1" s="157"/>
+      <c r="CN1" s="157"/>
+      <c r="CO1" s="157"/>
+      <c r="CP1" s="157"/>
+      <c r="CQ1" s="157"/>
+      <c r="CR1" s="157"/>
+      <c r="CS1" s="157"/>
+      <c r="CT1" s="157"/>
+      <c r="CU1" s="157"/>
+      <c r="CV1" s="157"/>
+      <c r="CW1" s="157"/>
+      <c r="CX1" s="157"/>
+      <c r="CY1" s="157"/>
+      <c r="CZ1" s="157"/>
+      <c r="DA1" s="157"/>
+      <c r="DB1" s="157"/>
+      <c r="DC1" s="157"/>
+      <c r="DD1" s="157"/>
+      <c r="DE1" s="157"/>
+      <c r="DF1" s="157"/>
+      <c r="DG1" s="157"/>
+      <c r="DH1" s="157"/>
+      <c r="DI1" s="157"/>
+      <c r="DJ1" s="157"/>
+      <c r="DK1" s="157"/>
+      <c r="DL1" s="157"/>
+      <c r="DM1" s="157"/>
+      <c r="DN1" s="157"/>
+      <c r="DO1" s="157"/>
+      <c r="DP1" s="157"/>
+      <c r="DQ1" s="157"/>
+      <c r="DR1" s="157"/>
+      <c r="DS1" s="157"/>
+      <c r="DT1" s="157"/>
+      <c r="DU1" s="157"/>
+      <c r="DV1" s="157"/>
+      <c r="DW1" s="157"/>
+      <c r="DX1" s="157"/>
+      <c r="DY1" s="157"/>
+      <c r="DZ1" s="157"/>
+      <c r="EA1" s="157"/>
+      <c r="EB1" s="157"/>
+      <c r="EC1" s="157"/>
+      <c r="ED1" s="157"/>
+      <c r="EE1" s="157"/>
+      <c r="EF1" s="157"/>
+      <c r="EG1" s="157"/>
+      <c r="EH1" s="157"/>
+      <c r="EI1" s="157"/>
+      <c r="EJ1" s="157"/>
+      <c r="EK1" s="157"/>
+      <c r="EL1" s="157"/>
+      <c r="EM1" s="157"/>
+      <c r="EN1" s="157"/>
+      <c r="EO1" s="157"/>
+      <c r="EP1" s="157"/>
+      <c r="EQ1" s="157"/>
+      <c r="ER1" s="157"/>
+      <c r="ES1" s="157"/>
+      <c r="ET1" s="157"/>
+      <c r="EU1" s="157"/>
+      <c r="EV1" s="157"/>
+      <c r="EW1" s="157"/>
+      <c r="EX1" s="157"/>
+      <c r="EY1" s="157"/>
+      <c r="EZ1" s="157"/>
+      <c r="FA1" s="157"/>
+      <c r="FB1" s="157"/>
+      <c r="FC1" s="157"/>
+      <c r="FD1" s="157"/>
+      <c r="FE1" s="157"/>
+      <c r="FF1" s="157"/>
+      <c r="FG1" s="157"/>
+      <c r="FH1" s="157"/>
+      <c r="FI1" s="157"/>
+      <c r="FJ1" s="157"/>
+      <c r="FK1" s="157"/>
+      <c r="FL1" s="157"/>
+      <c r="FM1" s="157"/>
+      <c r="FN1" s="157"/>
+      <c r="FO1" s="157"/>
+      <c r="FP1" s="157"/>
+      <c r="FQ1" s="157"/>
+      <c r="FR1" s="157"/>
+      <c r="FS1" s="157"/>
+      <c r="FT1" s="157"/>
+      <c r="FU1" s="157"/>
+      <c r="FV1" s="157"/>
+      <c r="FW1" s="157"/>
+      <c r="FX1" s="157"/>
+      <c r="FY1" s="157"/>
+      <c r="FZ1" s="157"/>
+      <c r="GA1" s="157"/>
+      <c r="GB1" s="157"/>
+      <c r="GC1" s="157"/>
+      <c r="GD1" s="157"/>
+      <c r="GE1" s="157"/>
+      <c r="GF1" s="157"/>
+      <c r="GG1" s="157"/>
+      <c r="GH1" s="157"/>
+      <c r="GI1" s="157"/>
+      <c r="GJ1" s="157"/>
+      <c r="GK1" s="157"/>
+      <c r="GL1" s="157"/>
+      <c r="GM1" s="157"/>
+      <c r="GN1" s="157"/>
+      <c r="GO1" s="157"/>
+      <c r="GP1" s="157"/>
+      <c r="GQ1" s="157"/>
+      <c r="GR1" s="157"/>
+      <c r="GS1" s="157"/>
+      <c r="GT1" s="157"/>
+      <c r="GU1" s="157"/>
+      <c r="GV1" s="157"/>
+      <c r="GW1" s="157"/>
+      <c r="GX1" s="157"/>
+      <c r="GY1" s="157"/>
+      <c r="GZ1" s="157"/>
+      <c r="HA1" s="157"/>
+      <c r="HB1" s="157"/>
+      <c r="HC1" s="157"/>
+      <c r="HD1" s="157"/>
+      <c r="HE1" s="157"/>
+      <c r="HF1" s="157"/>
+      <c r="HG1" s="157"/>
+      <c r="HH1" s="157"/>
+      <c r="HI1" s="157"/>
+      <c r="HJ1" s="157"/>
+      <c r="HK1" s="157"/>
+      <c r="HL1" s="157"/>
+      <c r="HM1" s="157"/>
+      <c r="HN1" s="157"/>
+      <c r="HO1" s="157"/>
+      <c r="HP1" s="157"/>
+      <c r="HQ1" s="157"/>
+      <c r="HR1" s="157"/>
+      <c r="HS1" s="157"/>
+      <c r="HT1" s="157"/>
+      <c r="HU1" s="157"/>
+      <c r="HV1" s="157"/>
+      <c r="HW1" s="157"/>
+      <c r="HX1" s="157"/>
+      <c r="HY1" s="157"/>
+      <c r="HZ1" s="157"/>
+      <c r="IA1" s="157"/>
+      <c r="IB1" s="157"/>
+      <c r="IC1" s="157"/>
+      <c r="ID1" s="157"/>
+      <c r="IE1" s="157"/>
+      <c r="IF1" s="157"/>
+      <c r="IG1" s="157"/>
+      <c r="IH1" s="157"/>
+      <c r="II1" s="157"/>
+      <c r="IJ1" s="157"/>
+      <c r="IK1" s="157"/>
+      <c r="IL1" s="157"/>
+      <c r="IM1" s="157"/>
+      <c r="IN1" s="157"/>
     </row>
     <row r="2" spans="1:248" s="48" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="49"/>
@@ -10107,274 +10107,274 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
-      <c r="U2" s="163"/>
-      <c r="V2" s="163" t="s">
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="158"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="158"/>
+      <c r="T2" s="158"/>
+      <c r="U2" s="158"/>
+      <c r="V2" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="W2" s="163"/>
-      <c r="X2" s="163"/>
-      <c r="Y2" s="163"/>
-      <c r="Z2" s="163"/>
-      <c r="AA2" s="163"/>
-      <c r="AB2" s="163"/>
-      <c r="AC2" s="163" t="s">
+      <c r="W2" s="158"/>
+      <c r="X2" s="158"/>
+      <c r="Y2" s="158"/>
+      <c r="Z2" s="158"/>
+      <c r="AA2" s="158"/>
+      <c r="AB2" s="158"/>
+      <c r="AC2" s="158" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="163"/>
-      <c r="AE2" s="163"/>
-      <c r="AF2" s="163"/>
-      <c r="AG2" s="163"/>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="163" t="s">
+      <c r="AD2" s="158"/>
+      <c r="AE2" s="158"/>
+      <c r="AF2" s="158"/>
+      <c r="AG2" s="158"/>
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="163"/>
-      <c r="AK2" s="163"/>
-      <c r="AL2" s="163"/>
-      <c r="AM2" s="163"/>
+      <c r="AJ2" s="158"/>
+      <c r="AK2" s="158"/>
+      <c r="AL2" s="158"/>
+      <c r="AM2" s="158"/>
       <c r="AN2" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="164" t="s">
+      <c r="AO2" s="159" t="s">
         <v>335</v>
       </c>
-      <c r="AP2" s="164"/>
-      <c r="AQ2" s="164"/>
-      <c r="AR2" s="164"/>
-      <c r="AS2" s="164"/>
-      <c r="AT2" s="164"/>
-      <c r="AU2" s="164"/>
-      <c r="AV2" s="164"/>
-      <c r="AW2" s="164"/>
-      <c r="AX2" s="164"/>
-      <c r="AY2" s="164"/>
-      <c r="AZ2" s="164"/>
-      <c r="BA2" s="164"/>
-      <c r="BB2" s="164"/>
-      <c r="BC2" s="164"/>
-      <c r="BD2" s="164"/>
-      <c r="BE2" s="164"/>
-      <c r="BF2" s="164"/>
-      <c r="BG2" s="164"/>
-      <c r="BH2" s="164"/>
-      <c r="BI2" s="165" t="s">
+      <c r="AP2" s="159"/>
+      <c r="AQ2" s="159"/>
+      <c r="AR2" s="159"/>
+      <c r="AS2" s="159"/>
+      <c r="AT2" s="159"/>
+      <c r="AU2" s="159"/>
+      <c r="AV2" s="159"/>
+      <c r="AW2" s="159"/>
+      <c r="AX2" s="159"/>
+      <c r="AY2" s="159"/>
+      <c r="AZ2" s="159"/>
+      <c r="BA2" s="159"/>
+      <c r="BB2" s="159"/>
+      <c r="BC2" s="159"/>
+      <c r="BD2" s="159"/>
+      <c r="BE2" s="159"/>
+      <c r="BF2" s="159"/>
+      <c r="BG2" s="159"/>
+      <c r="BH2" s="159"/>
+      <c r="BI2" s="160" t="s">
         <v>334</v>
       </c>
-      <c r="BJ2" s="165"/>
-      <c r="BK2" s="165"/>
-      <c r="BL2" s="165"/>
-      <c r="BM2" s="165"/>
-      <c r="BN2" s="165"/>
-      <c r="BO2" s="165"/>
-      <c r="BP2" s="165"/>
-      <c r="BQ2" s="165"/>
-      <c r="BR2" s="165"/>
-      <c r="BS2" s="165"/>
-      <c r="BT2" s="165"/>
-      <c r="BU2" s="165"/>
-      <c r="BV2" s="165"/>
-      <c r="BW2" s="165"/>
-      <c r="BX2" s="165"/>
-      <c r="BY2" s="167" t="s">
+      <c r="BJ2" s="160"/>
+      <c r="BK2" s="160"/>
+      <c r="BL2" s="160"/>
+      <c r="BM2" s="160"/>
+      <c r="BN2" s="160"/>
+      <c r="BO2" s="160"/>
+      <c r="BP2" s="160"/>
+      <c r="BQ2" s="160"/>
+      <c r="BR2" s="160"/>
+      <c r="BS2" s="160"/>
+      <c r="BT2" s="160"/>
+      <c r="BU2" s="160"/>
+      <c r="BV2" s="160"/>
+      <c r="BW2" s="160"/>
+      <c r="BX2" s="160"/>
+      <c r="BY2" s="162" t="s">
         <v>333</v>
       </c>
-      <c r="BZ2" s="167"/>
-      <c r="CA2" s="167"/>
-      <c r="CB2" s="167"/>
-      <c r="CC2" s="167"/>
-      <c r="CD2" s="167"/>
-      <c r="CE2" s="167"/>
-      <c r="CF2" s="167"/>
-      <c r="CG2" s="167"/>
-      <c r="CH2" s="167"/>
-      <c r="CI2" s="167"/>
-      <c r="CJ2" s="154" t="s">
+      <c r="BZ2" s="162"/>
+      <c r="CA2" s="162"/>
+      <c r="CB2" s="162"/>
+      <c r="CC2" s="162"/>
+      <c r="CD2" s="162"/>
+      <c r="CE2" s="162"/>
+      <c r="CF2" s="162"/>
+      <c r="CG2" s="162"/>
+      <c r="CH2" s="162"/>
+      <c r="CI2" s="162"/>
+      <c r="CJ2" s="163" t="s">
         <v>332</v>
       </c>
-      <c r="CK2" s="154"/>
-      <c r="CL2" s="154"/>
-      <c r="CM2" s="154"/>
-      <c r="CN2" s="154"/>
-      <c r="CO2" s="154"/>
-      <c r="CP2" s="154"/>
-      <c r="CQ2" s="154"/>
-      <c r="CR2" s="154"/>
-      <c r="CS2" s="154"/>
-      <c r="CT2" s="154"/>
-      <c r="CU2" s="154"/>
-      <c r="CV2" s="154"/>
-      <c r="CW2" s="154"/>
-      <c r="CX2" s="154"/>
-      <c r="CY2" s="154"/>
-      <c r="CZ2" s="154"/>
-      <c r="DA2" s="154"/>
-      <c r="DB2" s="154"/>
-      <c r="DC2" s="154"/>
-      <c r="DD2" s="154"/>
-      <c r="DE2" s="155" t="s">
+      <c r="CK2" s="163"/>
+      <c r="CL2" s="163"/>
+      <c r="CM2" s="163"/>
+      <c r="CN2" s="163"/>
+      <c r="CO2" s="163"/>
+      <c r="CP2" s="163"/>
+      <c r="CQ2" s="163"/>
+      <c r="CR2" s="163"/>
+      <c r="CS2" s="163"/>
+      <c r="CT2" s="163"/>
+      <c r="CU2" s="163"/>
+      <c r="CV2" s="163"/>
+      <c r="CW2" s="163"/>
+      <c r="CX2" s="163"/>
+      <c r="CY2" s="163"/>
+      <c r="CZ2" s="163"/>
+      <c r="DA2" s="163"/>
+      <c r="DB2" s="163"/>
+      <c r="DC2" s="163"/>
+      <c r="DD2" s="163"/>
+      <c r="DE2" s="164" t="s">
         <v>331</v>
       </c>
-      <c r="DF2" s="155"/>
-      <c r="DG2" s="155"/>
-      <c r="DH2" s="155"/>
-      <c r="DI2" s="155"/>
-      <c r="DJ2" s="156" t="s">
+      <c r="DF2" s="164"/>
+      <c r="DG2" s="164"/>
+      <c r="DH2" s="164"/>
+      <c r="DI2" s="164"/>
+      <c r="DJ2" s="165" t="s">
         <v>330</v>
       </c>
-      <c r="DK2" s="156"/>
-      <c r="DL2" s="156"/>
-      <c r="DM2" s="156"/>
-      <c r="DN2" s="157" t="s">
+      <c r="DK2" s="165"/>
+      <c r="DL2" s="165"/>
+      <c r="DM2" s="165"/>
+      <c r="DN2" s="166" t="s">
         <v>329</v>
       </c>
-      <c r="DO2" s="157"/>
-      <c r="DP2" s="157"/>
-      <c r="DQ2" s="157"/>
-      <c r="DR2" s="157"/>
-      <c r="DS2" s="157"/>
-      <c r="DT2" s="158" t="s">
+      <c r="DO2" s="166"/>
+      <c r="DP2" s="166"/>
+      <c r="DQ2" s="166"/>
+      <c r="DR2" s="166"/>
+      <c r="DS2" s="166"/>
+      <c r="DT2" s="167" t="s">
         <v>328</v>
       </c>
-      <c r="DU2" s="158"/>
-      <c r="DV2" s="158"/>
-      <c r="DW2" s="158"/>
-      <c r="DX2" s="158"/>
-      <c r="DY2" s="158"/>
-      <c r="DZ2" s="158"/>
-      <c r="EA2" s="158"/>
-      <c r="EB2" s="158"/>
-      <c r="EC2" s="158"/>
-      <c r="ED2" s="158"/>
-      <c r="EE2" s="158"/>
-      <c r="EF2" s="158"/>
-      <c r="EG2" s="158"/>
-      <c r="EH2" s="158"/>
-      <c r="EI2" s="158"/>
-      <c r="EJ2" s="158"/>
-      <c r="EK2" s="158"/>
-      <c r="EL2" s="158"/>
-      <c r="EM2" s="158"/>
-      <c r="EN2" s="158"/>
-      <c r="EO2" s="166" t="s">
+      <c r="DU2" s="167"/>
+      <c r="DV2" s="167"/>
+      <c r="DW2" s="167"/>
+      <c r="DX2" s="167"/>
+      <c r="DY2" s="167"/>
+      <c r="DZ2" s="167"/>
+      <c r="EA2" s="167"/>
+      <c r="EB2" s="167"/>
+      <c r="EC2" s="167"/>
+      <c r="ED2" s="167"/>
+      <c r="EE2" s="167"/>
+      <c r="EF2" s="167"/>
+      <c r="EG2" s="167"/>
+      <c r="EH2" s="167"/>
+      <c r="EI2" s="167"/>
+      <c r="EJ2" s="167"/>
+      <c r="EK2" s="167"/>
+      <c r="EL2" s="167"/>
+      <c r="EM2" s="167"/>
+      <c r="EN2" s="167"/>
+      <c r="EO2" s="161" t="s">
         <v>336</v>
       </c>
-      <c r="EP2" s="166"/>
-      <c r="EQ2" s="166"/>
-      <c r="ER2" s="166"/>
-      <c r="ES2" s="166"/>
-      <c r="ET2" s="166"/>
-      <c r="EU2" s="166"/>
-      <c r="EV2" s="166"/>
-      <c r="EW2" s="166"/>
-      <c r="EX2" s="166"/>
-      <c r="EY2" s="166"/>
-      <c r="EZ2" s="166"/>
-      <c r="FA2" s="166"/>
-      <c r="FB2" s="166"/>
-      <c r="FC2" s="166"/>
-      <c r="FD2" s="166"/>
-      <c r="FE2" s="166"/>
-      <c r="FF2" s="166"/>
-      <c r="FG2" s="166"/>
-      <c r="FH2" s="166"/>
-      <c r="FI2" s="166"/>
-      <c r="FJ2" s="166"/>
-      <c r="FK2" s="166"/>
-      <c r="FL2" s="166"/>
-      <c r="FM2" s="166"/>
-      <c r="FN2" s="166"/>
-      <c r="FO2" s="166"/>
-      <c r="FP2" s="166"/>
-      <c r="FQ2" s="166"/>
-      <c r="FR2" s="166"/>
-      <c r="FS2" s="166"/>
-      <c r="FT2" s="166"/>
-      <c r="FU2" s="166"/>
-      <c r="FV2" s="166"/>
-      <c r="FW2" s="166"/>
-      <c r="FX2" s="166"/>
-      <c r="FY2" s="166"/>
-      <c r="FZ2" s="166"/>
-      <c r="GA2" s="166"/>
-      <c r="GB2" s="166"/>
-      <c r="GC2" s="166"/>
-      <c r="GD2" s="166"/>
-      <c r="GE2" s="166"/>
-      <c r="GF2" s="166"/>
-      <c r="GG2" s="166"/>
-      <c r="GH2" s="166"/>
-      <c r="GI2" s="166"/>
-      <c r="GJ2" s="166"/>
-      <c r="GK2" s="166"/>
-      <c r="GL2" s="166"/>
-      <c r="GM2" s="166"/>
-      <c r="GN2" s="166"/>
-      <c r="GO2" s="166"/>
-      <c r="GP2" s="166"/>
-      <c r="GQ2" s="166"/>
-      <c r="GR2" s="166"/>
-      <c r="GS2" s="166"/>
-      <c r="GT2" s="166"/>
-      <c r="GU2" s="166"/>
-      <c r="GV2" s="166"/>
-      <c r="GW2" s="166"/>
-      <c r="GX2" s="166"/>
-      <c r="GY2" s="166"/>
-      <c r="GZ2" s="166"/>
-      <c r="HA2" s="166"/>
-      <c r="HB2" s="166"/>
-      <c r="HC2" s="166"/>
-      <c r="HD2" s="166"/>
-      <c r="HE2" s="166"/>
-      <c r="HF2" s="166"/>
-      <c r="HG2" s="166"/>
-      <c r="HH2" s="166"/>
-      <c r="HI2" s="166"/>
-      <c r="HJ2" s="166"/>
-      <c r="HK2" s="166"/>
-      <c r="HL2" s="166"/>
-      <c r="HM2" s="166"/>
-      <c r="HN2" s="166"/>
-      <c r="HO2" s="166"/>
-      <c r="HP2" s="166"/>
-      <c r="HQ2" s="166"/>
-      <c r="HR2" s="166"/>
-      <c r="HS2" s="166"/>
-      <c r="HT2" s="166"/>
-      <c r="HU2" s="166"/>
-      <c r="HV2" s="166"/>
-      <c r="HW2" s="166"/>
-      <c r="HX2" s="166"/>
-      <c r="HY2" s="166"/>
-      <c r="HZ2" s="166"/>
-      <c r="IA2" s="166"/>
-      <c r="IB2" s="166"/>
-      <c r="IC2" s="166"/>
-      <c r="ID2" s="166"/>
-      <c r="IE2" s="166"/>
-      <c r="IF2" s="166"/>
-      <c r="IG2" s="166"/>
-      <c r="IH2" s="166"/>
-      <c r="II2" s="166"/>
-      <c r="IJ2" s="166"/>
-      <c r="IK2" s="166"/>
-      <c r="IL2" s="166"/>
-      <c r="IM2" s="166"/>
-      <c r="IN2" s="166"/>
+      <c r="EP2" s="161"/>
+      <c r="EQ2" s="161"/>
+      <c r="ER2" s="161"/>
+      <c r="ES2" s="161"/>
+      <c r="ET2" s="161"/>
+      <c r="EU2" s="161"/>
+      <c r="EV2" s="161"/>
+      <c r="EW2" s="161"/>
+      <c r="EX2" s="161"/>
+      <c r="EY2" s="161"/>
+      <c r="EZ2" s="161"/>
+      <c r="FA2" s="161"/>
+      <c r="FB2" s="161"/>
+      <c r="FC2" s="161"/>
+      <c r="FD2" s="161"/>
+      <c r="FE2" s="161"/>
+      <c r="FF2" s="161"/>
+      <c r="FG2" s="161"/>
+      <c r="FH2" s="161"/>
+      <c r="FI2" s="161"/>
+      <c r="FJ2" s="161"/>
+      <c r="FK2" s="161"/>
+      <c r="FL2" s="161"/>
+      <c r="FM2" s="161"/>
+      <c r="FN2" s="161"/>
+      <c r="FO2" s="161"/>
+      <c r="FP2" s="161"/>
+      <c r="FQ2" s="161"/>
+      <c r="FR2" s="161"/>
+      <c r="FS2" s="161"/>
+      <c r="FT2" s="161"/>
+      <c r="FU2" s="161"/>
+      <c r="FV2" s="161"/>
+      <c r="FW2" s="161"/>
+      <c r="FX2" s="161"/>
+      <c r="FY2" s="161"/>
+      <c r="FZ2" s="161"/>
+      <c r="GA2" s="161"/>
+      <c r="GB2" s="161"/>
+      <c r="GC2" s="161"/>
+      <c r="GD2" s="161"/>
+      <c r="GE2" s="161"/>
+      <c r="GF2" s="161"/>
+      <c r="GG2" s="161"/>
+      <c r="GH2" s="161"/>
+      <c r="GI2" s="161"/>
+      <c r="GJ2" s="161"/>
+      <c r="GK2" s="161"/>
+      <c r="GL2" s="161"/>
+      <c r="GM2" s="161"/>
+      <c r="GN2" s="161"/>
+      <c r="GO2" s="161"/>
+      <c r="GP2" s="161"/>
+      <c r="GQ2" s="161"/>
+      <c r="GR2" s="161"/>
+      <c r="GS2" s="161"/>
+      <c r="GT2" s="161"/>
+      <c r="GU2" s="161"/>
+      <c r="GV2" s="161"/>
+      <c r="GW2" s="161"/>
+      <c r="GX2" s="161"/>
+      <c r="GY2" s="161"/>
+      <c r="GZ2" s="161"/>
+      <c r="HA2" s="161"/>
+      <c r="HB2" s="161"/>
+      <c r="HC2" s="161"/>
+      <c r="HD2" s="161"/>
+      <c r="HE2" s="161"/>
+      <c r="HF2" s="161"/>
+      <c r="HG2" s="161"/>
+      <c r="HH2" s="161"/>
+      <c r="HI2" s="161"/>
+      <c r="HJ2" s="161"/>
+      <c r="HK2" s="161"/>
+      <c r="HL2" s="161"/>
+      <c r="HM2" s="161"/>
+      <c r="HN2" s="161"/>
+      <c r="HO2" s="161"/>
+      <c r="HP2" s="161"/>
+      <c r="HQ2" s="161"/>
+      <c r="HR2" s="161"/>
+      <c r="HS2" s="161"/>
+      <c r="HT2" s="161"/>
+      <c r="HU2" s="161"/>
+      <c r="HV2" s="161"/>
+      <c r="HW2" s="161"/>
+      <c r="HX2" s="161"/>
+      <c r="HY2" s="161"/>
+      <c r="HZ2" s="161"/>
+      <c r="IA2" s="161"/>
+      <c r="IB2" s="161"/>
+      <c r="IC2" s="161"/>
+      <c r="ID2" s="161"/>
+      <c r="IE2" s="161"/>
+      <c r="IF2" s="161"/>
+      <c r="IG2" s="161"/>
+      <c r="IH2" s="161"/>
+      <c r="II2" s="161"/>
+      <c r="IJ2" s="161"/>
+      <c r="IK2" s="161"/>
+      <c r="IL2" s="161"/>
+      <c r="IM2" s="161"/>
+      <c r="IN2" s="161"/>
     </row>
     <row r="3" spans="1:248" s="58" customFormat="1" ht="64">
       <c r="A3" s="49" t="s">
@@ -11390,6 +11390,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="DT2:EN2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:AM1"/>
@@ -11406,7 +11407,6 @@
     <mergeCell ref="DE2:DI2"/>
     <mergeCell ref="DJ2:DM2"/>
     <mergeCell ref="DN2:DS2"/>
-    <mergeCell ref="DT2:EN2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.0.30-SNAPSHOT support {{fieldName}} in template excel
</commit_message>
<xml_diff>
--- a/src/test/resources/ceping.xlsx
+++ b/src/test/resources/ceping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80275E7F-6877-9242-BCAC-43EC1ED5FCF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94199C1A-7A30-C54F-9A79-9A8E7AEA129C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
   <sheets>
     <sheet name="有评语-模板" sheetId="5" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="356">
   <si>
     <t>大数据类候选人测评结论表</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1412,6 +1412,30 @@
   <si>
     <t>通过模板单元格</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{gender}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{age}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份证姓名</t>
+  </si>
+  <si>
+    <t>{name}</t>
+  </si>
+  <si>
+    <t>{gender}</t>
+  </si>
+  <si>
+    <t>{age}</t>
   </si>
 </sst>
 </file>
@@ -1866,7 +1890,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2097,6 +2121,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2334,6 +2361,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2368,12 +2401,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6934,8 +6961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0B56D7-DA51-554E-86D1-0655EAEF35DF}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -6951,51 +6978,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7"/>
+      <c r="A3" s="78" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>353</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="38.25" customHeight="1">
       <c r="A4" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>6</v>
@@ -7006,27 +7039,27 @@
       <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="84">
         <v>1.2</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="17" customHeight="1">
       <c r="A6" s="38"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="85" t="s">
+      <c r="B6" s="85"/>
+      <c r="C6" s="86" t="s">
         <v>346</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:7" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A7" s="74"/>
@@ -7042,28 +7075,28 @@
       <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="79"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="80"/>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="80" t="s">
+      <c r="C9" s="80"/>
+      <c r="D9" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="80"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="33" t="s">
         <v>13</v>
       </c>
@@ -7091,13 +7124,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:G5"/>
@@ -7116,7 +7148,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7132,51 +7164,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7"/>
+      <c r="A3" s="78" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>353</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="38.25" customHeight="1">
       <c r="A4" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="70"/>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="10"/>
       <c r="F4" s="72" t="s">
         <v>6</v>
@@ -7185,54 +7223,54 @@
       <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="84">
         <v>1.2</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="17" customHeight="1">
-      <c r="A6" s="87"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="85" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86" t="s">
         <v>346</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:8" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="79"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="80"/>
     </row>
     <row r="8" spans="1:8" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80" t="s">
+      <c r="C8" s="80"/>
+      <c r="D8" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="81"/>
       <c r="F8" s="69" t="s">
         <v>13</v>
       </c>
@@ -7260,14 +7298,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:G5"/>
@@ -7285,8 +7322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6F288-1AD6-674A-831C-FFD9B35C5B5E}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="135" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7306,15 +7343,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="I1" s="2"/>
       <c r="K1" s="3"/>
       <c r="L1" s="4"/>
@@ -7323,15 +7360,15 @@
       <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
       <c r="I2" s="2"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -7343,16 +7380,22 @@
       <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="6" t="s">
+        <v>350</v>
+      </c>
       <c r="F3" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>351</v>
+      </c>
       <c r="I3" s="9"/>
       <c r="K3" s="4"/>
       <c r="M3" s="4"/>
@@ -7365,10 +7408,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="61"/>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="10"/>
       <c r="F4" s="62" t="s">
         <v>6</v>
@@ -7382,17 +7425,17 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" s="8" customFormat="1" ht="63" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="89">
+      <c r="B5" s="89"/>
+      <c r="C5" s="90">
         <v>6</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="12"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -7403,15 +7446,15 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="79"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -7421,14 +7464,14 @@
       <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80" t="s">
+      <c r="C7" s="80"/>
+      <c r="D7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="81"/>
       <c r="F7" s="60" t="s">
         <v>13</v>
       </c>
@@ -7501,36 +7544,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>3</v>
@@ -7542,10 +7585,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="10"/>
       <c r="F4" s="25" t="s">
         <v>6</v>
@@ -7553,186 +7596,186 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="95">
+      <c r="C5" s="96">
         <v>1.2</v>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="98"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="92"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="100"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="92"/>
-      <c r="B7" s="101" t="s">
+      <c r="A7" s="93"/>
+      <c r="B7" s="102" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="92"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="84" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="92"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="92"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A11" s="92"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="92"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="104"/>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A13" s="92"/>
-      <c r="B13" s="102"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A14" s="92"/>
-      <c r="B14" s="102"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="106"/>
+      <c r="A14" s="93"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="107"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A15" s="92"/>
-      <c r="B15" s="102"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="106"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="107"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A16" s="92"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="106"/>
+      <c r="A16" s="93"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="107"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A17" s="92"/>
-      <c r="B17" s="102"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="106"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="107"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A18" s="92"/>
-      <c r="B18" s="102"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A19" s="92"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="93" t="s">
+      <c r="A19" s="93"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="103"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A20" s="92"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="79"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="80"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="80" t="s">
+      <c r="C22" s="80"/>
+      <c r="D22" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="80"/>
+      <c r="E22" s="81"/>
       <c r="F22" s="16" t="s">
         <v>13</v>
       </c>
@@ -7741,548 +7784,548 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="111" t="s">
+      <c r="B23" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="113" t="s">
+      <c r="C23" s="113"/>
+      <c r="D23" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="114"/>
+      <c r="E23" s="115"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="115" t="s">
+      <c r="A24" s="110"/>
+      <c r="B24" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="116"/>
-      <c r="D24" s="113" t="s">
+      <c r="C24" s="117"/>
+      <c r="D24" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="114"/>
-      <c r="F24" s="121">
+      <c r="E24" s="115"/>
+      <c r="F24" s="122">
         <v>2</v>
       </c>
-      <c r="G24" s="124" t="s">
+      <c r="G24" s="125" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="113" t="s">
+      <c r="A25" s="110"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="114"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="125"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="123"/>
+      <c r="G25" s="126"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="109"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="113" t="s">
+      <c r="A26" s="110"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="125"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="126"/>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="109"/>
-      <c r="B27" s="117"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="113" t="s">
+      <c r="A27" s="110"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="114"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="125"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="126"/>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="109"/>
-      <c r="B28" s="119"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="113" t="s">
+      <c r="A28" s="110"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="114"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="125"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="126"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="109"/>
-      <c r="B29" s="127" t="s">
+      <c r="A29" s="110"/>
+      <c r="B29" s="128" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="113" t="s">
+      <c r="C29" s="129"/>
+      <c r="D29" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="114"/>
-      <c r="F29" s="121">
+      <c r="E29" s="115"/>
+      <c r="F29" s="122">
         <v>2</v>
       </c>
-      <c r="G29" s="125"/>
+      <c r="G29" s="126"/>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="109"/>
-      <c r="B30" s="131"/>
-      <c r="C30" s="132"/>
-      <c r="D30" s="113" t="s">
+      <c r="A30" s="110"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="133"/>
+      <c r="D30" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="114"/>
-      <c r="F30" s="122"/>
-      <c r="G30" s="125"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="126"/>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="109"/>
-      <c r="B31" s="131"/>
-      <c r="C31" s="132"/>
-      <c r="D31" s="113" t="s">
+      <c r="A31" s="110"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="114"/>
-      <c r="F31" s="122"/>
-      <c r="G31" s="125"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="126"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="109"/>
-      <c r="B32" s="131"/>
-      <c r="C32" s="132"/>
-      <c r="D32" s="113" t="s">
+      <c r="A32" s="110"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="114"/>
-      <c r="F32" s="122"/>
-      <c r="G32" s="125"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="126"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="109"/>
-      <c r="B33" s="129"/>
-      <c r="C33" s="130"/>
-      <c r="D33" s="113" t="s">
+      <c r="A33" s="110"/>
+      <c r="B33" s="130"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="114"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="126"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="127"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="109"/>
-      <c r="B34" s="127" t="s">
+      <c r="A34" s="110"/>
+      <c r="B34" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="128"/>
-      <c r="D34" s="113" t="s">
+      <c r="C34" s="129"/>
+      <c r="D34" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="114"/>
-      <c r="F34" s="121">
+      <c r="E34" s="115"/>
+      <c r="F34" s="122">
         <v>0</v>
       </c>
-      <c r="G34" s="124" t="s">
+      <c r="G34" s="125" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="109"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="130"/>
-      <c r="D35" s="113" t="s">
+      <c r="A35" s="110"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="114"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="126"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="127"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="115" t="s">
+      <c r="A36" s="110"/>
+      <c r="B36" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="116"/>
-      <c r="D36" s="113" t="s">
+      <c r="C36" s="117"/>
+      <c r="D36" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="114"/>
-      <c r="F36" s="121">
+      <c r="E36" s="115"/>
+      <c r="F36" s="122">
         <v>2</v>
       </c>
-      <c r="G36" s="124" t="s">
+      <c r="G36" s="125" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="109"/>
-      <c r="B37" s="117"/>
-      <c r="C37" s="118"/>
-      <c r="D37" s="113" t="s">
+      <c r="A37" s="110"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="114"/>
-      <c r="F37" s="122"/>
-      <c r="G37" s="125"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="126"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="109"/>
-      <c r="B38" s="117"/>
-      <c r="C38" s="118"/>
-      <c r="D38" s="113" t="s">
+      <c r="A38" s="110"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="114"/>
-      <c r="F38" s="122"/>
-      <c r="G38" s="125"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="126"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="109"/>
-      <c r="B39" s="117"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="113" t="s">
+      <c r="A39" s="110"/>
+      <c r="B39" s="118"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="114"/>
-      <c r="F39" s="122"/>
-      <c r="G39" s="125"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="123"/>
+      <c r="G39" s="126"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="109"/>
-      <c r="B40" s="119"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="113" t="s">
+      <c r="A40" s="110"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="114"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="125"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="124"/>
+      <c r="G40" s="126"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="109"/>
-      <c r="B41" s="127" t="s">
+      <c r="A41" s="110"/>
+      <c r="B41" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="128"/>
-      <c r="D41" s="113" t="s">
+      <c r="C41" s="129"/>
+      <c r="D41" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="114"/>
-      <c r="F41" s="121">
+      <c r="E41" s="115"/>
+      <c r="F41" s="122">
         <v>2</v>
       </c>
-      <c r="G41" s="125"/>
+      <c r="G41" s="126"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="109"/>
-      <c r="B42" s="131"/>
-      <c r="C42" s="132"/>
-      <c r="D42" s="113" t="s">
+      <c r="A42" s="110"/>
+      <c r="B42" s="132"/>
+      <c r="C42" s="133"/>
+      <c r="D42" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="114"/>
-      <c r="F42" s="122"/>
-      <c r="G42" s="125"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="126"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="109"/>
-      <c r="B43" s="131"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="113" t="s">
+      <c r="A43" s="110"/>
+      <c r="B43" s="132"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="125"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="126"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="109"/>
-      <c r="B44" s="131"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="113" t="s">
+      <c r="A44" s="110"/>
+      <c r="B44" s="132"/>
+      <c r="C44" s="133"/>
+      <c r="D44" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="114"/>
-      <c r="F44" s="122"/>
-      <c r="G44" s="125"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="126"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="109"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="130"/>
-      <c r="D45" s="113" t="s">
+      <c r="A45" s="110"/>
+      <c r="B45" s="130"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="114"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="125"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="126"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="109"/>
-      <c r="B46" s="127" t="s">
+      <c r="A46" s="110"/>
+      <c r="B46" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="128"/>
-      <c r="D46" s="113" t="s">
+      <c r="C46" s="129"/>
+      <c r="D46" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="114"/>
-      <c r="F46" s="121">
+      <c r="E46" s="115"/>
+      <c r="F46" s="122">
         <v>2</v>
       </c>
-      <c r="G46" s="125"/>
+      <c r="G46" s="126"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="109"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="132"/>
-      <c r="D47" s="113" t="s">
+      <c r="A47" s="110"/>
+      <c r="B47" s="132"/>
+      <c r="C47" s="133"/>
+      <c r="D47" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="114"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="125"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="126"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="109"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="132"/>
-      <c r="D48" s="113" t="s">
+      <c r="A48" s="110"/>
+      <c r="B48" s="132"/>
+      <c r="C48" s="133"/>
+      <c r="D48" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="114"/>
-      <c r="F48" s="122"/>
-      <c r="G48" s="125"/>
+      <c r="E48" s="115"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="126"/>
     </row>
     <row r="49" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="109"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="113" t="s">
+      <c r="A49" s="110"/>
+      <c r="B49" s="132"/>
+      <c r="C49" s="133"/>
+      <c r="D49" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="114"/>
-      <c r="F49" s="122"/>
-      <c r="G49" s="125"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="126"/>
     </row>
     <row r="50" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="109"/>
-      <c r="B50" s="129"/>
-      <c r="C50" s="130"/>
-      <c r="D50" s="113" t="s">
+      <c r="A50" s="110"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="131"/>
+      <c r="D50" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="114"/>
-      <c r="F50" s="123"/>
-      <c r="G50" s="125"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="124"/>
+      <c r="G50" s="126"/>
     </row>
     <row r="51" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="109"/>
-      <c r="B51" s="127" t="s">
+      <c r="A51" s="110"/>
+      <c r="B51" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="128"/>
-      <c r="D51" s="113" t="s">
+      <c r="C51" s="129"/>
+      <c r="D51" s="114" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="114"/>
-      <c r="F51" s="121">
+      <c r="E51" s="115"/>
+      <c r="F51" s="122">
         <v>2</v>
       </c>
-      <c r="G51" s="125"/>
+      <c r="G51" s="126"/>
     </row>
     <row r="52" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A52" s="109"/>
-      <c r="B52" s="131"/>
-      <c r="C52" s="132"/>
-      <c r="D52" s="113" t="s">
+      <c r="A52" s="110"/>
+      <c r="B52" s="132"/>
+      <c r="C52" s="133"/>
+      <c r="D52" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="E52" s="114"/>
-      <c r="F52" s="122"/>
-      <c r="G52" s="125"/>
+      <c r="E52" s="115"/>
+      <c r="F52" s="123"/>
+      <c r="G52" s="126"/>
     </row>
     <row r="53" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A53" s="109"/>
-      <c r="B53" s="131"/>
-      <c r="C53" s="132"/>
-      <c r="D53" s="113" t="s">
+      <c r="A53" s="110"/>
+      <c r="B53" s="132"/>
+      <c r="C53" s="133"/>
+      <c r="D53" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="E53" s="114"/>
-      <c r="F53" s="122"/>
-      <c r="G53" s="125"/>
+      <c r="E53" s="115"/>
+      <c r="F53" s="123"/>
+      <c r="G53" s="126"/>
     </row>
     <row r="54" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A54" s="109"/>
-      <c r="B54" s="131"/>
-      <c r="C54" s="132"/>
-      <c r="D54" s="113" t="s">
+      <c r="A54" s="110"/>
+      <c r="B54" s="132"/>
+      <c r="C54" s="133"/>
+      <c r="D54" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="E54" s="114"/>
-      <c r="F54" s="122"/>
-      <c r="G54" s="125"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="126"/>
     </row>
     <row r="55" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A55" s="109"/>
-      <c r="B55" s="129"/>
-      <c r="C55" s="130"/>
-      <c r="D55" s="113" t="s">
+      <c r="A55" s="110"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="131"/>
+      <c r="D55" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="E55" s="114"/>
-      <c r="F55" s="123"/>
-      <c r="G55" s="126"/>
+      <c r="E55" s="115"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="127"/>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A56" s="109"/>
-      <c r="B56" s="127" t="s">
+      <c r="A56" s="110"/>
+      <c r="B56" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="128"/>
-      <c r="D56" s="113" t="s">
+      <c r="C56" s="129"/>
+      <c r="D56" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="114"/>
-      <c r="F56" s="121">
+      <c r="E56" s="115"/>
+      <c r="F56" s="122">
         <v>0</v>
       </c>
-      <c r="G56" s="124" t="s">
+      <c r="G56" s="125" t="s">
         <v>34</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A57" s="109"/>
-      <c r="B57" s="129"/>
-      <c r="C57" s="130"/>
-      <c r="D57" s="113" t="s">
+      <c r="A57" s="110"/>
+      <c r="B57" s="130"/>
+      <c r="C57" s="131"/>
+      <c r="D57" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="114"/>
-      <c r="F57" s="123"/>
-      <c r="G57" s="126"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="124"/>
+      <c r="G57" s="127"/>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A58" s="109"/>
-      <c r="B58" s="127" t="s">
+      <c r="A58" s="110"/>
+      <c r="B58" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="128"/>
-      <c r="D58" s="113" t="s">
+      <c r="C58" s="129"/>
+      <c r="D58" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="114"/>
-      <c r="F58" s="121">
+      <c r="E58" s="115"/>
+      <c r="F58" s="122">
         <v>0</v>
       </c>
-      <c r="G58" s="124" t="s">
+      <c r="G58" s="125" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A59" s="109"/>
-      <c r="B59" s="129"/>
-      <c r="C59" s="130"/>
-      <c r="D59" s="113" t="s">
+      <c r="A59" s="110"/>
+      <c r="B59" s="130"/>
+      <c r="C59" s="131"/>
+      <c r="D59" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="114"/>
-      <c r="F59" s="123"/>
-      <c r="G59" s="125"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="124"/>
+      <c r="G59" s="126"/>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A60" s="109"/>
-      <c r="B60" s="127" t="s">
+      <c r="A60" s="110"/>
+      <c r="B60" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="128"/>
-      <c r="D60" s="113" t="s">
+      <c r="C60" s="129"/>
+      <c r="D60" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="114"/>
-      <c r="F60" s="121">
+      <c r="E60" s="115"/>
+      <c r="F60" s="122">
         <v>0</v>
       </c>
-      <c r="G60" s="125"/>
+      <c r="G60" s="126"/>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A61" s="109"/>
-      <c r="B61" s="131"/>
-      <c r="C61" s="132"/>
-      <c r="D61" s="113" t="s">
+      <c r="A61" s="110"/>
+      <c r="B61" s="132"/>
+      <c r="C61" s="133"/>
+      <c r="D61" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="114"/>
-      <c r="F61" s="122"/>
-      <c r="G61" s="125"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="123"/>
+      <c r="G61" s="126"/>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A62" s="109"/>
-      <c r="B62" s="131"/>
-      <c r="C62" s="132"/>
-      <c r="D62" s="113" t="s">
+      <c r="A62" s="110"/>
+      <c r="B62" s="132"/>
+      <c r="C62" s="133"/>
+      <c r="D62" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="114"/>
-      <c r="F62" s="122"/>
-      <c r="G62" s="125"/>
+      <c r="E62" s="115"/>
+      <c r="F62" s="123"/>
+      <c r="G62" s="126"/>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A63" s="109"/>
-      <c r="B63" s="131"/>
-      <c r="C63" s="132"/>
-      <c r="D63" s="113" t="s">
+      <c r="A63" s="110"/>
+      <c r="B63" s="132"/>
+      <c r="C63" s="133"/>
+      <c r="D63" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="114"/>
-      <c r="F63" s="122"/>
-      <c r="G63" s="125"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="123"/>
+      <c r="G63" s="126"/>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A64" s="109"/>
-      <c r="B64" s="131"/>
-      <c r="C64" s="132"/>
-      <c r="D64" s="113" t="s">
+      <c r="A64" s="110"/>
+      <c r="B64" s="132"/>
+      <c r="C64" s="133"/>
+      <c r="D64" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="114"/>
-      <c r="F64" s="122"/>
-      <c r="G64" s="125"/>
+      <c r="E64" s="115"/>
+      <c r="F64" s="123"/>
+      <c r="G64" s="126"/>
     </row>
     <row r="65" spans="1:7" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A65" s="110"/>
-      <c r="B65" s="129"/>
-      <c r="C65" s="130"/>
-      <c r="D65" s="113" t="s">
+      <c r="A65" s="111"/>
+      <c r="B65" s="130"/>
+      <c r="C65" s="131"/>
+      <c r="D65" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="114"/>
-      <c r="F65" s="123"/>
-      <c r="G65" s="126"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="127"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A66" s="133" t="s">
+      <c r="A66" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="134" t="s">
+      <c r="B66" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="134"/>
-      <c r="D66" s="134" t="s">
+      <c r="C66" s="135"/>
+      <c r="D66" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="134"/>
+      <c r="E66" s="135"/>
       <c r="F66" s="17">
         <v>0</v>
       </c>
@@ -8291,15 +8334,15 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A67" s="133"/>
-      <c r="B67" s="135" t="s">
+      <c r="A67" s="134"/>
+      <c r="B67" s="136" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="135"/>
-      <c r="D67" s="136" t="s">
+      <c r="C67" s="136"/>
+      <c r="D67" s="137" t="s">
         <v>76</v>
       </c>
-      <c r="E67" s="136"/>
+      <c r="E67" s="137"/>
       <c r="F67" s="26">
         <v>0</v>
       </c>
@@ -8308,104 +8351,104 @@
       </c>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A68" s="133"/>
-      <c r="B68" s="137" t="s">
+      <c r="A68" s="134"/>
+      <c r="B68" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="138"/>
-      <c r="D68" s="143" t="s">
+      <c r="C68" s="139"/>
+      <c r="D68" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="E68" s="144"/>
-      <c r="F68" s="146">
+      <c r="E68" s="145"/>
+      <c r="F68" s="147">
         <v>0</v>
       </c>
-      <c r="G68" s="124" t="s">
+      <c r="G68" s="125" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A69" s="133"/>
-      <c r="B69" s="139"/>
-      <c r="C69" s="140"/>
-      <c r="D69" s="143" t="s">
+      <c r="A69" s="134"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="141"/>
+      <c r="D69" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="E69" s="144"/>
-      <c r="F69" s="147"/>
-      <c r="G69" s="125"/>
+      <c r="E69" s="145"/>
+      <c r="F69" s="148"/>
+      <c r="G69" s="126"/>
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A70" s="133"/>
-      <c r="B70" s="139"/>
-      <c r="C70" s="140"/>
-      <c r="D70" s="143" t="s">
+      <c r="A70" s="134"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="141"/>
+      <c r="D70" s="144" t="s">
         <v>81</v>
       </c>
-      <c r="E70" s="144"/>
-      <c r="F70" s="147"/>
-      <c r="G70" s="125"/>
+      <c r="E70" s="145"/>
+      <c r="F70" s="148"/>
+      <c r="G70" s="126"/>
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A71" s="133"/>
-      <c r="B71" s="141"/>
-      <c r="C71" s="142"/>
-      <c r="D71" s="143" t="s">
+      <c r="A71" s="134"/>
+      <c r="B71" s="142"/>
+      <c r="C71" s="143"/>
+      <c r="D71" s="144" t="s">
         <v>82</v>
       </c>
-      <c r="E71" s="144"/>
-      <c r="F71" s="148"/>
-      <c r="G71" s="126"/>
+      <c r="E71" s="145"/>
+      <c r="F71" s="149"/>
+      <c r="G71" s="127"/>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A72" s="133"/>
-      <c r="B72" s="145" t="s">
+      <c r="A72" s="134"/>
+      <c r="B72" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="145"/>
-      <c r="D72" s="145" t="s">
+      <c r="C72" s="146"/>
+      <c r="D72" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="145"/>
-      <c r="F72" s="149">
+      <c r="E72" s="146"/>
+      <c r="F72" s="150">
         <v>0</v>
       </c>
-      <c r="G72" s="136" t="s">
+      <c r="G72" s="137" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A73" s="133"/>
-      <c r="B73" s="145"/>
-      <c r="C73" s="145"/>
-      <c r="D73" s="150" t="s">
+      <c r="A73" s="134"/>
+      <c r="B73" s="146"/>
+      <c r="C73" s="146"/>
+      <c r="D73" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="E73" s="150"/>
-      <c r="F73" s="149"/>
-      <c r="G73" s="136"/>
+      <c r="E73" s="151"/>
+      <c r="F73" s="150"/>
+      <c r="G73" s="137"/>
     </row>
     <row r="74" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A74" s="133"/>
-      <c r="B74" s="145"/>
-      <c r="C74" s="145"/>
-      <c r="D74" s="145" t="s">
+      <c r="A74" s="134"/>
+      <c r="B74" s="146"/>
+      <c r="C74" s="146"/>
+      <c r="D74" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="E74" s="145"/>
-      <c r="F74" s="149"/>
-      <c r="G74" s="136"/>
+      <c r="E74" s="146"/>
+      <c r="F74" s="150"/>
+      <c r="G74" s="137"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A75" s="133"/>
-      <c r="B75" s="145"/>
-      <c r="C75" s="145"/>
-      <c r="D75" s="145" t="s">
+      <c r="A75" s="134"/>
+      <c r="B75" s="146"/>
+      <c r="C75" s="146"/>
+      <c r="D75" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="145"/>
-      <c r="F75" s="149"/>
-      <c r="G75" s="136"/>
+      <c r="E75" s="146"/>
+      <c r="F75" s="150"/>
+      <c r="G75" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="117">
@@ -8587,15 +8630,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -8604,15 +8647,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -8625,10 +8668,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>3</v>
@@ -8646,10 +8689,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -8663,19 +8706,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="95">
+      <c r="C5" s="96">
         <v>6</v>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="98"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -8687,28 +8730,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="92"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="79"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="80"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -8718,14 +8761,14 @@
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80" t="s">
+      <c r="C8" s="80"/>
+      <c r="D8" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="81"/>
       <c r="F8" s="16" t="s">
         <v>13</v>
       </c>
@@ -8738,17 +8781,17 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="113" t="s">
+      <c r="C9" s="113"/>
+      <c r="D9" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="114"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
         <v>18</v>
@@ -8758,19 +8801,19 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="109"/>
-      <c r="B10" s="115" t="s">
+      <c r="A10" s="110"/>
+      <c r="B10" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="113" t="s">
+      <c r="C10" s="117"/>
+      <c r="D10" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="114"/>
-      <c r="F10" s="121">
+      <c r="E10" s="115"/>
+      <c r="F10" s="122">
         <v>2</v>
       </c>
-      <c r="G10" s="151" t="s">
+      <c r="G10" s="152" t="s">
         <v>21</v>
       </c>
       <c r="K10" s="4"/>
@@ -8779,79 +8822,79 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A11" s="109"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="113" t="s">
+      <c r="A11" s="110"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="152"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="153"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="109"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="113" t="s">
+      <c r="A12" s="110"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="152"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="153"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="109"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="113" t="s">
+      <c r="A13" s="110"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="122"/>
-      <c r="G13" s="152"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="153"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="109"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="113" t="s">
+      <c r="A14" s="110"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="152"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="153"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="109"/>
-      <c r="B15" s="127" t="s">
+      <c r="A15" s="110"/>
+      <c r="B15" s="128" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="128"/>
-      <c r="D15" s="113" t="s">
+      <c r="C15" s="129"/>
+      <c r="D15" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="114"/>
-      <c r="F15" s="121">
+      <c r="E15" s="115"/>
+      <c r="F15" s="122">
         <v>2</v>
       </c>
-      <c r="G15" s="152"/>
+      <c r="G15" s="153"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -8861,15 +8904,15 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A16" s="109"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="113" t="s">
+      <c r="A16" s="110"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="114"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="152"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="153"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -8879,15 +8922,15 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="109"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="113" t="s">
+      <c r="A17" s="110"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="114"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="152"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="153"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -8897,15 +8940,15 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A18" s="109"/>
-      <c r="B18" s="131"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="113" t="s">
+      <c r="A18" s="110"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="152"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="153"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -8915,15 +8958,15 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A19" s="109"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="130"/>
-      <c r="D19" s="113" t="s">
+      <c r="A19" s="110"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="131"/>
+      <c r="D19" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="114"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="153"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="154"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -8933,19 +8976,19 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A20" s="109"/>
-      <c r="B20" s="127" t="s">
+      <c r="A20" s="110"/>
+      <c r="B20" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="128"/>
-      <c r="D20" s="113" t="s">
+      <c r="C20" s="129"/>
+      <c r="D20" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="114"/>
-      <c r="F20" s="121">
+      <c r="E20" s="115"/>
+      <c r="F20" s="122">
         <v>0</v>
       </c>
-      <c r="G20" s="151" t="s">
+      <c r="G20" s="152" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="4"/>
@@ -8954,34 +8997,34 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A21" s="109"/>
-      <c r="B21" s="129"/>
-      <c r="C21" s="130"/>
-      <c r="D21" s="113" t="s">
+      <c r="A21" s="110"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="153"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="154"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A22" s="109"/>
-      <c r="B22" s="115" t="s">
+      <c r="A22" s="110"/>
+      <c r="B22" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="116"/>
-      <c r="D22" s="113" t="s">
+      <c r="C22" s="117"/>
+      <c r="D22" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="114"/>
-      <c r="F22" s="121">
+      <c r="E22" s="115"/>
+      <c r="F22" s="122">
         <v>2</v>
       </c>
-      <c r="G22" s="124" t="s">
+      <c r="G22" s="125" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="4"/>
@@ -8990,79 +9033,79 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="109"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="113" t="s">
+      <c r="A23" s="110"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="114"/>
-      <c r="F23" s="122"/>
-      <c r="G23" s="125"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="123"/>
+      <c r="G23" s="126"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="117"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="113" t="s">
+      <c r="A24" s="110"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="114"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="125"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="126"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="113" t="s">
+      <c r="A25" s="110"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="114"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="125"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="123"/>
+      <c r="G25" s="126"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="109"/>
-      <c r="B26" s="119"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="113" t="s">
+      <c r="A26" s="110"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="125"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="126"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="109"/>
-      <c r="B27" s="127" t="s">
+      <c r="A27" s="110"/>
+      <c r="B27" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="128"/>
-      <c r="D27" s="113" t="s">
+      <c r="C27" s="129"/>
+      <c r="D27" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="114"/>
-      <c r="F27" s="121">
+      <c r="E27" s="115"/>
+      <c r="F27" s="122">
         <v>2</v>
       </c>
-      <c r="G27" s="125"/>
+      <c r="G27" s="126"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
@@ -9072,15 +9115,15 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="109"/>
-      <c r="B28" s="131"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="113" t="s">
+      <c r="A28" s="110"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="133"/>
+      <c r="D28" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="114"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="125"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="126"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -9089,15 +9132,15 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="109"/>
-      <c r="B29" s="131"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="113" t="s">
+      <c r="A29" s="110"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="114"/>
-      <c r="F29" s="122"/>
-      <c r="G29" s="125"/>
+      <c r="E29" s="115"/>
+      <c r="F29" s="123"/>
+      <c r="G29" s="126"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -9106,15 +9149,15 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="109"/>
-      <c r="B30" s="131"/>
-      <c r="C30" s="132"/>
-      <c r="D30" s="113" t="s">
+      <c r="A30" s="110"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="133"/>
+      <c r="D30" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="114"/>
-      <c r="F30" s="122"/>
-      <c r="G30" s="125"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="126"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -9123,15 +9166,15 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="109"/>
-      <c r="B31" s="129"/>
-      <c r="C31" s="130"/>
-      <c r="D31" s="113" t="s">
+      <c r="A31" s="110"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="114"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="125"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="126"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -9140,19 +9183,19 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="109"/>
-      <c r="B32" s="127" t="s">
+      <c r="A32" s="110"/>
+      <c r="B32" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="128"/>
-      <c r="D32" s="113" t="s">
+      <c r="C32" s="129"/>
+      <c r="D32" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="114"/>
-      <c r="F32" s="121">
+      <c r="E32" s="115"/>
+      <c r="F32" s="122">
         <v>2</v>
       </c>
-      <c r="G32" s="125" t="s">
+      <c r="G32" s="126" t="s">
         <v>49</v>
       </c>
       <c r="H32" s="19"/>
@@ -9164,15 +9207,15 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="109"/>
-      <c r="B33" s="131"/>
-      <c r="C33" s="132"/>
-      <c r="D33" s="113" t="s">
+      <c r="A33" s="110"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="133"/>
+      <c r="D33" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="114"/>
-      <c r="F33" s="122"/>
-      <c r="G33" s="125"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="126"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -9182,15 +9225,15 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="109"/>
-      <c r="B34" s="131"/>
-      <c r="C34" s="132"/>
-      <c r="D34" s="113" t="s">
+      <c r="A34" s="110"/>
+      <c r="B34" s="132"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="114"/>
-      <c r="F34" s="122"/>
-      <c r="G34" s="125"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="126"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -9200,15 +9243,15 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="109"/>
-      <c r="B35" s="131"/>
-      <c r="C35" s="132"/>
-      <c r="D35" s="113" t="s">
+      <c r="A35" s="110"/>
+      <c r="B35" s="132"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="114"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="125"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="126"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -9218,15 +9261,15 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="129"/>
-      <c r="C36" s="130"/>
-      <c r="D36" s="113" t="s">
+      <c r="A36" s="110"/>
+      <c r="B36" s="130"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="114"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="125"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="126"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -9236,98 +9279,98 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="109"/>
-      <c r="B37" s="127" t="s">
+      <c r="A37" s="110"/>
+      <c r="B37" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="128"/>
-      <c r="D37" s="113" t="s">
+      <c r="C37" s="129"/>
+      <c r="D37" s="114" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="114"/>
-      <c r="F37" s="121">
+      <c r="E37" s="115"/>
+      <c r="F37" s="122">
         <v>2</v>
       </c>
-      <c r="G37" s="125"/>
+      <c r="G37" s="126"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="109"/>
-      <c r="B38" s="131"/>
-      <c r="C38" s="132"/>
-      <c r="D38" s="113" t="s">
+      <c r="A38" s="110"/>
+      <c r="B38" s="132"/>
+      <c r="C38" s="133"/>
+      <c r="D38" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="114"/>
-      <c r="F38" s="122"/>
-      <c r="G38" s="125"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="126"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="109"/>
-      <c r="B39" s="131"/>
-      <c r="C39" s="132"/>
-      <c r="D39" s="113" t="s">
+      <c r="A39" s="110"/>
+      <c r="B39" s="132"/>
+      <c r="C39" s="133"/>
+      <c r="D39" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="114"/>
-      <c r="F39" s="122"/>
-      <c r="G39" s="125"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="123"/>
+      <c r="G39" s="126"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="109"/>
-      <c r="B40" s="131"/>
-      <c r="C40" s="132"/>
-      <c r="D40" s="113" t="s">
+      <c r="A40" s="110"/>
+      <c r="B40" s="132"/>
+      <c r="C40" s="133"/>
+      <c r="D40" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="114"/>
-      <c r="F40" s="122"/>
-      <c r="G40" s="125"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="126"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="109"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
-      <c r="D41" s="113" t="s">
+      <c r="A41" s="110"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="114"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="126"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="124"/>
+      <c r="G41" s="127"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="109"/>
-      <c r="B42" s="127" t="s">
+      <c r="A42" s="110"/>
+      <c r="B42" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="128"/>
-      <c r="D42" s="113" t="s">
+      <c r="C42" s="129"/>
+      <c r="D42" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="114"/>
-      <c r="F42" s="121">
+      <c r="E42" s="115"/>
+      <c r="F42" s="122">
         <v>0</v>
       </c>
-      <c r="G42" s="124" t="s">
+      <c r="G42" s="125" t="s">
         <v>34</v>
       </c>
       <c r="K42" s="21"/>
@@ -9337,34 +9380,34 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="109"/>
-      <c r="B43" s="129"/>
-      <c r="C43" s="130"/>
-      <c r="D43" s="113" t="s">
+      <c r="A43" s="110"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="131"/>
+      <c r="D43" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="126"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="127"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
     </row>
     <row r="44" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="109"/>
-      <c r="B44" s="127" t="s">
+      <c r="A44" s="110"/>
+      <c r="B44" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="128"/>
-      <c r="D44" s="113" t="s">
+      <c r="C44" s="129"/>
+      <c r="D44" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="114"/>
-      <c r="F44" s="121">
+      <c r="E44" s="115"/>
+      <c r="F44" s="122">
         <v>0</v>
       </c>
-      <c r="G44" s="124" t="s">
+      <c r="G44" s="125" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="8"/>
@@ -9376,15 +9419,15 @@
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="109"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="130"/>
-      <c r="D45" s="113" t="s">
+      <c r="A45" s="110"/>
+      <c r="B45" s="130"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="114"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="125"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="126"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -9394,111 +9437,111 @@
       <c r="N45" s="21"/>
     </row>
     <row r="46" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="109"/>
-      <c r="B46" s="127" t="s">
+      <c r="A46" s="110"/>
+      <c r="B46" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="128"/>
-      <c r="D46" s="113" t="s">
+      <c r="C46" s="129"/>
+      <c r="D46" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="114"/>
-      <c r="F46" s="121">
+      <c r="E46" s="115"/>
+      <c r="F46" s="122">
         <v>0</v>
       </c>
-      <c r="G46" s="125"/>
+      <c r="G46" s="126"/>
       <c r="K46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="109"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="132"/>
-      <c r="D47" s="113" t="s">
+      <c r="A47" s="110"/>
+      <c r="B47" s="132"/>
+      <c r="C47" s="133"/>
+      <c r="D47" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="114"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="125"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="126"/>
       <c r="K47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="109"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="132"/>
-      <c r="D48" s="113" t="s">
+      <c r="A48" s="110"/>
+      <c r="B48" s="132"/>
+      <c r="C48" s="133"/>
+      <c r="D48" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="E48" s="114"/>
-      <c r="F48" s="122"/>
-      <c r="G48" s="125"/>
+      <c r="E48" s="115"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="126"/>
       <c r="K48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
     </row>
     <row r="49" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="109"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="113" t="s">
+      <c r="A49" s="110"/>
+      <c r="B49" s="132"/>
+      <c r="C49" s="133"/>
+      <c r="D49" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="114"/>
-      <c r="F49" s="122"/>
-      <c r="G49" s="125"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="126"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
     </row>
     <row r="50" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="109"/>
-      <c r="B50" s="131"/>
-      <c r="C50" s="132"/>
-      <c r="D50" s="113" t="s">
+      <c r="A50" s="110"/>
+      <c r="B50" s="132"/>
+      <c r="C50" s="133"/>
+      <c r="D50" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="114"/>
-      <c r="F50" s="122"/>
-      <c r="G50" s="125"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="126"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
     </row>
     <row r="51" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="110"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="130"/>
-      <c r="D51" s="113" t="s">
+      <c r="A51" s="111"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="114"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="126"/>
+      <c r="E51" s="115"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="127"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
     </row>
     <row r="52" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A52" s="133" t="s">
+      <c r="A52" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="134" t="s">
+      <c r="B52" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="134"/>
-      <c r="D52" s="134" t="s">
+      <c r="C52" s="135"/>
+      <c r="D52" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="134"/>
+      <c r="E52" s="135"/>
       <c r="F52" s="17">
         <v>0</v>
       </c>
@@ -9510,15 +9553,15 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="1:16" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A53" s="133"/>
-      <c r="B53" s="135" t="s">
+      <c r="A53" s="134"/>
+      <c r="B53" s="136" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="135"/>
-      <c r="D53" s="136" t="s">
+      <c r="C53" s="136"/>
+      <c r="D53" s="137" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="136"/>
+      <c r="E53" s="137"/>
       <c r="F53" s="26">
         <v>0</v>
       </c>
@@ -9530,19 +9573,19 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="133"/>
-      <c r="B54" s="137" t="s">
+      <c r="A54" s="134"/>
+      <c r="B54" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="138"/>
-      <c r="D54" s="143" t="s">
+      <c r="C54" s="139"/>
+      <c r="D54" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="144"/>
-      <c r="F54" s="146">
+      <c r="E54" s="145"/>
+      <c r="F54" s="147">
         <v>0</v>
       </c>
-      <c r="G54" s="124" t="s">
+      <c r="G54" s="125" t="s">
         <v>79</v>
       </c>
       <c r="K54" s="4"/>
@@ -9551,30 +9594,30 @@
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="133"/>
-      <c r="B55" s="139"/>
-      <c r="C55" s="140"/>
-      <c r="D55" s="143" t="s">
+      <c r="A55" s="134"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="141"/>
+      <c r="D55" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="144"/>
-      <c r="F55" s="147"/>
-      <c r="G55" s="125"/>
+      <c r="E55" s="145"/>
+      <c r="F55" s="148"/>
+      <c r="G55" s="126"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="133"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="140"/>
-      <c r="D56" s="143" t="s">
+      <c r="A56" s="134"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="141"/>
+      <c r="D56" s="144" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="144"/>
-      <c r="F56" s="147"/>
-      <c r="G56" s="125"/>
+      <c r="E56" s="145"/>
+      <c r="F56" s="148"/>
+      <c r="G56" s="126"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -9582,15 +9625,15 @@
       <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="133"/>
-      <c r="B57" s="141"/>
-      <c r="C57" s="142"/>
-      <c r="D57" s="143" t="s">
+      <c r="A57" s="134"/>
+      <c r="B57" s="142"/>
+      <c r="C57" s="143"/>
+      <c r="D57" s="144" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="144"/>
-      <c r="F57" s="148"/>
-      <c r="G57" s="126"/>
+      <c r="E57" s="145"/>
+      <c r="F57" s="149"/>
+      <c r="G57" s="127"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="3"/>
@@ -9600,19 +9643,19 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="133"/>
-      <c r="B58" s="145" t="s">
+      <c r="A58" s="134"/>
+      <c r="B58" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="145"/>
-      <c r="D58" s="145" t="s">
+      <c r="C58" s="146"/>
+      <c r="D58" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="E58" s="145"/>
-      <c r="F58" s="149">
+      <c r="E58" s="146"/>
+      <c r="F58" s="150">
         <v>0</v>
       </c>
-      <c r="G58" s="136" t="s">
+      <c r="G58" s="137" t="s">
         <v>85</v>
       </c>
       <c r="K58" s="4"/>
@@ -9621,44 +9664,44 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="133"/>
-      <c r="B59" s="145"/>
-      <c r="C59" s="145"/>
-      <c r="D59" s="150" t="s">
+      <c r="A59" s="134"/>
+      <c r="B59" s="146"/>
+      <c r="C59" s="146"/>
+      <c r="D59" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="150"/>
-      <c r="F59" s="149"/>
-      <c r="G59" s="136"/>
+      <c r="E59" s="151"/>
+      <c r="F59" s="150"/>
+      <c r="G59" s="137"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="133"/>
-      <c r="B60" s="145"/>
-      <c r="C60" s="145"/>
-      <c r="D60" s="145" t="s">
+      <c r="A60" s="134"/>
+      <c r="B60" s="146"/>
+      <c r="C60" s="146"/>
+      <c r="D60" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="E60" s="145"/>
-      <c r="F60" s="149"/>
-      <c r="G60" s="136"/>
+      <c r="E60" s="146"/>
+      <c r="F60" s="150"/>
+      <c r="G60" s="137"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
     <row r="61" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="133"/>
-      <c r="B61" s="145"/>
-      <c r="C61" s="145"/>
-      <c r="D61" s="145" t="s">
+      <c r="A61" s="134"/>
+      <c r="B61" s="146"/>
+      <c r="C61" s="146"/>
+      <c r="D61" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="145"/>
-      <c r="F61" s="149"/>
-      <c r="G61" s="136"/>
+      <c r="E61" s="146"/>
+      <c r="F61" s="150"/>
+      <c r="G61" s="137"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -9840,262 +9883,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:248" s="48" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="161" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="159" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="162" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="160" t="s">
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="163" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="160"/>
-      <c r="K1" s="160"/>
-      <c r="L1" s="160"/>
-      <c r="M1" s="160"/>
-      <c r="N1" s="160"/>
-      <c r="O1" s="160"/>
-      <c r="P1" s="160"/>
-      <c r="Q1" s="160"/>
-      <c r="R1" s="160"/>
-      <c r="S1" s="160"/>
-      <c r="T1" s="160"/>
-      <c r="U1" s="160"/>
-      <c r="V1" s="160"/>
-      <c r="W1" s="160"/>
-      <c r="X1" s="160"/>
-      <c r="Y1" s="160"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="160"/>
-      <c r="AB1" s="160"/>
-      <c r="AC1" s="160"/>
-      <c r="AD1" s="160"/>
-      <c r="AE1" s="160"/>
-      <c r="AF1" s="160"/>
-      <c r="AG1" s="160"/>
-      <c r="AH1" s="160"/>
-      <c r="AI1" s="160"/>
-      <c r="AJ1" s="160"/>
-      <c r="AK1" s="160"/>
-      <c r="AL1" s="160"/>
-      <c r="AM1" s="160"/>
-      <c r="AN1" s="161" t="s">
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
+      <c r="AF1" s="163"/>
+      <c r="AG1" s="163"/>
+      <c r="AH1" s="163"/>
+      <c r="AI1" s="163"/>
+      <c r="AJ1" s="163"/>
+      <c r="AK1" s="163"/>
+      <c r="AL1" s="163"/>
+      <c r="AM1" s="163"/>
+      <c r="AN1" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="161"/>
-      <c r="AP1" s="161"/>
-      <c r="AQ1" s="161"/>
-      <c r="AR1" s="161"/>
-      <c r="AS1" s="161"/>
-      <c r="AT1" s="161"/>
-      <c r="AU1" s="161"/>
-      <c r="AV1" s="161"/>
-      <c r="AW1" s="161"/>
-      <c r="AX1" s="161"/>
-      <c r="AY1" s="161"/>
-      <c r="AZ1" s="161"/>
-      <c r="BA1" s="161"/>
-      <c r="BB1" s="161"/>
-      <c r="BC1" s="161"/>
-      <c r="BD1" s="161"/>
-      <c r="BE1" s="161"/>
-      <c r="BF1" s="161"/>
-      <c r="BG1" s="161"/>
-      <c r="BH1" s="161"/>
-      <c r="BI1" s="161"/>
-      <c r="BJ1" s="161"/>
-      <c r="BK1" s="161"/>
-      <c r="BL1" s="161"/>
-      <c r="BM1" s="161"/>
-      <c r="BN1" s="161"/>
-      <c r="BO1" s="161"/>
-      <c r="BP1" s="161"/>
-      <c r="BQ1" s="161"/>
-      <c r="BR1" s="161"/>
-      <c r="BS1" s="161"/>
-      <c r="BT1" s="161"/>
-      <c r="BU1" s="161"/>
-      <c r="BV1" s="161"/>
-      <c r="BW1" s="161"/>
-      <c r="BX1" s="161"/>
-      <c r="BY1" s="161"/>
-      <c r="BZ1" s="161"/>
-      <c r="CA1" s="161"/>
-      <c r="CB1" s="161"/>
-      <c r="CC1" s="161"/>
-      <c r="CD1" s="161"/>
-      <c r="CE1" s="161"/>
-      <c r="CF1" s="161"/>
-      <c r="CG1" s="161"/>
-      <c r="CH1" s="161"/>
-      <c r="CI1" s="161"/>
-      <c r="CJ1" s="161"/>
-      <c r="CK1" s="161"/>
-      <c r="CL1" s="161"/>
-      <c r="CM1" s="161"/>
-      <c r="CN1" s="161"/>
-      <c r="CO1" s="161"/>
-      <c r="CP1" s="161"/>
-      <c r="CQ1" s="161"/>
-      <c r="CR1" s="161"/>
-      <c r="CS1" s="161"/>
-      <c r="CT1" s="161"/>
-      <c r="CU1" s="161"/>
-      <c r="CV1" s="161"/>
-      <c r="CW1" s="161"/>
-      <c r="CX1" s="161"/>
-      <c r="CY1" s="161"/>
-      <c r="CZ1" s="161"/>
-      <c r="DA1" s="161"/>
-      <c r="DB1" s="161"/>
-      <c r="DC1" s="161"/>
-      <c r="DD1" s="161"/>
-      <c r="DE1" s="161"/>
-      <c r="DF1" s="161"/>
-      <c r="DG1" s="161"/>
-      <c r="DH1" s="161"/>
-      <c r="DI1" s="161"/>
-      <c r="DJ1" s="161"/>
-      <c r="DK1" s="161"/>
-      <c r="DL1" s="161"/>
-      <c r="DM1" s="161"/>
-      <c r="DN1" s="161"/>
-      <c r="DO1" s="161"/>
-      <c r="DP1" s="161"/>
-      <c r="DQ1" s="161"/>
-      <c r="DR1" s="161"/>
-      <c r="DS1" s="161"/>
-      <c r="DT1" s="161"/>
-      <c r="DU1" s="161"/>
-      <c r="DV1" s="161"/>
-      <c r="DW1" s="161"/>
-      <c r="DX1" s="161"/>
-      <c r="DY1" s="161"/>
-      <c r="DZ1" s="161"/>
-      <c r="EA1" s="161"/>
-      <c r="EB1" s="161"/>
-      <c r="EC1" s="161"/>
-      <c r="ED1" s="161"/>
-      <c r="EE1" s="161"/>
-      <c r="EF1" s="161"/>
-      <c r="EG1" s="161"/>
-      <c r="EH1" s="161"/>
-      <c r="EI1" s="161"/>
-      <c r="EJ1" s="161"/>
-      <c r="EK1" s="161"/>
-      <c r="EL1" s="161"/>
-      <c r="EM1" s="161"/>
-      <c r="EN1" s="161"/>
-      <c r="EO1" s="161"/>
-      <c r="EP1" s="161"/>
-      <c r="EQ1" s="161"/>
-      <c r="ER1" s="161"/>
-      <c r="ES1" s="161"/>
-      <c r="ET1" s="161"/>
-      <c r="EU1" s="161"/>
-      <c r="EV1" s="161"/>
-      <c r="EW1" s="161"/>
-      <c r="EX1" s="161"/>
-      <c r="EY1" s="161"/>
-      <c r="EZ1" s="161"/>
-      <c r="FA1" s="161"/>
-      <c r="FB1" s="161"/>
-      <c r="FC1" s="161"/>
-      <c r="FD1" s="161"/>
-      <c r="FE1" s="161"/>
-      <c r="FF1" s="161"/>
-      <c r="FG1" s="161"/>
-      <c r="FH1" s="161"/>
-      <c r="FI1" s="161"/>
-      <c r="FJ1" s="161"/>
-      <c r="FK1" s="161"/>
-      <c r="FL1" s="161"/>
-      <c r="FM1" s="161"/>
-      <c r="FN1" s="161"/>
-      <c r="FO1" s="161"/>
-      <c r="FP1" s="161"/>
-      <c r="FQ1" s="161"/>
-      <c r="FR1" s="161"/>
-      <c r="FS1" s="161"/>
-      <c r="FT1" s="161"/>
-      <c r="FU1" s="161"/>
-      <c r="FV1" s="161"/>
-      <c r="FW1" s="161"/>
-      <c r="FX1" s="161"/>
-      <c r="FY1" s="161"/>
-      <c r="FZ1" s="161"/>
-      <c r="GA1" s="161"/>
-      <c r="GB1" s="161"/>
-      <c r="GC1" s="161"/>
-      <c r="GD1" s="161"/>
-      <c r="GE1" s="161"/>
-      <c r="GF1" s="161"/>
-      <c r="GG1" s="161"/>
-      <c r="GH1" s="161"/>
-      <c r="GI1" s="161"/>
-      <c r="GJ1" s="161"/>
-      <c r="GK1" s="161"/>
-      <c r="GL1" s="161"/>
-      <c r="GM1" s="161"/>
-      <c r="GN1" s="161"/>
-      <c r="GO1" s="161"/>
-      <c r="GP1" s="161"/>
-      <c r="GQ1" s="161"/>
-      <c r="GR1" s="161"/>
-      <c r="GS1" s="161"/>
-      <c r="GT1" s="161"/>
-      <c r="GU1" s="161"/>
-      <c r="GV1" s="161"/>
-      <c r="GW1" s="161"/>
-      <c r="GX1" s="161"/>
-      <c r="GY1" s="161"/>
-      <c r="GZ1" s="161"/>
-      <c r="HA1" s="161"/>
-      <c r="HB1" s="161"/>
-      <c r="HC1" s="161"/>
-      <c r="HD1" s="161"/>
-      <c r="HE1" s="161"/>
-      <c r="HF1" s="161"/>
-      <c r="HG1" s="161"/>
-      <c r="HH1" s="161"/>
-      <c r="HI1" s="161"/>
-      <c r="HJ1" s="161"/>
-      <c r="HK1" s="161"/>
-      <c r="HL1" s="161"/>
-      <c r="HM1" s="161"/>
-      <c r="HN1" s="161"/>
-      <c r="HO1" s="161"/>
-      <c r="HP1" s="161"/>
-      <c r="HQ1" s="161"/>
-      <c r="HR1" s="161"/>
-      <c r="HS1" s="161"/>
-      <c r="HT1" s="161"/>
-      <c r="HU1" s="161"/>
-      <c r="HV1" s="161"/>
-      <c r="HW1" s="161"/>
-      <c r="HX1" s="161"/>
-      <c r="HY1" s="161"/>
-      <c r="HZ1" s="161"/>
-      <c r="IA1" s="161"/>
-      <c r="IB1" s="161"/>
-      <c r="IC1" s="161"/>
-      <c r="ID1" s="161"/>
-      <c r="IE1" s="161"/>
-      <c r="IF1" s="161"/>
-      <c r="IG1" s="161"/>
-      <c r="IH1" s="161"/>
-      <c r="II1" s="161"/>
-      <c r="IJ1" s="161"/>
-      <c r="IK1" s="161"/>
-      <c r="IL1" s="161"/>
-      <c r="IM1" s="161"/>
-      <c r="IN1" s="161"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
+      <c r="AV1" s="164"/>
+      <c r="AW1" s="164"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
+      <c r="AZ1" s="164"/>
+      <c r="BA1" s="164"/>
+      <c r="BB1" s="164"/>
+      <c r="BC1" s="164"/>
+      <c r="BD1" s="164"/>
+      <c r="BE1" s="164"/>
+      <c r="BF1" s="164"/>
+      <c r="BG1" s="164"/>
+      <c r="BH1" s="164"/>
+      <c r="BI1" s="164"/>
+      <c r="BJ1" s="164"/>
+      <c r="BK1" s="164"/>
+      <c r="BL1" s="164"/>
+      <c r="BM1" s="164"/>
+      <c r="BN1" s="164"/>
+      <c r="BO1" s="164"/>
+      <c r="BP1" s="164"/>
+      <c r="BQ1" s="164"/>
+      <c r="BR1" s="164"/>
+      <c r="BS1" s="164"/>
+      <c r="BT1" s="164"/>
+      <c r="BU1" s="164"/>
+      <c r="BV1" s="164"/>
+      <c r="BW1" s="164"/>
+      <c r="BX1" s="164"/>
+      <c r="BY1" s="164"/>
+      <c r="BZ1" s="164"/>
+      <c r="CA1" s="164"/>
+      <c r="CB1" s="164"/>
+      <c r="CC1" s="164"/>
+      <c r="CD1" s="164"/>
+      <c r="CE1" s="164"/>
+      <c r="CF1" s="164"/>
+      <c r="CG1" s="164"/>
+      <c r="CH1" s="164"/>
+      <c r="CI1" s="164"/>
+      <c r="CJ1" s="164"/>
+      <c r="CK1" s="164"/>
+      <c r="CL1" s="164"/>
+      <c r="CM1" s="164"/>
+      <c r="CN1" s="164"/>
+      <c r="CO1" s="164"/>
+      <c r="CP1" s="164"/>
+      <c r="CQ1" s="164"/>
+      <c r="CR1" s="164"/>
+      <c r="CS1" s="164"/>
+      <c r="CT1" s="164"/>
+      <c r="CU1" s="164"/>
+      <c r="CV1" s="164"/>
+      <c r="CW1" s="164"/>
+      <c r="CX1" s="164"/>
+      <c r="CY1" s="164"/>
+      <c r="CZ1" s="164"/>
+      <c r="DA1" s="164"/>
+      <c r="DB1" s="164"/>
+      <c r="DC1" s="164"/>
+      <c r="DD1" s="164"/>
+      <c r="DE1" s="164"/>
+      <c r="DF1" s="164"/>
+      <c r="DG1" s="164"/>
+      <c r="DH1" s="164"/>
+      <c r="DI1" s="164"/>
+      <c r="DJ1" s="164"/>
+      <c r="DK1" s="164"/>
+      <c r="DL1" s="164"/>
+      <c r="DM1" s="164"/>
+      <c r="DN1" s="164"/>
+      <c r="DO1" s="164"/>
+      <c r="DP1" s="164"/>
+      <c r="DQ1" s="164"/>
+      <c r="DR1" s="164"/>
+      <c r="DS1" s="164"/>
+      <c r="DT1" s="164"/>
+      <c r="DU1" s="164"/>
+      <c r="DV1" s="164"/>
+      <c r="DW1" s="164"/>
+      <c r="DX1" s="164"/>
+      <c r="DY1" s="164"/>
+      <c r="DZ1" s="164"/>
+      <c r="EA1" s="164"/>
+      <c r="EB1" s="164"/>
+      <c r="EC1" s="164"/>
+      <c r="ED1" s="164"/>
+      <c r="EE1" s="164"/>
+      <c r="EF1" s="164"/>
+      <c r="EG1" s="164"/>
+      <c r="EH1" s="164"/>
+      <c r="EI1" s="164"/>
+      <c r="EJ1" s="164"/>
+      <c r="EK1" s="164"/>
+      <c r="EL1" s="164"/>
+      <c r="EM1" s="164"/>
+      <c r="EN1" s="164"/>
+      <c r="EO1" s="164"/>
+      <c r="EP1" s="164"/>
+      <c r="EQ1" s="164"/>
+      <c r="ER1" s="164"/>
+      <c r="ES1" s="164"/>
+      <c r="ET1" s="164"/>
+      <c r="EU1" s="164"/>
+      <c r="EV1" s="164"/>
+      <c r="EW1" s="164"/>
+      <c r="EX1" s="164"/>
+      <c r="EY1" s="164"/>
+      <c r="EZ1" s="164"/>
+      <c r="FA1" s="164"/>
+      <c r="FB1" s="164"/>
+      <c r="FC1" s="164"/>
+      <c r="FD1" s="164"/>
+      <c r="FE1" s="164"/>
+      <c r="FF1" s="164"/>
+      <c r="FG1" s="164"/>
+      <c r="FH1" s="164"/>
+      <c r="FI1" s="164"/>
+      <c r="FJ1" s="164"/>
+      <c r="FK1" s="164"/>
+      <c r="FL1" s="164"/>
+      <c r="FM1" s="164"/>
+      <c r="FN1" s="164"/>
+      <c r="FO1" s="164"/>
+      <c r="FP1" s="164"/>
+      <c r="FQ1" s="164"/>
+      <c r="FR1" s="164"/>
+      <c r="FS1" s="164"/>
+      <c r="FT1" s="164"/>
+      <c r="FU1" s="164"/>
+      <c r="FV1" s="164"/>
+      <c r="FW1" s="164"/>
+      <c r="FX1" s="164"/>
+      <c r="FY1" s="164"/>
+      <c r="FZ1" s="164"/>
+      <c r="GA1" s="164"/>
+      <c r="GB1" s="164"/>
+      <c r="GC1" s="164"/>
+      <c r="GD1" s="164"/>
+      <c r="GE1" s="164"/>
+      <c r="GF1" s="164"/>
+      <c r="GG1" s="164"/>
+      <c r="GH1" s="164"/>
+      <c r="GI1" s="164"/>
+      <c r="GJ1" s="164"/>
+      <c r="GK1" s="164"/>
+      <c r="GL1" s="164"/>
+      <c r="GM1" s="164"/>
+      <c r="GN1" s="164"/>
+      <c r="GO1" s="164"/>
+      <c r="GP1" s="164"/>
+      <c r="GQ1" s="164"/>
+      <c r="GR1" s="164"/>
+      <c r="GS1" s="164"/>
+      <c r="GT1" s="164"/>
+      <c r="GU1" s="164"/>
+      <c r="GV1" s="164"/>
+      <c r="GW1" s="164"/>
+      <c r="GX1" s="164"/>
+      <c r="GY1" s="164"/>
+      <c r="GZ1" s="164"/>
+      <c r="HA1" s="164"/>
+      <c r="HB1" s="164"/>
+      <c r="HC1" s="164"/>
+      <c r="HD1" s="164"/>
+      <c r="HE1" s="164"/>
+      <c r="HF1" s="164"/>
+      <c r="HG1" s="164"/>
+      <c r="HH1" s="164"/>
+      <c r="HI1" s="164"/>
+      <c r="HJ1" s="164"/>
+      <c r="HK1" s="164"/>
+      <c r="HL1" s="164"/>
+      <c r="HM1" s="164"/>
+      <c r="HN1" s="164"/>
+      <c r="HO1" s="164"/>
+      <c r="HP1" s="164"/>
+      <c r="HQ1" s="164"/>
+      <c r="HR1" s="164"/>
+      <c r="HS1" s="164"/>
+      <c r="HT1" s="164"/>
+      <c r="HU1" s="164"/>
+      <c r="HV1" s="164"/>
+      <c r="HW1" s="164"/>
+      <c r="HX1" s="164"/>
+      <c r="HY1" s="164"/>
+      <c r="HZ1" s="164"/>
+      <c r="IA1" s="164"/>
+      <c r="IB1" s="164"/>
+      <c r="IC1" s="164"/>
+      <c r="ID1" s="164"/>
+      <c r="IE1" s="164"/>
+      <c r="IF1" s="164"/>
+      <c r="IG1" s="164"/>
+      <c r="IH1" s="164"/>
+      <c r="II1" s="164"/>
+      <c r="IJ1" s="164"/>
+      <c r="IK1" s="164"/>
+      <c r="IL1" s="164"/>
+      <c r="IM1" s="164"/>
+      <c r="IN1" s="164"/>
     </row>
     <row r="2" spans="1:248" s="48" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="49"/>
@@ -10106,274 +10149,274 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
-      <c r="I2" s="162" t="s">
+      <c r="I2" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="162"/>
-      <c r="M2" s="162"/>
-      <c r="N2" s="162"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="162"/>
-      <c r="Q2" s="162"/>
-      <c r="R2" s="162"/>
-      <c r="S2" s="162"/>
-      <c r="T2" s="162"/>
-      <c r="U2" s="162"/>
-      <c r="V2" s="162" t="s">
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="W2" s="162"/>
-      <c r="X2" s="162"/>
-      <c r="Y2" s="162"/>
-      <c r="Z2" s="162"/>
-      <c r="AA2" s="162"/>
-      <c r="AB2" s="162"/>
-      <c r="AC2" s="162" t="s">
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
+      <c r="AA2" s="165"/>
+      <c r="AB2" s="165"/>
+      <c r="AC2" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="162"/>
-      <c r="AE2" s="162"/>
-      <c r="AF2" s="162"/>
-      <c r="AG2" s="162"/>
-      <c r="AH2" s="162"/>
-      <c r="AI2" s="162" t="s">
+      <c r="AD2" s="165"/>
+      <c r="AE2" s="165"/>
+      <c r="AF2" s="165"/>
+      <c r="AG2" s="165"/>
+      <c r="AH2" s="165"/>
+      <c r="AI2" s="165" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="162"/>
-      <c r="AK2" s="162"/>
-      <c r="AL2" s="162"/>
-      <c r="AM2" s="162"/>
+      <c r="AJ2" s="165"/>
+      <c r="AK2" s="165"/>
+      <c r="AL2" s="165"/>
+      <c r="AM2" s="165"/>
       <c r="AN2" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="163" t="s">
+      <c r="AO2" s="166" t="s">
         <v>335</v>
       </c>
-      <c r="AP2" s="163"/>
-      <c r="AQ2" s="163"/>
-      <c r="AR2" s="163"/>
-      <c r="AS2" s="163"/>
-      <c r="AT2" s="163"/>
-      <c r="AU2" s="163"/>
-      <c r="AV2" s="163"/>
-      <c r="AW2" s="163"/>
-      <c r="AX2" s="163"/>
-      <c r="AY2" s="163"/>
-      <c r="AZ2" s="163"/>
-      <c r="BA2" s="163"/>
-      <c r="BB2" s="163"/>
-      <c r="BC2" s="163"/>
-      <c r="BD2" s="163"/>
-      <c r="BE2" s="163"/>
-      <c r="BF2" s="163"/>
-      <c r="BG2" s="163"/>
-      <c r="BH2" s="163"/>
-      <c r="BI2" s="164" t="s">
+      <c r="AP2" s="166"/>
+      <c r="AQ2" s="166"/>
+      <c r="AR2" s="166"/>
+      <c r="AS2" s="166"/>
+      <c r="AT2" s="166"/>
+      <c r="AU2" s="166"/>
+      <c r="AV2" s="166"/>
+      <c r="AW2" s="166"/>
+      <c r="AX2" s="166"/>
+      <c r="AY2" s="166"/>
+      <c r="AZ2" s="166"/>
+      <c r="BA2" s="166"/>
+      <c r="BB2" s="166"/>
+      <c r="BC2" s="166"/>
+      <c r="BD2" s="166"/>
+      <c r="BE2" s="166"/>
+      <c r="BF2" s="166"/>
+      <c r="BG2" s="166"/>
+      <c r="BH2" s="166"/>
+      <c r="BI2" s="167" t="s">
         <v>334</v>
       </c>
-      <c r="BJ2" s="164"/>
-      <c r="BK2" s="164"/>
-      <c r="BL2" s="164"/>
-      <c r="BM2" s="164"/>
-      <c r="BN2" s="164"/>
-      <c r="BO2" s="164"/>
-      <c r="BP2" s="164"/>
-      <c r="BQ2" s="164"/>
-      <c r="BR2" s="164"/>
-      <c r="BS2" s="164"/>
-      <c r="BT2" s="164"/>
-      <c r="BU2" s="164"/>
-      <c r="BV2" s="164"/>
-      <c r="BW2" s="164"/>
-      <c r="BX2" s="164"/>
-      <c r="BY2" s="166" t="s">
+      <c r="BJ2" s="167"/>
+      <c r="BK2" s="167"/>
+      <c r="BL2" s="167"/>
+      <c r="BM2" s="167"/>
+      <c r="BN2" s="167"/>
+      <c r="BO2" s="167"/>
+      <c r="BP2" s="167"/>
+      <c r="BQ2" s="167"/>
+      <c r="BR2" s="167"/>
+      <c r="BS2" s="167"/>
+      <c r="BT2" s="167"/>
+      <c r="BU2" s="167"/>
+      <c r="BV2" s="167"/>
+      <c r="BW2" s="167"/>
+      <c r="BX2" s="167"/>
+      <c r="BY2" s="169" t="s">
         <v>333</v>
       </c>
-      <c r="BZ2" s="166"/>
-      <c r="CA2" s="166"/>
-      <c r="CB2" s="166"/>
-      <c r="CC2" s="166"/>
-      <c r="CD2" s="166"/>
-      <c r="CE2" s="166"/>
-      <c r="CF2" s="166"/>
-      <c r="CG2" s="166"/>
-      <c r="CH2" s="166"/>
-      <c r="CI2" s="166"/>
-      <c r="CJ2" s="167" t="s">
+      <c r="BZ2" s="169"/>
+      <c r="CA2" s="169"/>
+      <c r="CB2" s="169"/>
+      <c r="CC2" s="169"/>
+      <c r="CD2" s="169"/>
+      <c r="CE2" s="169"/>
+      <c r="CF2" s="169"/>
+      <c r="CG2" s="169"/>
+      <c r="CH2" s="169"/>
+      <c r="CI2" s="169"/>
+      <c r="CJ2" s="170" t="s">
         <v>332</v>
       </c>
-      <c r="CK2" s="167"/>
-      <c r="CL2" s="167"/>
-      <c r="CM2" s="167"/>
-      <c r="CN2" s="167"/>
-      <c r="CO2" s="167"/>
-      <c r="CP2" s="167"/>
-      <c r="CQ2" s="167"/>
-      <c r="CR2" s="167"/>
-      <c r="CS2" s="167"/>
-      <c r="CT2" s="167"/>
-      <c r="CU2" s="167"/>
-      <c r="CV2" s="167"/>
-      <c r="CW2" s="167"/>
-      <c r="CX2" s="167"/>
-      <c r="CY2" s="167"/>
-      <c r="CZ2" s="167"/>
-      <c r="DA2" s="167"/>
-      <c r="DB2" s="167"/>
-      <c r="DC2" s="167"/>
-      <c r="DD2" s="167"/>
-      <c r="DE2" s="168" t="s">
+      <c r="CK2" s="170"/>
+      <c r="CL2" s="170"/>
+      <c r="CM2" s="170"/>
+      <c r="CN2" s="170"/>
+      <c r="CO2" s="170"/>
+      <c r="CP2" s="170"/>
+      <c r="CQ2" s="170"/>
+      <c r="CR2" s="170"/>
+      <c r="CS2" s="170"/>
+      <c r="CT2" s="170"/>
+      <c r="CU2" s="170"/>
+      <c r="CV2" s="170"/>
+      <c r="CW2" s="170"/>
+      <c r="CX2" s="170"/>
+      <c r="CY2" s="170"/>
+      <c r="CZ2" s="170"/>
+      <c r="DA2" s="170"/>
+      <c r="DB2" s="170"/>
+      <c r="DC2" s="170"/>
+      <c r="DD2" s="170"/>
+      <c r="DE2" s="171" t="s">
         <v>331</v>
       </c>
-      <c r="DF2" s="168"/>
-      <c r="DG2" s="168"/>
-      <c r="DH2" s="168"/>
-      <c r="DI2" s="168"/>
-      <c r="DJ2" s="169" t="s">
+      <c r="DF2" s="171"/>
+      <c r="DG2" s="171"/>
+      <c r="DH2" s="171"/>
+      <c r="DI2" s="171"/>
+      <c r="DJ2" s="158" t="s">
         <v>330</v>
       </c>
-      <c r="DK2" s="169"/>
-      <c r="DL2" s="169"/>
-      <c r="DM2" s="169"/>
-      <c r="DN2" s="170" t="s">
+      <c r="DK2" s="158"/>
+      <c r="DL2" s="158"/>
+      <c r="DM2" s="158"/>
+      <c r="DN2" s="159" t="s">
         <v>329</v>
       </c>
-      <c r="DO2" s="170"/>
-      <c r="DP2" s="170"/>
-      <c r="DQ2" s="170"/>
-      <c r="DR2" s="170"/>
-      <c r="DS2" s="170"/>
-      <c r="DT2" s="157" t="s">
+      <c r="DO2" s="159"/>
+      <c r="DP2" s="159"/>
+      <c r="DQ2" s="159"/>
+      <c r="DR2" s="159"/>
+      <c r="DS2" s="159"/>
+      <c r="DT2" s="160" t="s">
         <v>328</v>
       </c>
-      <c r="DU2" s="157"/>
-      <c r="DV2" s="157"/>
-      <c r="DW2" s="157"/>
-      <c r="DX2" s="157"/>
-      <c r="DY2" s="157"/>
-      <c r="DZ2" s="157"/>
-      <c r="EA2" s="157"/>
-      <c r="EB2" s="157"/>
-      <c r="EC2" s="157"/>
-      <c r="ED2" s="157"/>
-      <c r="EE2" s="157"/>
-      <c r="EF2" s="157"/>
-      <c r="EG2" s="157"/>
-      <c r="EH2" s="157"/>
-      <c r="EI2" s="157"/>
-      <c r="EJ2" s="157"/>
-      <c r="EK2" s="157"/>
-      <c r="EL2" s="157"/>
-      <c r="EM2" s="157"/>
-      <c r="EN2" s="157"/>
-      <c r="EO2" s="165" t="s">
+      <c r="DU2" s="160"/>
+      <c r="DV2" s="160"/>
+      <c r="DW2" s="160"/>
+      <c r="DX2" s="160"/>
+      <c r="DY2" s="160"/>
+      <c r="DZ2" s="160"/>
+      <c r="EA2" s="160"/>
+      <c r="EB2" s="160"/>
+      <c r="EC2" s="160"/>
+      <c r="ED2" s="160"/>
+      <c r="EE2" s="160"/>
+      <c r="EF2" s="160"/>
+      <c r="EG2" s="160"/>
+      <c r="EH2" s="160"/>
+      <c r="EI2" s="160"/>
+      <c r="EJ2" s="160"/>
+      <c r="EK2" s="160"/>
+      <c r="EL2" s="160"/>
+      <c r="EM2" s="160"/>
+      <c r="EN2" s="160"/>
+      <c r="EO2" s="168" t="s">
         <v>336</v>
       </c>
-      <c r="EP2" s="165"/>
-      <c r="EQ2" s="165"/>
-      <c r="ER2" s="165"/>
-      <c r="ES2" s="165"/>
-      <c r="ET2" s="165"/>
-      <c r="EU2" s="165"/>
-      <c r="EV2" s="165"/>
-      <c r="EW2" s="165"/>
-      <c r="EX2" s="165"/>
-      <c r="EY2" s="165"/>
-      <c r="EZ2" s="165"/>
-      <c r="FA2" s="165"/>
-      <c r="FB2" s="165"/>
-      <c r="FC2" s="165"/>
-      <c r="FD2" s="165"/>
-      <c r="FE2" s="165"/>
-      <c r="FF2" s="165"/>
-      <c r="FG2" s="165"/>
-      <c r="FH2" s="165"/>
-      <c r="FI2" s="165"/>
-      <c r="FJ2" s="165"/>
-      <c r="FK2" s="165"/>
-      <c r="FL2" s="165"/>
-      <c r="FM2" s="165"/>
-      <c r="FN2" s="165"/>
-      <c r="FO2" s="165"/>
-      <c r="FP2" s="165"/>
-      <c r="FQ2" s="165"/>
-      <c r="FR2" s="165"/>
-      <c r="FS2" s="165"/>
-      <c r="FT2" s="165"/>
-      <c r="FU2" s="165"/>
-      <c r="FV2" s="165"/>
-      <c r="FW2" s="165"/>
-      <c r="FX2" s="165"/>
-      <c r="FY2" s="165"/>
-      <c r="FZ2" s="165"/>
-      <c r="GA2" s="165"/>
-      <c r="GB2" s="165"/>
-      <c r="GC2" s="165"/>
-      <c r="GD2" s="165"/>
-      <c r="GE2" s="165"/>
-      <c r="GF2" s="165"/>
-      <c r="GG2" s="165"/>
-      <c r="GH2" s="165"/>
-      <c r="GI2" s="165"/>
-      <c r="GJ2" s="165"/>
-      <c r="GK2" s="165"/>
-      <c r="GL2" s="165"/>
-      <c r="GM2" s="165"/>
-      <c r="GN2" s="165"/>
-      <c r="GO2" s="165"/>
-      <c r="GP2" s="165"/>
-      <c r="GQ2" s="165"/>
-      <c r="GR2" s="165"/>
-      <c r="GS2" s="165"/>
-      <c r="GT2" s="165"/>
-      <c r="GU2" s="165"/>
-      <c r="GV2" s="165"/>
-      <c r="GW2" s="165"/>
-      <c r="GX2" s="165"/>
-      <c r="GY2" s="165"/>
-      <c r="GZ2" s="165"/>
-      <c r="HA2" s="165"/>
-      <c r="HB2" s="165"/>
-      <c r="HC2" s="165"/>
-      <c r="HD2" s="165"/>
-      <c r="HE2" s="165"/>
-      <c r="HF2" s="165"/>
-      <c r="HG2" s="165"/>
-      <c r="HH2" s="165"/>
-      <c r="HI2" s="165"/>
-      <c r="HJ2" s="165"/>
-      <c r="HK2" s="165"/>
-      <c r="HL2" s="165"/>
-      <c r="HM2" s="165"/>
-      <c r="HN2" s="165"/>
-      <c r="HO2" s="165"/>
-      <c r="HP2" s="165"/>
-      <c r="HQ2" s="165"/>
-      <c r="HR2" s="165"/>
-      <c r="HS2" s="165"/>
-      <c r="HT2" s="165"/>
-      <c r="HU2" s="165"/>
-      <c r="HV2" s="165"/>
-      <c r="HW2" s="165"/>
-      <c r="HX2" s="165"/>
-      <c r="HY2" s="165"/>
-      <c r="HZ2" s="165"/>
-      <c r="IA2" s="165"/>
-      <c r="IB2" s="165"/>
-      <c r="IC2" s="165"/>
-      <c r="ID2" s="165"/>
-      <c r="IE2" s="165"/>
-      <c r="IF2" s="165"/>
-      <c r="IG2" s="165"/>
-      <c r="IH2" s="165"/>
-      <c r="II2" s="165"/>
-      <c r="IJ2" s="165"/>
-      <c r="IK2" s="165"/>
-      <c r="IL2" s="165"/>
-      <c r="IM2" s="165"/>
-      <c r="IN2" s="165"/>
+      <c r="EP2" s="168"/>
+      <c r="EQ2" s="168"/>
+      <c r="ER2" s="168"/>
+      <c r="ES2" s="168"/>
+      <c r="ET2" s="168"/>
+      <c r="EU2" s="168"/>
+      <c r="EV2" s="168"/>
+      <c r="EW2" s="168"/>
+      <c r="EX2" s="168"/>
+      <c r="EY2" s="168"/>
+      <c r="EZ2" s="168"/>
+      <c r="FA2" s="168"/>
+      <c r="FB2" s="168"/>
+      <c r="FC2" s="168"/>
+      <c r="FD2" s="168"/>
+      <c r="FE2" s="168"/>
+      <c r="FF2" s="168"/>
+      <c r="FG2" s="168"/>
+      <c r="FH2" s="168"/>
+      <c r="FI2" s="168"/>
+      <c r="FJ2" s="168"/>
+      <c r="FK2" s="168"/>
+      <c r="FL2" s="168"/>
+      <c r="FM2" s="168"/>
+      <c r="FN2" s="168"/>
+      <c r="FO2" s="168"/>
+      <c r="FP2" s="168"/>
+      <c r="FQ2" s="168"/>
+      <c r="FR2" s="168"/>
+      <c r="FS2" s="168"/>
+      <c r="FT2" s="168"/>
+      <c r="FU2" s="168"/>
+      <c r="FV2" s="168"/>
+      <c r="FW2" s="168"/>
+      <c r="FX2" s="168"/>
+      <c r="FY2" s="168"/>
+      <c r="FZ2" s="168"/>
+      <c r="GA2" s="168"/>
+      <c r="GB2" s="168"/>
+      <c r="GC2" s="168"/>
+      <c r="GD2" s="168"/>
+      <c r="GE2" s="168"/>
+      <c r="GF2" s="168"/>
+      <c r="GG2" s="168"/>
+      <c r="GH2" s="168"/>
+      <c r="GI2" s="168"/>
+      <c r="GJ2" s="168"/>
+      <c r="GK2" s="168"/>
+      <c r="GL2" s="168"/>
+      <c r="GM2" s="168"/>
+      <c r="GN2" s="168"/>
+      <c r="GO2" s="168"/>
+      <c r="GP2" s="168"/>
+      <c r="GQ2" s="168"/>
+      <c r="GR2" s="168"/>
+      <c r="GS2" s="168"/>
+      <c r="GT2" s="168"/>
+      <c r="GU2" s="168"/>
+      <c r="GV2" s="168"/>
+      <c r="GW2" s="168"/>
+      <c r="GX2" s="168"/>
+      <c r="GY2" s="168"/>
+      <c r="GZ2" s="168"/>
+      <c r="HA2" s="168"/>
+      <c r="HB2" s="168"/>
+      <c r="HC2" s="168"/>
+      <c r="HD2" s="168"/>
+      <c r="HE2" s="168"/>
+      <c r="HF2" s="168"/>
+      <c r="HG2" s="168"/>
+      <c r="HH2" s="168"/>
+      <c r="HI2" s="168"/>
+      <c r="HJ2" s="168"/>
+      <c r="HK2" s="168"/>
+      <c r="HL2" s="168"/>
+      <c r="HM2" s="168"/>
+      <c r="HN2" s="168"/>
+      <c r="HO2" s="168"/>
+      <c r="HP2" s="168"/>
+      <c r="HQ2" s="168"/>
+      <c r="HR2" s="168"/>
+      <c r="HS2" s="168"/>
+      <c r="HT2" s="168"/>
+      <c r="HU2" s="168"/>
+      <c r="HV2" s="168"/>
+      <c r="HW2" s="168"/>
+      <c r="HX2" s="168"/>
+      <c r="HY2" s="168"/>
+      <c r="HZ2" s="168"/>
+      <c r="IA2" s="168"/>
+      <c r="IB2" s="168"/>
+      <c r="IC2" s="168"/>
+      <c r="ID2" s="168"/>
+      <c r="IE2" s="168"/>
+      <c r="IF2" s="168"/>
+      <c r="IG2" s="168"/>
+      <c r="IH2" s="168"/>
+      <c r="II2" s="168"/>
+      <c r="IJ2" s="168"/>
+      <c r="IK2" s="168"/>
+      <c r="IL2" s="168"/>
+      <c r="IM2" s="168"/>
+      <c r="IN2" s="168"/>
     </row>
     <row r="3" spans="1:248" s="58" customFormat="1" ht="64">
       <c r="A3" s="49" t="s">
@@ -11389,6 +11432,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="DE2:DI2"/>
+    <mergeCell ref="DJ2:DM2"/>
     <mergeCell ref="DN2:DS2"/>
     <mergeCell ref="DT2:EN2"/>
     <mergeCell ref="A1:D1"/>
@@ -11404,8 +11449,6 @@
     <mergeCell ref="EO2:IN2"/>
     <mergeCell ref="BY2:CI2"/>
     <mergeCell ref="CJ2:DD2"/>
-    <mergeCell ref="DE2:DI2"/>
-    <mergeCell ref="DJ2:DM2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.0.31-SNAPSHOT print area, add image
</commit_message>
<xml_diff>
--- a/src/test/resources/ceping.xlsx
+++ b/src/test/resources/ceping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94199C1A-7A30-C54F-9A79-9A8E7AEA129C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02AB9C1-0079-FF41-8F8F-714B5C76AD6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
   <sheets>
     <sheet name="有评语-模板" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">有评语!$A$22:$G$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'有评语-模板'!$A$9:$G$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">无评语!$A$1:$G$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'无评语-模板'!$A$1:$G$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'无总评语-模板'!$A$1:$G$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">有评语!$A$1:$G$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'有评语-模板'!$A$1:$G$124</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1890,7 +1893,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2111,9 +2114,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6961,8 +6961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0B56D7-DA51-554E-86D1-0655EAEF35DF}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView view="pageBreakPreview" zoomScale="125" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:AM1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -6978,42 +6978,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="77" t="s">
         <v>352</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="78"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="77" t="s">
         <v>116</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -7025,10 +7025,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>6</v>
@@ -7039,27 +7039,27 @@
       <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="83">
         <v>1.2</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="17" customHeight="1">
       <c r="A6" s="38"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86" t="s">
+      <c r="B6" s="84"/>
+      <c r="C6" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
     </row>
     <row r="7" spans="1:7" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A7" s="74"/>
@@ -7075,28 +7075,28 @@
       <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="80"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="79"/>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="81" t="s">
+      <c r="C9" s="79"/>
+      <c r="D9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="81"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="33" t="s">
         <v>13</v>
       </c>
@@ -7145,10 +7145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4695B6-0F6F-5D43-8678-5A2A085127DD}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView view="pageBreakPreview" zoomScale="125" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7163,114 +7163,113 @@
     <col min="8" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A2" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-    </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
+      <c r="A3" s="77" t="s">
         <v>352</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="78"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="77" t="s">
         <v>116</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="8" customFormat="1" ht="38.25" customHeight="1">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="38.25" customHeight="1">
       <c r="A4" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="70"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="10"/>
       <c r="F4" s="72" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="70"/>
-      <c r="H4" s="75"/>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="87" t="s">
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A5" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="83">
         <v>1.2</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="17" customHeight="1">
-      <c r="A6" s="88"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86" t="s">
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="17" customHeight="1">
+      <c r="A6" s="87"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-    </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="79" t="s">
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="80"/>
-    </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="18" customHeight="1">
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="79"/>
+    </row>
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="81"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="69" t="s">
         <v>13</v>
       </c>
@@ -7278,7 +7277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
+    <row r="9" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="A9" s="72" t="s">
         <v>15</v>
       </c>
@@ -7320,10 +7319,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6F288-1AD6-674A-831C-FFD9B35C5B5E}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="125" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7335,58 +7334,42 @@
     <col min="5" max="5" width="15.5" style="28" customWidth="1"/>
     <col min="6" max="6" width="14" style="28" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="9" style="28"/>
-    <col min="9" max="9" width="9.6640625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="9" style="28"/>
-    <col min="11" max="15" width="9" style="30"/>
-    <col min="16" max="16384" width="9" style="28"/>
+    <col min="8" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="I1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A2" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="I2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" ht="27" customHeight="1">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="61" t="s">
         <v>349</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="6" t="s">
         <v>350</v>
       </c>
@@ -7396,94 +7379,66 @@
       <c r="G3" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="K3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" ht="36.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="36.75" customHeight="1">
       <c r="A4" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="61"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="10"/>
       <c r="F4" s="62" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="61"/>
-      <c r="I4" s="9"/>
-      <c r="K4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" ht="63" customHeight="1">
-      <c r="A5" s="89" t="s">
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="63" customHeight="1">
+      <c r="A5" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="90">
+      <c r="B5" s="88"/>
+      <c r="C5" s="89">
         <v>6</v>
       </c>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A6" s="79" t="s">
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="90"/>
+    </row>
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A6" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" ht="18" customHeight="1">
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="79"/>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="80"/>
       <c r="F7" s="60" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
+    </row>
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="A8" s="66" t="s">
         <v>15</v>
       </c>
@@ -7499,9 +7454,6 @@
       <c r="G8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7527,8 +7479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B0BF8C-2422-9C41-8C7B-F10DC2F2FA45}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="177" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView zoomScale="177" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7544,36 +7496,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>3</v>
@@ -7585,10 +7537,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="10"/>
       <c r="F4" s="25" t="s">
         <v>6</v>
@@ -7596,186 +7548,186 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="95">
         <v>1.2</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="97"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="93"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="100"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="93"/>
-      <c r="B7" s="102" t="s">
+      <c r="A7" s="92"/>
+      <c r="B7" s="101" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="93"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="85" t="s">
+      <c r="A8" s="92"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="93"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="93"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A11" s="93"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="107"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="106"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="93"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A13" s="93"/>
-      <c r="B13" s="103"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A14" s="93"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="107"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="106"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A15" s="93"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="107"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="106"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A16" s="93"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106"/>
-      <c r="G16" s="107"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="106"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A17" s="93"/>
-      <c r="B17" s="103"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="107"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="106"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A18" s="93"/>
-      <c r="B18" s="103"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A19" s="93"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="94" t="s">
+      <c r="A19" s="92"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="104"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A20" s="93"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="104"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="79"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="81" t="s">
+      <c r="C22" s="79"/>
+      <c r="D22" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="81"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="16" t="s">
         <v>13</v>
       </c>
@@ -7784,548 +7736,548 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="109" t="s">
+      <c r="A23" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="113"/>
-      <c r="D23" s="114" t="s">
+      <c r="C23" s="112"/>
+      <c r="D23" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="115"/>
+      <c r="E23" s="114"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="110"/>
-      <c r="B24" s="116" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="114" t="s">
+      <c r="C24" s="116"/>
+      <c r="D24" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="115"/>
-      <c r="F24" s="122">
+      <c r="E24" s="114"/>
+      <c r="F24" s="121">
         <v>2</v>
       </c>
-      <c r="G24" s="125" t="s">
+      <c r="G24" s="124" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="110"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="114" t="s">
+      <c r="A25" s="109"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="115"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="126"/>
+      <c r="E25" s="114"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="125"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="110"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="114" t="s">
+      <c r="A26" s="109"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="126"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="125"/>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="110"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="114" t="s">
+      <c r="A27" s="109"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="115"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="126"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="125"/>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="110"/>
-      <c r="B28" s="120"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="114" t="s">
+      <c r="A28" s="109"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="115"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="126"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="125"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="110"/>
-      <c r="B29" s="128" t="s">
+      <c r="A29" s="109"/>
+      <c r="B29" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="129"/>
-      <c r="D29" s="114" t="s">
+      <c r="C29" s="128"/>
+      <c r="D29" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="115"/>
-      <c r="F29" s="122">
+      <c r="E29" s="114"/>
+      <c r="F29" s="121">
         <v>2</v>
       </c>
-      <c r="G29" s="126"/>
+      <c r="G29" s="125"/>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="110"/>
-      <c r="B30" s="132"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="114" t="s">
+      <c r="A30" s="109"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="115"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="126"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="125"/>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="110"/>
-      <c r="B31" s="132"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="114" t="s">
+      <c r="A31" s="109"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="115"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="126"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="125"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="110"/>
-      <c r="B32" s="132"/>
-      <c r="C32" s="133"/>
-      <c r="D32" s="114" t="s">
+      <c r="A32" s="109"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="115"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="126"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="125"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="110"/>
-      <c r="B33" s="130"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="114" t="s">
+      <c r="A33" s="109"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="130"/>
+      <c r="D33" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="115"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="127"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="126"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="110"/>
-      <c r="B34" s="128" t="s">
+      <c r="A34" s="109"/>
+      <c r="B34" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="129"/>
-      <c r="D34" s="114" t="s">
+      <c r="C34" s="128"/>
+      <c r="D34" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="115"/>
-      <c r="F34" s="122">
+      <c r="E34" s="114"/>
+      <c r="F34" s="121">
         <v>0</v>
       </c>
-      <c r="G34" s="125" t="s">
+      <c r="G34" s="124" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="110"/>
-      <c r="B35" s="130"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="114" t="s">
+      <c r="A35" s="109"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="130"/>
+      <c r="D35" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="115"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="127"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="126"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="110"/>
-      <c r="B36" s="116" t="s">
+      <c r="A36" s="109"/>
+      <c r="B36" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="117"/>
-      <c r="D36" s="114" t="s">
+      <c r="C36" s="116"/>
+      <c r="D36" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="115"/>
-      <c r="F36" s="122">
+      <c r="E36" s="114"/>
+      <c r="F36" s="121">
         <v>2</v>
       </c>
-      <c r="G36" s="125" t="s">
+      <c r="G36" s="124" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="110"/>
-      <c r="B37" s="118"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="114" t="s">
+      <c r="A37" s="109"/>
+      <c r="B37" s="117"/>
+      <c r="C37" s="118"/>
+      <c r="D37" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="115"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="126"/>
+      <c r="E37" s="114"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="125"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="110"/>
-      <c r="B38" s="118"/>
-      <c r="C38" s="119"/>
-      <c r="D38" s="114" t="s">
+      <c r="A38" s="109"/>
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="115"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="126"/>
+      <c r="E38" s="114"/>
+      <c r="F38" s="122"/>
+      <c r="G38" s="125"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="110"/>
-      <c r="B39" s="118"/>
-      <c r="C39" s="119"/>
-      <c r="D39" s="114" t="s">
+      <c r="A39" s="109"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="115"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="126"/>
+      <c r="E39" s="114"/>
+      <c r="F39" s="122"/>
+      <c r="G39" s="125"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="110"/>
-      <c r="B40" s="120"/>
-      <c r="C40" s="121"/>
-      <c r="D40" s="114" t="s">
+      <c r="A40" s="109"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="120"/>
+      <c r="D40" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="115"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="126"/>
+      <c r="E40" s="114"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="125"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="110"/>
-      <c r="B41" s="128" t="s">
+      <c r="A41" s="109"/>
+      <c r="B41" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="129"/>
-      <c r="D41" s="114" t="s">
+      <c r="C41" s="128"/>
+      <c r="D41" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="115"/>
-      <c r="F41" s="122">
+      <c r="E41" s="114"/>
+      <c r="F41" s="121">
         <v>2</v>
       </c>
-      <c r="G41" s="126"/>
+      <c r="G41" s="125"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="110"/>
-      <c r="B42" s="132"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="114" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="115"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="126"/>
+      <c r="E42" s="114"/>
+      <c r="F42" s="122"/>
+      <c r="G42" s="125"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="110"/>
-      <c r="B43" s="132"/>
-      <c r="C43" s="133"/>
-      <c r="D43" s="114" t="s">
+      <c r="A43" s="109"/>
+      <c r="B43" s="131"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="115"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="126"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="122"/>
+      <c r="G43" s="125"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="110"/>
-      <c r="B44" s="132"/>
-      <c r="C44" s="133"/>
-      <c r="D44" s="114" t="s">
+      <c r="A44" s="109"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="132"/>
+      <c r="D44" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="115"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="126"/>
+      <c r="E44" s="114"/>
+      <c r="F44" s="122"/>
+      <c r="G44" s="125"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="110"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="114" t="s">
+      <c r="A45" s="109"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="130"/>
+      <c r="D45" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="115"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="126"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="125"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="110"/>
-      <c r="B46" s="128" t="s">
+      <c r="A46" s="109"/>
+      <c r="B46" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="129"/>
-      <c r="D46" s="114" t="s">
+      <c r="C46" s="128"/>
+      <c r="D46" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="115"/>
-      <c r="F46" s="122">
+      <c r="E46" s="114"/>
+      <c r="F46" s="121">
         <v>2</v>
       </c>
-      <c r="G46" s="126"/>
+      <c r="G46" s="125"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="110"/>
-      <c r="B47" s="132"/>
-      <c r="C47" s="133"/>
-      <c r="D47" s="114" t="s">
+      <c r="A47" s="109"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="132"/>
+      <c r="D47" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="115"/>
-      <c r="F47" s="123"/>
-      <c r="G47" s="126"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="122"/>
+      <c r="G47" s="125"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="110"/>
-      <c r="B48" s="132"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="114" t="s">
+      <c r="A48" s="109"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="132"/>
+      <c r="D48" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="115"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="126"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="122"/>
+      <c r="G48" s="125"/>
     </row>
     <row r="49" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="110"/>
-      <c r="B49" s="132"/>
-      <c r="C49" s="133"/>
-      <c r="D49" s="114" t="s">
+      <c r="A49" s="109"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="115"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="126"/>
+      <c r="E49" s="114"/>
+      <c r="F49" s="122"/>
+      <c r="G49" s="125"/>
     </row>
     <row r="50" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="110"/>
-      <c r="B50" s="130"/>
-      <c r="C50" s="131"/>
-      <c r="D50" s="114" t="s">
+      <c r="A50" s="109"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="130"/>
+      <c r="D50" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="115"/>
-      <c r="F50" s="124"/>
-      <c r="G50" s="126"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="125"/>
     </row>
     <row r="51" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="110"/>
-      <c r="B51" s="128" t="s">
+      <c r="A51" s="109"/>
+      <c r="B51" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="129"/>
-      <c r="D51" s="114" t="s">
+      <c r="C51" s="128"/>
+      <c r="D51" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="115"/>
-      <c r="F51" s="122">
+      <c r="E51" s="114"/>
+      <c r="F51" s="121">
         <v>2</v>
       </c>
-      <c r="G51" s="126"/>
+      <c r="G51" s="125"/>
     </row>
     <row r="52" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A52" s="110"/>
-      <c r="B52" s="132"/>
-      <c r="C52" s="133"/>
-      <c r="D52" s="114" t="s">
+      <c r="A52" s="109"/>
+      <c r="B52" s="131"/>
+      <c r="C52" s="132"/>
+      <c r="D52" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="E52" s="115"/>
-      <c r="F52" s="123"/>
-      <c r="G52" s="126"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="122"/>
+      <c r="G52" s="125"/>
     </row>
     <row r="53" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A53" s="110"/>
-      <c r="B53" s="132"/>
-      <c r="C53" s="133"/>
-      <c r="D53" s="114" t="s">
+      <c r="A53" s="109"/>
+      <c r="B53" s="131"/>
+      <c r="C53" s="132"/>
+      <c r="D53" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E53" s="115"/>
-      <c r="F53" s="123"/>
-      <c r="G53" s="126"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="122"/>
+      <c r="G53" s="125"/>
     </row>
     <row r="54" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A54" s="110"/>
-      <c r="B54" s="132"/>
-      <c r="C54" s="133"/>
-      <c r="D54" s="114" t="s">
+      <c r="A54" s="109"/>
+      <c r="B54" s="131"/>
+      <c r="C54" s="132"/>
+      <c r="D54" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="E54" s="115"/>
-      <c r="F54" s="123"/>
-      <c r="G54" s="126"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="122"/>
+      <c r="G54" s="125"/>
     </row>
     <row r="55" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A55" s="110"/>
-      <c r="B55" s="130"/>
-      <c r="C55" s="131"/>
-      <c r="D55" s="114" t="s">
+      <c r="A55" s="109"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="130"/>
+      <c r="D55" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="E55" s="115"/>
-      <c r="F55" s="124"/>
-      <c r="G55" s="127"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="123"/>
+      <c r="G55" s="126"/>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A56" s="110"/>
-      <c r="B56" s="128" t="s">
+      <c r="A56" s="109"/>
+      <c r="B56" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="129"/>
-      <c r="D56" s="114" t="s">
+      <c r="C56" s="128"/>
+      <c r="D56" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="115"/>
-      <c r="F56" s="122">
+      <c r="E56" s="114"/>
+      <c r="F56" s="121">
         <v>0</v>
       </c>
-      <c r="G56" s="125" t="s">
+      <c r="G56" s="124" t="s">
         <v>34</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A57" s="110"/>
-      <c r="B57" s="130"/>
-      <c r="C57" s="131"/>
-      <c r="D57" s="114" t="s">
+      <c r="A57" s="109"/>
+      <c r="B57" s="129"/>
+      <c r="C57" s="130"/>
+      <c r="D57" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="115"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="127"/>
+      <c r="E57" s="114"/>
+      <c r="F57" s="123"/>
+      <c r="G57" s="126"/>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A58" s="110"/>
-      <c r="B58" s="128" t="s">
+      <c r="A58" s="109"/>
+      <c r="B58" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="129"/>
-      <c r="D58" s="114" t="s">
+      <c r="C58" s="128"/>
+      <c r="D58" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="115"/>
-      <c r="F58" s="122">
+      <c r="E58" s="114"/>
+      <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="G58" s="125" t="s">
+      <c r="G58" s="124" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A59" s="110"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="131"/>
-      <c r="D59" s="114" t="s">
+      <c r="A59" s="109"/>
+      <c r="B59" s="129"/>
+      <c r="C59" s="130"/>
+      <c r="D59" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="115"/>
-      <c r="F59" s="124"/>
-      <c r="G59" s="126"/>
+      <c r="E59" s="114"/>
+      <c r="F59" s="123"/>
+      <c r="G59" s="125"/>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A60" s="110"/>
-      <c r="B60" s="128" t="s">
+      <c r="A60" s="109"/>
+      <c r="B60" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="129"/>
-      <c r="D60" s="114" t="s">
+      <c r="C60" s="128"/>
+      <c r="D60" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="115"/>
-      <c r="F60" s="122">
+      <c r="E60" s="114"/>
+      <c r="F60" s="121">
         <v>0</v>
       </c>
-      <c r="G60" s="126"/>
+      <c r="G60" s="125"/>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A61" s="110"/>
-      <c r="B61" s="132"/>
-      <c r="C61" s="133"/>
-      <c r="D61" s="114" t="s">
+      <c r="A61" s="109"/>
+      <c r="B61" s="131"/>
+      <c r="C61" s="132"/>
+      <c r="D61" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="115"/>
-      <c r="F61" s="123"/>
-      <c r="G61" s="126"/>
+      <c r="E61" s="114"/>
+      <c r="F61" s="122"/>
+      <c r="G61" s="125"/>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A62" s="110"/>
-      <c r="B62" s="132"/>
-      <c r="C62" s="133"/>
-      <c r="D62" s="114" t="s">
+      <c r="A62" s="109"/>
+      <c r="B62" s="131"/>
+      <c r="C62" s="132"/>
+      <c r="D62" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="115"/>
-      <c r="F62" s="123"/>
-      <c r="G62" s="126"/>
+      <c r="E62" s="114"/>
+      <c r="F62" s="122"/>
+      <c r="G62" s="125"/>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A63" s="110"/>
-      <c r="B63" s="132"/>
-      <c r="C63" s="133"/>
-      <c r="D63" s="114" t="s">
+      <c r="A63" s="109"/>
+      <c r="B63" s="131"/>
+      <c r="C63" s="132"/>
+      <c r="D63" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="115"/>
-      <c r="F63" s="123"/>
-      <c r="G63" s="126"/>
+      <c r="E63" s="114"/>
+      <c r="F63" s="122"/>
+      <c r="G63" s="125"/>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A64" s="110"/>
-      <c r="B64" s="132"/>
-      <c r="C64" s="133"/>
-      <c r="D64" s="114" t="s">
+      <c r="A64" s="109"/>
+      <c r="B64" s="131"/>
+      <c r="C64" s="132"/>
+      <c r="D64" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="115"/>
-      <c r="F64" s="123"/>
-      <c r="G64" s="126"/>
+      <c r="E64" s="114"/>
+      <c r="F64" s="122"/>
+      <c r="G64" s="125"/>
     </row>
     <row r="65" spans="1:7" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A65" s="111"/>
-      <c r="B65" s="130"/>
-      <c r="C65" s="131"/>
-      <c r="D65" s="114" t="s">
+      <c r="A65" s="110"/>
+      <c r="B65" s="129"/>
+      <c r="C65" s="130"/>
+      <c r="D65" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="115"/>
-      <c r="F65" s="124"/>
-      <c r="G65" s="127"/>
+      <c r="E65" s="114"/>
+      <c r="F65" s="123"/>
+      <c r="G65" s="126"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A66" s="134" t="s">
+      <c r="A66" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="135" t="s">
+      <c r="B66" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="135"/>
-      <c r="D66" s="135" t="s">
+      <c r="C66" s="134"/>
+      <c r="D66" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="135"/>
+      <c r="E66" s="134"/>
       <c r="F66" s="17">
         <v>0</v>
       </c>
@@ -8334,15 +8286,15 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A67" s="134"/>
-      <c r="B67" s="136" t="s">
+      <c r="A67" s="133"/>
+      <c r="B67" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="136"/>
-      <c r="D67" s="137" t="s">
+      <c r="C67" s="135"/>
+      <c r="D67" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="E67" s="137"/>
+      <c r="E67" s="136"/>
       <c r="F67" s="26">
         <v>0</v>
       </c>
@@ -8351,104 +8303,104 @@
       </c>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A68" s="134"/>
-      <c r="B68" s="138" t="s">
+      <c r="A68" s="133"/>
+      <c r="B68" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="139"/>
-      <c r="D68" s="144" t="s">
+      <c r="C68" s="138"/>
+      <c r="D68" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="E68" s="145"/>
-      <c r="F68" s="147">
+      <c r="E68" s="144"/>
+      <c r="F68" s="146">
         <v>0</v>
       </c>
-      <c r="G68" s="125" t="s">
+      <c r="G68" s="124" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A69" s="134"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="141"/>
-      <c r="D69" s="144" t="s">
+      <c r="A69" s="133"/>
+      <c r="B69" s="139"/>
+      <c r="C69" s="140"/>
+      <c r="D69" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="E69" s="145"/>
-      <c r="F69" s="148"/>
-      <c r="G69" s="126"/>
+      <c r="E69" s="144"/>
+      <c r="F69" s="147"/>
+      <c r="G69" s="125"/>
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A70" s="134"/>
-      <c r="B70" s="140"/>
-      <c r="C70" s="141"/>
-      <c r="D70" s="144" t="s">
+      <c r="A70" s="133"/>
+      <c r="B70" s="139"/>
+      <c r="C70" s="140"/>
+      <c r="D70" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="E70" s="145"/>
-      <c r="F70" s="148"/>
-      <c r="G70" s="126"/>
+      <c r="E70" s="144"/>
+      <c r="F70" s="147"/>
+      <c r="G70" s="125"/>
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A71" s="134"/>
-      <c r="B71" s="142"/>
-      <c r="C71" s="143"/>
-      <c r="D71" s="144" t="s">
+      <c r="A71" s="133"/>
+      <c r="B71" s="141"/>
+      <c r="C71" s="142"/>
+      <c r="D71" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="E71" s="145"/>
-      <c r="F71" s="149"/>
-      <c r="G71" s="127"/>
+      <c r="E71" s="144"/>
+      <c r="F71" s="148"/>
+      <c r="G71" s="126"/>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A72" s="134"/>
-      <c r="B72" s="146" t="s">
+      <c r="A72" s="133"/>
+      <c r="B72" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="146"/>
-      <c r="D72" s="146" t="s">
+      <c r="C72" s="145"/>
+      <c r="D72" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="146"/>
-      <c r="F72" s="150">
+      <c r="E72" s="145"/>
+      <c r="F72" s="149">
         <v>0</v>
       </c>
-      <c r="G72" s="137" t="s">
+      <c r="G72" s="136" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A73" s="134"/>
-      <c r="B73" s="146"/>
-      <c r="C73" s="146"/>
-      <c r="D73" s="151" t="s">
+      <c r="A73" s="133"/>
+      <c r="B73" s="145"/>
+      <c r="C73" s="145"/>
+      <c r="D73" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="E73" s="151"/>
-      <c r="F73" s="150"/>
-      <c r="G73" s="137"/>
+      <c r="E73" s="150"/>
+      <c r="F73" s="149"/>
+      <c r="G73" s="136"/>
     </row>
     <row r="74" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A74" s="134"/>
-      <c r="B74" s="146"/>
-      <c r="C74" s="146"/>
-      <c r="D74" s="146" t="s">
+      <c r="A74" s="133"/>
+      <c r="B74" s="145"/>
+      <c r="C74" s="145"/>
+      <c r="D74" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="E74" s="146"/>
-      <c r="F74" s="150"/>
-      <c r="G74" s="137"/>
+      <c r="E74" s="145"/>
+      <c r="F74" s="149"/>
+      <c r="G74" s="136"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A75" s="134"/>
-      <c r="B75" s="146"/>
-      <c r="C75" s="146"/>
-      <c r="D75" s="146" t="s">
+      <c r="A75" s="133"/>
+      <c r="B75" s="145"/>
+      <c r="C75" s="145"/>
+      <c r="D75" s="145" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="146"/>
-      <c r="F75" s="150"/>
-      <c r="G75" s="137"/>
+      <c r="E75" s="145"/>
+      <c r="F75" s="149"/>
+      <c r="G75" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="117">
@@ -8609,7 +8561,7 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView zoomScale="168" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -8630,15 +8582,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -8647,15 +8599,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -8668,10 +8620,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>3</v>
@@ -8689,10 +8641,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -8706,19 +8658,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="95">
         <v>6</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -8730,28 +8682,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="93"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="156"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="79"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -8761,14 +8713,14 @@
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="81"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="16" t="s">
         <v>13</v>
       </c>
@@ -8781,17 +8733,17 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="114" t="s">
+      <c r="C9" s="112"/>
+      <c r="D9" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="115"/>
+      <c r="E9" s="114"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
         <v>18</v>
@@ -8801,19 +8753,19 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="116" t="s">
+      <c r="A10" s="109"/>
+      <c r="B10" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="114" t="s">
+      <c r="C10" s="116"/>
+      <c r="D10" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="115"/>
-      <c r="F10" s="122">
+      <c r="E10" s="114"/>
+      <c r="F10" s="121">
         <v>2</v>
       </c>
-      <c r="G10" s="152" t="s">
+      <c r="G10" s="151" t="s">
         <v>21</v>
       </c>
       <c r="K10" s="4"/>
@@ -8822,79 +8774,79 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A11" s="110"/>
-      <c r="B11" s="118"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="114" t="s">
+      <c r="A11" s="109"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="115"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="153"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="152"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="110"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="114" t="s">
+      <c r="A12" s="109"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="153"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="152"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="110"/>
-      <c r="B13" s="118"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="114" t="s">
+      <c r="A13" s="109"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="115"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="153"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="152"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="110"/>
-      <c r="B14" s="120"/>
-      <c r="C14" s="121"/>
-      <c r="D14" s="114" t="s">
+      <c r="A14" s="109"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="115"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="153"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="152"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="110"/>
-      <c r="B15" s="128" t="s">
+      <c r="A15" s="109"/>
+      <c r="B15" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="129"/>
-      <c r="D15" s="114" t="s">
+      <c r="C15" s="128"/>
+      <c r="D15" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="115"/>
-      <c r="F15" s="122">
+      <c r="E15" s="114"/>
+      <c r="F15" s="121">
         <v>2</v>
       </c>
-      <c r="G15" s="153"/>
+      <c r="G15" s="152"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -8904,15 +8856,15 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A16" s="110"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="114" t="s">
+      <c r="A16" s="109"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="115"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="153"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="152"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -8922,15 +8874,15 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="110"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="114" t="s">
+      <c r="A17" s="109"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="115"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="153"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="152"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -8940,15 +8892,15 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A18" s="110"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="114" t="s">
+      <c r="A18" s="109"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="115"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="153"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="152"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -8958,15 +8910,15 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A19" s="110"/>
-      <c r="B19" s="130"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="114" t="s">
+      <c r="A19" s="109"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="115"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="154"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="153"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -8976,19 +8928,19 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A20" s="110"/>
-      <c r="B20" s="128" t="s">
+      <c r="A20" s="109"/>
+      <c r="B20" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="129"/>
-      <c r="D20" s="114" t="s">
+      <c r="C20" s="128"/>
+      <c r="D20" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="115"/>
-      <c r="F20" s="122">
+      <c r="E20" s="114"/>
+      <c r="F20" s="121">
         <v>0</v>
       </c>
-      <c r="G20" s="152" t="s">
+      <c r="G20" s="151" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="4"/>
@@ -8997,34 +8949,34 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A21" s="110"/>
-      <c r="B21" s="130"/>
-      <c r="C21" s="131"/>
-      <c r="D21" s="114" t="s">
+      <c r="A21" s="109"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="115"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="154"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="153"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A22" s="110"/>
-      <c r="B22" s="116" t="s">
+      <c r="A22" s="109"/>
+      <c r="B22" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="117"/>
-      <c r="D22" s="114" t="s">
+      <c r="C22" s="116"/>
+      <c r="D22" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="115"/>
-      <c r="F22" s="122">
+      <c r="E22" s="114"/>
+      <c r="F22" s="121">
         <v>2</v>
       </c>
-      <c r="G22" s="125" t="s">
+      <c r="G22" s="124" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="4"/>
@@ -9033,79 +8985,79 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="110"/>
-      <c r="B23" s="118"/>
-      <c r="C23" s="119"/>
-      <c r="D23" s="114" t="s">
+      <c r="A23" s="109"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="115"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="126"/>
+      <c r="E23" s="114"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="125"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="110"/>
-      <c r="B24" s="118"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="114" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="115"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="126"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="125"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="110"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="114" t="s">
+      <c r="A25" s="109"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="115"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="126"/>
+      <c r="E25" s="114"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="125"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="110"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="114" t="s">
+      <c r="A26" s="109"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="126"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="125"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="110"/>
-      <c r="B27" s="128" t="s">
+      <c r="A27" s="109"/>
+      <c r="B27" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="129"/>
-      <c r="D27" s="114" t="s">
+      <c r="C27" s="128"/>
+      <c r="D27" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="115"/>
-      <c r="F27" s="122">
+      <c r="E27" s="114"/>
+      <c r="F27" s="121">
         <v>2</v>
       </c>
-      <c r="G27" s="126"/>
+      <c r="G27" s="125"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
@@ -9115,15 +9067,15 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="110"/>
-      <c r="B28" s="132"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="114" t="s">
+      <c r="A28" s="109"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="115"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="126"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="125"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -9132,15 +9084,15 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="110"/>
-      <c r="B29" s="132"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="114" t="s">
+      <c r="A29" s="109"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="115"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="126"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="125"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -9149,15 +9101,15 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="110"/>
-      <c r="B30" s="132"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="114" t="s">
+      <c r="A30" s="109"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="115"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="126"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="125"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -9166,15 +9118,15 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="110"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="131"/>
-      <c r="D31" s="114" t="s">
+      <c r="A31" s="109"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="115"/>
-      <c r="F31" s="124"/>
-      <c r="G31" s="126"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="125"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -9183,19 +9135,19 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="110"/>
-      <c r="B32" s="128" t="s">
+      <c r="A32" s="109"/>
+      <c r="B32" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="129"/>
-      <c r="D32" s="114" t="s">
+      <c r="C32" s="128"/>
+      <c r="D32" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="115"/>
-      <c r="F32" s="122">
+      <c r="E32" s="114"/>
+      <c r="F32" s="121">
         <v>2</v>
       </c>
-      <c r="G32" s="126" t="s">
+      <c r="G32" s="125" t="s">
         <v>49</v>
       </c>
       <c r="H32" s="19"/>
@@ -9207,15 +9159,15 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="110"/>
-      <c r="B33" s="132"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="114" t="s">
+      <c r="A33" s="109"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="115"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="126"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="125"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -9225,15 +9177,15 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="110"/>
-      <c r="B34" s="132"/>
-      <c r="C34" s="133"/>
-      <c r="D34" s="114" t="s">
+      <c r="A34" s="109"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="132"/>
+      <c r="D34" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="115"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="126"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="125"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -9243,15 +9195,15 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="110"/>
-      <c r="B35" s="132"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="114" t="s">
+      <c r="A35" s="109"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="132"/>
+      <c r="D35" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="115"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="126"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="125"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -9261,15 +9213,15 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="110"/>
-      <c r="B36" s="130"/>
-      <c r="C36" s="131"/>
-      <c r="D36" s="114" t="s">
+      <c r="A36" s="109"/>
+      <c r="B36" s="129"/>
+      <c r="C36" s="130"/>
+      <c r="D36" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="115"/>
-      <c r="F36" s="124"/>
-      <c r="G36" s="126"/>
+      <c r="E36" s="114"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="125"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -9279,98 +9231,98 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="110"/>
-      <c r="B37" s="128" t="s">
+      <c r="A37" s="109"/>
+      <c r="B37" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="129"/>
-      <c r="D37" s="114" t="s">
+      <c r="C37" s="128"/>
+      <c r="D37" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="115"/>
-      <c r="F37" s="122">
+      <c r="E37" s="114"/>
+      <c r="F37" s="121">
         <v>2</v>
       </c>
-      <c r="G37" s="126"/>
+      <c r="G37" s="125"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="110"/>
-      <c r="B38" s="132"/>
-      <c r="C38" s="133"/>
-      <c r="D38" s="114" t="s">
+      <c r="A38" s="109"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="115"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="126"/>
+      <c r="E38" s="114"/>
+      <c r="F38" s="122"/>
+      <c r="G38" s="125"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="110"/>
-      <c r="B39" s="132"/>
-      <c r="C39" s="133"/>
-      <c r="D39" s="114" t="s">
+      <c r="A39" s="109"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="132"/>
+      <c r="D39" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="115"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="126"/>
+      <c r="E39" s="114"/>
+      <c r="F39" s="122"/>
+      <c r="G39" s="125"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="110"/>
-      <c r="B40" s="132"/>
-      <c r="C40" s="133"/>
-      <c r="D40" s="114" t="s">
+      <c r="A40" s="109"/>
+      <c r="B40" s="131"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="115"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="126"/>
+      <c r="E40" s="114"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="125"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="110"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="114" t="s">
+      <c r="A41" s="109"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130"/>
+      <c r="D41" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="115"/>
-      <c r="F41" s="124"/>
-      <c r="G41" s="127"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="126"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="110"/>
-      <c r="B42" s="128" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="129"/>
-      <c r="D42" s="114" t="s">
+      <c r="C42" s="128"/>
+      <c r="D42" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="115"/>
-      <c r="F42" s="122">
+      <c r="E42" s="114"/>
+      <c r="F42" s="121">
         <v>0</v>
       </c>
-      <c r="G42" s="125" t="s">
+      <c r="G42" s="124" t="s">
         <v>34</v>
       </c>
       <c r="K42" s="21"/>
@@ -9380,34 +9332,34 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="110"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="131"/>
-      <c r="D43" s="114" t="s">
+      <c r="A43" s="109"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="130"/>
+      <c r="D43" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="115"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="127"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="126"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
     </row>
     <row r="44" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="110"/>
-      <c r="B44" s="128" t="s">
+      <c r="A44" s="109"/>
+      <c r="B44" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="129"/>
-      <c r="D44" s="114" t="s">
+      <c r="C44" s="128"/>
+      <c r="D44" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="115"/>
-      <c r="F44" s="122">
+      <c r="E44" s="114"/>
+      <c r="F44" s="121">
         <v>0</v>
       </c>
-      <c r="G44" s="125" t="s">
+      <c r="G44" s="124" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="8"/>
@@ -9419,15 +9371,15 @@
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="110"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="114" t="s">
+      <c r="A45" s="109"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="130"/>
+      <c r="D45" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="115"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="126"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="125"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -9437,111 +9389,111 @@
       <c r="N45" s="21"/>
     </row>
     <row r="46" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="110"/>
-      <c r="B46" s="128" t="s">
+      <c r="A46" s="109"/>
+      <c r="B46" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="129"/>
-      <c r="D46" s="114" t="s">
+      <c r="C46" s="128"/>
+      <c r="D46" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="115"/>
-      <c r="F46" s="122">
+      <c r="E46" s="114"/>
+      <c r="F46" s="121">
         <v>0</v>
       </c>
-      <c r="G46" s="126"/>
+      <c r="G46" s="125"/>
       <c r="K46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="110"/>
-      <c r="B47" s="132"/>
-      <c r="C47" s="133"/>
-      <c r="D47" s="114" t="s">
+      <c r="A47" s="109"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="132"/>
+      <c r="D47" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="115"/>
-      <c r="F47" s="123"/>
-      <c r="G47" s="126"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="122"/>
+      <c r="G47" s="125"/>
       <c r="K47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="110"/>
-      <c r="B48" s="132"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="114" t="s">
+      <c r="A48" s="109"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="132"/>
+      <c r="D48" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="E48" s="115"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="126"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="122"/>
+      <c r="G48" s="125"/>
       <c r="K48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
     </row>
     <row r="49" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="110"/>
-      <c r="B49" s="132"/>
-      <c r="C49" s="133"/>
-      <c r="D49" s="114" t="s">
+      <c r="A49" s="109"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="115"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="126"/>
+      <c r="E49" s="114"/>
+      <c r="F49" s="122"/>
+      <c r="G49" s="125"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
     </row>
     <row r="50" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="110"/>
-      <c r="B50" s="132"/>
-      <c r="C50" s="133"/>
-      <c r="D50" s="114" t="s">
+      <c r="A50" s="109"/>
+      <c r="B50" s="131"/>
+      <c r="C50" s="132"/>
+      <c r="D50" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="115"/>
-      <c r="F50" s="123"/>
-      <c r="G50" s="126"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="122"/>
+      <c r="G50" s="125"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
     </row>
     <row r="51" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="111"/>
-      <c r="B51" s="130"/>
-      <c r="C51" s="131"/>
-      <c r="D51" s="114" t="s">
+      <c r="A51" s="110"/>
+      <c r="B51" s="129"/>
+      <c r="C51" s="130"/>
+      <c r="D51" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="115"/>
-      <c r="F51" s="124"/>
-      <c r="G51" s="127"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="126"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
     </row>
     <row r="52" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A52" s="134" t="s">
+      <c r="A52" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="135" t="s">
+      <c r="B52" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="135"/>
-      <c r="D52" s="135" t="s">
+      <c r="C52" s="134"/>
+      <c r="D52" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="135"/>
+      <c r="E52" s="134"/>
       <c r="F52" s="17">
         <v>0</v>
       </c>
@@ -9553,15 +9505,15 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="1:16" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A53" s="134"/>
-      <c r="B53" s="136" t="s">
+      <c r="A53" s="133"/>
+      <c r="B53" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="137" t="s">
+      <c r="C53" s="135"/>
+      <c r="D53" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="137"/>
+      <c r="E53" s="136"/>
       <c r="F53" s="26">
         <v>0</v>
       </c>
@@ -9573,19 +9525,19 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="134"/>
-      <c r="B54" s="138" t="s">
+      <c r="A54" s="133"/>
+      <c r="B54" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="139"/>
-      <c r="D54" s="144" t="s">
+      <c r="C54" s="138"/>
+      <c r="D54" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="145"/>
-      <c r="F54" s="147">
+      <c r="E54" s="144"/>
+      <c r="F54" s="146">
         <v>0</v>
       </c>
-      <c r="G54" s="125" t="s">
+      <c r="G54" s="124" t="s">
         <v>79</v>
       </c>
       <c r="K54" s="4"/>
@@ -9594,30 +9546,30 @@
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="134"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="141"/>
-      <c r="D55" s="144" t="s">
+      <c r="A55" s="133"/>
+      <c r="B55" s="139"/>
+      <c r="C55" s="140"/>
+      <c r="D55" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="145"/>
-      <c r="F55" s="148"/>
-      <c r="G55" s="126"/>
+      <c r="E55" s="144"/>
+      <c r="F55" s="147"/>
+      <c r="G55" s="125"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="134"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="141"/>
-      <c r="D56" s="144" t="s">
+      <c r="A56" s="133"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="140"/>
+      <c r="D56" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="145"/>
-      <c r="F56" s="148"/>
-      <c r="G56" s="126"/>
+      <c r="E56" s="144"/>
+      <c r="F56" s="147"/>
+      <c r="G56" s="125"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -9625,15 +9577,15 @@
       <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="134"/>
-      <c r="B57" s="142"/>
-      <c r="C57" s="143"/>
-      <c r="D57" s="144" t="s">
+      <c r="A57" s="133"/>
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="145"/>
-      <c r="F57" s="149"/>
-      <c r="G57" s="127"/>
+      <c r="E57" s="144"/>
+      <c r="F57" s="148"/>
+      <c r="G57" s="126"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="3"/>
@@ -9643,19 +9595,19 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="134"/>
-      <c r="B58" s="146" t="s">
+      <c r="A58" s="133"/>
+      <c r="B58" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="146"/>
-      <c r="D58" s="146" t="s">
+      <c r="C58" s="145"/>
+      <c r="D58" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="E58" s="146"/>
-      <c r="F58" s="150">
+      <c r="E58" s="145"/>
+      <c r="F58" s="149">
         <v>0</v>
       </c>
-      <c r="G58" s="137" t="s">
+      <c r="G58" s="136" t="s">
         <v>85</v>
       </c>
       <c r="K58" s="4"/>
@@ -9664,44 +9616,44 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="134"/>
-      <c r="B59" s="146"/>
-      <c r="C59" s="146"/>
-      <c r="D59" s="151" t="s">
+      <c r="A59" s="133"/>
+      <c r="B59" s="145"/>
+      <c r="C59" s="145"/>
+      <c r="D59" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="151"/>
-      <c r="F59" s="150"/>
-      <c r="G59" s="137"/>
+      <c r="E59" s="150"/>
+      <c r="F59" s="149"/>
+      <c r="G59" s="136"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="134"/>
-      <c r="B60" s="146"/>
-      <c r="C60" s="146"/>
-      <c r="D60" s="146" t="s">
+      <c r="A60" s="133"/>
+      <c r="B60" s="145"/>
+      <c r="C60" s="145"/>
+      <c r="D60" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="E60" s="146"/>
-      <c r="F60" s="150"/>
-      <c r="G60" s="137"/>
+      <c r="E60" s="145"/>
+      <c r="F60" s="149"/>
+      <c r="G60" s="136"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
     <row r="61" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="134"/>
-      <c r="B61" s="146"/>
-      <c r="C61" s="146"/>
-      <c r="D61" s="146" t="s">
+      <c r="A61" s="133"/>
+      <c r="B61" s="145"/>
+      <c r="C61" s="145"/>
+      <c r="D61" s="145" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="146"/>
-      <c r="F61" s="150"/>
-      <c r="G61" s="137"/>
+      <c r="E61" s="145"/>
+      <c r="F61" s="149"/>
+      <c r="G61" s="136"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -9868,8 +9820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B73DFC-ECC8-A147-B875-05F34F97B537}">
   <dimension ref="A1:IN4"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AP7" sqref="AP7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9883,262 +9835,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:248" s="48" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="162" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="161" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="163" t="s">
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="162" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-      <c r="AF1" s="163"/>
-      <c r="AG1" s="163"/>
-      <c r="AH1" s="163"/>
-      <c r="AI1" s="163"/>
-      <c r="AJ1" s="163"/>
-      <c r="AK1" s="163"/>
-      <c r="AL1" s="163"/>
-      <c r="AM1" s="163"/>
-      <c r="AN1" s="164" t="s">
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
+      <c r="L1" s="162"/>
+      <c r="M1" s="162"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="162"/>
+      <c r="P1" s="162"/>
+      <c r="Q1" s="162"/>
+      <c r="R1" s="162"/>
+      <c r="S1" s="162"/>
+      <c r="T1" s="162"/>
+      <c r="U1" s="162"/>
+      <c r="V1" s="162"/>
+      <c r="W1" s="162"/>
+      <c r="X1" s="162"/>
+      <c r="Y1" s="162"/>
+      <c r="Z1" s="162"/>
+      <c r="AA1" s="162"/>
+      <c r="AB1" s="162"/>
+      <c r="AC1" s="162"/>
+      <c r="AD1" s="162"/>
+      <c r="AE1" s="162"/>
+      <c r="AF1" s="162"/>
+      <c r="AG1" s="162"/>
+      <c r="AH1" s="162"/>
+      <c r="AI1" s="162"/>
+      <c r="AJ1" s="162"/>
+      <c r="AK1" s="162"/>
+      <c r="AL1" s="162"/>
+      <c r="AM1" s="162"/>
+      <c r="AN1" s="163" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="164"/>
-      <c r="AP1" s="164"/>
-      <c r="AQ1" s="164"/>
-      <c r="AR1" s="164"/>
-      <c r="AS1" s="164"/>
-      <c r="AT1" s="164"/>
-      <c r="AU1" s="164"/>
-      <c r="AV1" s="164"/>
-      <c r="AW1" s="164"/>
-      <c r="AX1" s="164"/>
-      <c r="AY1" s="164"/>
-      <c r="AZ1" s="164"/>
-      <c r="BA1" s="164"/>
-      <c r="BB1" s="164"/>
-      <c r="BC1" s="164"/>
-      <c r="BD1" s="164"/>
-      <c r="BE1" s="164"/>
-      <c r="BF1" s="164"/>
-      <c r="BG1" s="164"/>
-      <c r="BH1" s="164"/>
-      <c r="BI1" s="164"/>
-      <c r="BJ1" s="164"/>
-      <c r="BK1" s="164"/>
-      <c r="BL1" s="164"/>
-      <c r="BM1" s="164"/>
-      <c r="BN1" s="164"/>
-      <c r="BO1" s="164"/>
-      <c r="BP1" s="164"/>
-      <c r="BQ1" s="164"/>
-      <c r="BR1" s="164"/>
-      <c r="BS1" s="164"/>
-      <c r="BT1" s="164"/>
-      <c r="BU1" s="164"/>
-      <c r="BV1" s="164"/>
-      <c r="BW1" s="164"/>
-      <c r="BX1" s="164"/>
-      <c r="BY1" s="164"/>
-      <c r="BZ1" s="164"/>
-      <c r="CA1" s="164"/>
-      <c r="CB1" s="164"/>
-      <c r="CC1" s="164"/>
-      <c r="CD1" s="164"/>
-      <c r="CE1" s="164"/>
-      <c r="CF1" s="164"/>
-      <c r="CG1" s="164"/>
-      <c r="CH1" s="164"/>
-      <c r="CI1" s="164"/>
-      <c r="CJ1" s="164"/>
-      <c r="CK1" s="164"/>
-      <c r="CL1" s="164"/>
-      <c r="CM1" s="164"/>
-      <c r="CN1" s="164"/>
-      <c r="CO1" s="164"/>
-      <c r="CP1" s="164"/>
-      <c r="CQ1" s="164"/>
-      <c r="CR1" s="164"/>
-      <c r="CS1" s="164"/>
-      <c r="CT1" s="164"/>
-      <c r="CU1" s="164"/>
-      <c r="CV1" s="164"/>
-      <c r="CW1" s="164"/>
-      <c r="CX1" s="164"/>
-      <c r="CY1" s="164"/>
-      <c r="CZ1" s="164"/>
-      <c r="DA1" s="164"/>
-      <c r="DB1" s="164"/>
-      <c r="DC1" s="164"/>
-      <c r="DD1" s="164"/>
-      <c r="DE1" s="164"/>
-      <c r="DF1" s="164"/>
-      <c r="DG1" s="164"/>
-      <c r="DH1" s="164"/>
-      <c r="DI1" s="164"/>
-      <c r="DJ1" s="164"/>
-      <c r="DK1" s="164"/>
-      <c r="DL1" s="164"/>
-      <c r="DM1" s="164"/>
-      <c r="DN1" s="164"/>
-      <c r="DO1" s="164"/>
-      <c r="DP1" s="164"/>
-      <c r="DQ1" s="164"/>
-      <c r="DR1" s="164"/>
-      <c r="DS1" s="164"/>
-      <c r="DT1" s="164"/>
-      <c r="DU1" s="164"/>
-      <c r="DV1" s="164"/>
-      <c r="DW1" s="164"/>
-      <c r="DX1" s="164"/>
-      <c r="DY1" s="164"/>
-      <c r="DZ1" s="164"/>
-      <c r="EA1" s="164"/>
-      <c r="EB1" s="164"/>
-      <c r="EC1" s="164"/>
-      <c r="ED1" s="164"/>
-      <c r="EE1" s="164"/>
-      <c r="EF1" s="164"/>
-      <c r="EG1" s="164"/>
-      <c r="EH1" s="164"/>
-      <c r="EI1" s="164"/>
-      <c r="EJ1" s="164"/>
-      <c r="EK1" s="164"/>
-      <c r="EL1" s="164"/>
-      <c r="EM1" s="164"/>
-      <c r="EN1" s="164"/>
-      <c r="EO1" s="164"/>
-      <c r="EP1" s="164"/>
-      <c r="EQ1" s="164"/>
-      <c r="ER1" s="164"/>
-      <c r="ES1" s="164"/>
-      <c r="ET1" s="164"/>
-      <c r="EU1" s="164"/>
-      <c r="EV1" s="164"/>
-      <c r="EW1" s="164"/>
-      <c r="EX1" s="164"/>
-      <c r="EY1" s="164"/>
-      <c r="EZ1" s="164"/>
-      <c r="FA1" s="164"/>
-      <c r="FB1" s="164"/>
-      <c r="FC1" s="164"/>
-      <c r="FD1" s="164"/>
-      <c r="FE1" s="164"/>
-      <c r="FF1" s="164"/>
-      <c r="FG1" s="164"/>
-      <c r="FH1" s="164"/>
-      <c r="FI1" s="164"/>
-      <c r="FJ1" s="164"/>
-      <c r="FK1" s="164"/>
-      <c r="FL1" s="164"/>
-      <c r="FM1" s="164"/>
-      <c r="FN1" s="164"/>
-      <c r="FO1" s="164"/>
-      <c r="FP1" s="164"/>
-      <c r="FQ1" s="164"/>
-      <c r="FR1" s="164"/>
-      <c r="FS1" s="164"/>
-      <c r="FT1" s="164"/>
-      <c r="FU1" s="164"/>
-      <c r="FV1" s="164"/>
-      <c r="FW1" s="164"/>
-      <c r="FX1" s="164"/>
-      <c r="FY1" s="164"/>
-      <c r="FZ1" s="164"/>
-      <c r="GA1" s="164"/>
-      <c r="GB1" s="164"/>
-      <c r="GC1" s="164"/>
-      <c r="GD1" s="164"/>
-      <c r="GE1" s="164"/>
-      <c r="GF1" s="164"/>
-      <c r="GG1" s="164"/>
-      <c r="GH1" s="164"/>
-      <c r="GI1" s="164"/>
-      <c r="GJ1" s="164"/>
-      <c r="GK1" s="164"/>
-      <c r="GL1" s="164"/>
-      <c r="GM1" s="164"/>
-      <c r="GN1" s="164"/>
-      <c r="GO1" s="164"/>
-      <c r="GP1" s="164"/>
-      <c r="GQ1" s="164"/>
-      <c r="GR1" s="164"/>
-      <c r="GS1" s="164"/>
-      <c r="GT1" s="164"/>
-      <c r="GU1" s="164"/>
-      <c r="GV1" s="164"/>
-      <c r="GW1" s="164"/>
-      <c r="GX1" s="164"/>
-      <c r="GY1" s="164"/>
-      <c r="GZ1" s="164"/>
-      <c r="HA1" s="164"/>
-      <c r="HB1" s="164"/>
-      <c r="HC1" s="164"/>
-      <c r="HD1" s="164"/>
-      <c r="HE1" s="164"/>
-      <c r="HF1" s="164"/>
-      <c r="HG1" s="164"/>
-      <c r="HH1" s="164"/>
-      <c r="HI1" s="164"/>
-      <c r="HJ1" s="164"/>
-      <c r="HK1" s="164"/>
-      <c r="HL1" s="164"/>
-      <c r="HM1" s="164"/>
-      <c r="HN1" s="164"/>
-      <c r="HO1" s="164"/>
-      <c r="HP1" s="164"/>
-      <c r="HQ1" s="164"/>
-      <c r="HR1" s="164"/>
-      <c r="HS1" s="164"/>
-      <c r="HT1" s="164"/>
-      <c r="HU1" s="164"/>
-      <c r="HV1" s="164"/>
-      <c r="HW1" s="164"/>
-      <c r="HX1" s="164"/>
-      <c r="HY1" s="164"/>
-      <c r="HZ1" s="164"/>
-      <c r="IA1" s="164"/>
-      <c r="IB1" s="164"/>
-      <c r="IC1" s="164"/>
-      <c r="ID1" s="164"/>
-      <c r="IE1" s="164"/>
-      <c r="IF1" s="164"/>
-      <c r="IG1" s="164"/>
-      <c r="IH1" s="164"/>
-      <c r="II1" s="164"/>
-      <c r="IJ1" s="164"/>
-      <c r="IK1" s="164"/>
-      <c r="IL1" s="164"/>
-      <c r="IM1" s="164"/>
-      <c r="IN1" s="164"/>
+      <c r="AO1" s="163"/>
+      <c r="AP1" s="163"/>
+      <c r="AQ1" s="163"/>
+      <c r="AR1" s="163"/>
+      <c r="AS1" s="163"/>
+      <c r="AT1" s="163"/>
+      <c r="AU1" s="163"/>
+      <c r="AV1" s="163"/>
+      <c r="AW1" s="163"/>
+      <c r="AX1" s="163"/>
+      <c r="AY1" s="163"/>
+      <c r="AZ1" s="163"/>
+      <c r="BA1" s="163"/>
+      <c r="BB1" s="163"/>
+      <c r="BC1" s="163"/>
+      <c r="BD1" s="163"/>
+      <c r="BE1" s="163"/>
+      <c r="BF1" s="163"/>
+      <c r="BG1" s="163"/>
+      <c r="BH1" s="163"/>
+      <c r="BI1" s="163"/>
+      <c r="BJ1" s="163"/>
+      <c r="BK1" s="163"/>
+      <c r="BL1" s="163"/>
+      <c r="BM1" s="163"/>
+      <c r="BN1" s="163"/>
+      <c r="BO1" s="163"/>
+      <c r="BP1" s="163"/>
+      <c r="BQ1" s="163"/>
+      <c r="BR1" s="163"/>
+      <c r="BS1" s="163"/>
+      <c r="BT1" s="163"/>
+      <c r="BU1" s="163"/>
+      <c r="BV1" s="163"/>
+      <c r="BW1" s="163"/>
+      <c r="BX1" s="163"/>
+      <c r="BY1" s="163"/>
+      <c r="BZ1" s="163"/>
+      <c r="CA1" s="163"/>
+      <c r="CB1" s="163"/>
+      <c r="CC1" s="163"/>
+      <c r="CD1" s="163"/>
+      <c r="CE1" s="163"/>
+      <c r="CF1" s="163"/>
+      <c r="CG1" s="163"/>
+      <c r="CH1" s="163"/>
+      <c r="CI1" s="163"/>
+      <c r="CJ1" s="163"/>
+      <c r="CK1" s="163"/>
+      <c r="CL1" s="163"/>
+      <c r="CM1" s="163"/>
+      <c r="CN1" s="163"/>
+      <c r="CO1" s="163"/>
+      <c r="CP1" s="163"/>
+      <c r="CQ1" s="163"/>
+      <c r="CR1" s="163"/>
+      <c r="CS1" s="163"/>
+      <c r="CT1" s="163"/>
+      <c r="CU1" s="163"/>
+      <c r="CV1" s="163"/>
+      <c r="CW1" s="163"/>
+      <c r="CX1" s="163"/>
+      <c r="CY1" s="163"/>
+      <c r="CZ1" s="163"/>
+      <c r="DA1" s="163"/>
+      <c r="DB1" s="163"/>
+      <c r="DC1" s="163"/>
+      <c r="DD1" s="163"/>
+      <c r="DE1" s="163"/>
+      <c r="DF1" s="163"/>
+      <c r="DG1" s="163"/>
+      <c r="DH1" s="163"/>
+      <c r="DI1" s="163"/>
+      <c r="DJ1" s="163"/>
+      <c r="DK1" s="163"/>
+      <c r="DL1" s="163"/>
+      <c r="DM1" s="163"/>
+      <c r="DN1" s="163"/>
+      <c r="DO1" s="163"/>
+      <c r="DP1" s="163"/>
+      <c r="DQ1" s="163"/>
+      <c r="DR1" s="163"/>
+      <c r="DS1" s="163"/>
+      <c r="DT1" s="163"/>
+      <c r="DU1" s="163"/>
+      <c r="DV1" s="163"/>
+      <c r="DW1" s="163"/>
+      <c r="DX1" s="163"/>
+      <c r="DY1" s="163"/>
+      <c r="DZ1" s="163"/>
+      <c r="EA1" s="163"/>
+      <c r="EB1" s="163"/>
+      <c r="EC1" s="163"/>
+      <c r="ED1" s="163"/>
+      <c r="EE1" s="163"/>
+      <c r="EF1" s="163"/>
+      <c r="EG1" s="163"/>
+      <c r="EH1" s="163"/>
+      <c r="EI1" s="163"/>
+      <c r="EJ1" s="163"/>
+      <c r="EK1" s="163"/>
+      <c r="EL1" s="163"/>
+      <c r="EM1" s="163"/>
+      <c r="EN1" s="163"/>
+      <c r="EO1" s="163"/>
+      <c r="EP1" s="163"/>
+      <c r="EQ1" s="163"/>
+      <c r="ER1" s="163"/>
+      <c r="ES1" s="163"/>
+      <c r="ET1" s="163"/>
+      <c r="EU1" s="163"/>
+      <c r="EV1" s="163"/>
+      <c r="EW1" s="163"/>
+      <c r="EX1" s="163"/>
+      <c r="EY1" s="163"/>
+      <c r="EZ1" s="163"/>
+      <c r="FA1" s="163"/>
+      <c r="FB1" s="163"/>
+      <c r="FC1" s="163"/>
+      <c r="FD1" s="163"/>
+      <c r="FE1" s="163"/>
+      <c r="FF1" s="163"/>
+      <c r="FG1" s="163"/>
+      <c r="FH1" s="163"/>
+      <c r="FI1" s="163"/>
+      <c r="FJ1" s="163"/>
+      <c r="FK1" s="163"/>
+      <c r="FL1" s="163"/>
+      <c r="FM1" s="163"/>
+      <c r="FN1" s="163"/>
+      <c r="FO1" s="163"/>
+      <c r="FP1" s="163"/>
+      <c r="FQ1" s="163"/>
+      <c r="FR1" s="163"/>
+      <c r="FS1" s="163"/>
+      <c r="FT1" s="163"/>
+      <c r="FU1" s="163"/>
+      <c r="FV1" s="163"/>
+      <c r="FW1" s="163"/>
+      <c r="FX1" s="163"/>
+      <c r="FY1" s="163"/>
+      <c r="FZ1" s="163"/>
+      <c r="GA1" s="163"/>
+      <c r="GB1" s="163"/>
+      <c r="GC1" s="163"/>
+      <c r="GD1" s="163"/>
+      <c r="GE1" s="163"/>
+      <c r="GF1" s="163"/>
+      <c r="GG1" s="163"/>
+      <c r="GH1" s="163"/>
+      <c r="GI1" s="163"/>
+      <c r="GJ1" s="163"/>
+      <c r="GK1" s="163"/>
+      <c r="GL1" s="163"/>
+      <c r="GM1" s="163"/>
+      <c r="GN1" s="163"/>
+      <c r="GO1" s="163"/>
+      <c r="GP1" s="163"/>
+      <c r="GQ1" s="163"/>
+      <c r="GR1" s="163"/>
+      <c r="GS1" s="163"/>
+      <c r="GT1" s="163"/>
+      <c r="GU1" s="163"/>
+      <c r="GV1" s="163"/>
+      <c r="GW1" s="163"/>
+      <c r="GX1" s="163"/>
+      <c r="GY1" s="163"/>
+      <c r="GZ1" s="163"/>
+      <c r="HA1" s="163"/>
+      <c r="HB1" s="163"/>
+      <c r="HC1" s="163"/>
+      <c r="HD1" s="163"/>
+      <c r="HE1" s="163"/>
+      <c r="HF1" s="163"/>
+      <c r="HG1" s="163"/>
+      <c r="HH1" s="163"/>
+      <c r="HI1" s="163"/>
+      <c r="HJ1" s="163"/>
+      <c r="HK1" s="163"/>
+      <c r="HL1" s="163"/>
+      <c r="HM1" s="163"/>
+      <c r="HN1" s="163"/>
+      <c r="HO1" s="163"/>
+      <c r="HP1" s="163"/>
+      <c r="HQ1" s="163"/>
+      <c r="HR1" s="163"/>
+      <c r="HS1" s="163"/>
+      <c r="HT1" s="163"/>
+      <c r="HU1" s="163"/>
+      <c r="HV1" s="163"/>
+      <c r="HW1" s="163"/>
+      <c r="HX1" s="163"/>
+      <c r="HY1" s="163"/>
+      <c r="HZ1" s="163"/>
+      <c r="IA1" s="163"/>
+      <c r="IB1" s="163"/>
+      <c r="IC1" s="163"/>
+      <c r="ID1" s="163"/>
+      <c r="IE1" s="163"/>
+      <c r="IF1" s="163"/>
+      <c r="IG1" s="163"/>
+      <c r="IH1" s="163"/>
+      <c r="II1" s="163"/>
+      <c r="IJ1" s="163"/>
+      <c r="IK1" s="163"/>
+      <c r="IL1" s="163"/>
+      <c r="IM1" s="163"/>
+      <c r="IN1" s="163"/>
     </row>
     <row r="2" spans="1:248" s="48" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="49"/>
@@ -10149,274 +10101,274 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
-      <c r="I2" s="165" t="s">
+      <c r="I2" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="165"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
-      <c r="S2" s="165"/>
-      <c r="T2" s="165"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="165" t="s">
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="164"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="164"/>
+      <c r="P2" s="164"/>
+      <c r="Q2" s="164"/>
+      <c r="R2" s="164"/>
+      <c r="S2" s="164"/>
+      <c r="T2" s="164"/>
+      <c r="U2" s="164"/>
+      <c r="V2" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="W2" s="165"/>
-      <c r="X2" s="165"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="165"/>
-      <c r="AA2" s="165"/>
-      <c r="AB2" s="165"/>
-      <c r="AC2" s="165" t="s">
+      <c r="W2" s="164"/>
+      <c r="X2" s="164"/>
+      <c r="Y2" s="164"/>
+      <c r="Z2" s="164"/>
+      <c r="AA2" s="164"/>
+      <c r="AB2" s="164"/>
+      <c r="AC2" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="165"/>
-      <c r="AE2" s="165"/>
-      <c r="AF2" s="165"/>
-      <c r="AG2" s="165"/>
-      <c r="AH2" s="165"/>
-      <c r="AI2" s="165" t="s">
+      <c r="AD2" s="164"/>
+      <c r="AE2" s="164"/>
+      <c r="AF2" s="164"/>
+      <c r="AG2" s="164"/>
+      <c r="AH2" s="164"/>
+      <c r="AI2" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="165"/>
-      <c r="AK2" s="165"/>
-      <c r="AL2" s="165"/>
-      <c r="AM2" s="165"/>
+      <c r="AJ2" s="164"/>
+      <c r="AK2" s="164"/>
+      <c r="AL2" s="164"/>
+      <c r="AM2" s="164"/>
       <c r="AN2" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="166" t="s">
+      <c r="AO2" s="165" t="s">
         <v>335</v>
       </c>
-      <c r="AP2" s="166"/>
-      <c r="AQ2" s="166"/>
-      <c r="AR2" s="166"/>
-      <c r="AS2" s="166"/>
-      <c r="AT2" s="166"/>
-      <c r="AU2" s="166"/>
-      <c r="AV2" s="166"/>
-      <c r="AW2" s="166"/>
-      <c r="AX2" s="166"/>
-      <c r="AY2" s="166"/>
-      <c r="AZ2" s="166"/>
-      <c r="BA2" s="166"/>
-      <c r="BB2" s="166"/>
-      <c r="BC2" s="166"/>
-      <c r="BD2" s="166"/>
-      <c r="BE2" s="166"/>
-      <c r="BF2" s="166"/>
-      <c r="BG2" s="166"/>
-      <c r="BH2" s="166"/>
-      <c r="BI2" s="167" t="s">
+      <c r="AP2" s="165"/>
+      <c r="AQ2" s="165"/>
+      <c r="AR2" s="165"/>
+      <c r="AS2" s="165"/>
+      <c r="AT2" s="165"/>
+      <c r="AU2" s="165"/>
+      <c r="AV2" s="165"/>
+      <c r="AW2" s="165"/>
+      <c r="AX2" s="165"/>
+      <c r="AY2" s="165"/>
+      <c r="AZ2" s="165"/>
+      <c r="BA2" s="165"/>
+      <c r="BB2" s="165"/>
+      <c r="BC2" s="165"/>
+      <c r="BD2" s="165"/>
+      <c r="BE2" s="165"/>
+      <c r="BF2" s="165"/>
+      <c r="BG2" s="165"/>
+      <c r="BH2" s="165"/>
+      <c r="BI2" s="166" t="s">
         <v>334</v>
       </c>
-      <c r="BJ2" s="167"/>
-      <c r="BK2" s="167"/>
-      <c r="BL2" s="167"/>
-      <c r="BM2" s="167"/>
-      <c r="BN2" s="167"/>
-      <c r="BO2" s="167"/>
-      <c r="BP2" s="167"/>
-      <c r="BQ2" s="167"/>
-      <c r="BR2" s="167"/>
-      <c r="BS2" s="167"/>
-      <c r="BT2" s="167"/>
-      <c r="BU2" s="167"/>
-      <c r="BV2" s="167"/>
-      <c r="BW2" s="167"/>
-      <c r="BX2" s="167"/>
-      <c r="BY2" s="169" t="s">
+      <c r="BJ2" s="166"/>
+      <c r="BK2" s="166"/>
+      <c r="BL2" s="166"/>
+      <c r="BM2" s="166"/>
+      <c r="BN2" s="166"/>
+      <c r="BO2" s="166"/>
+      <c r="BP2" s="166"/>
+      <c r="BQ2" s="166"/>
+      <c r="BR2" s="166"/>
+      <c r="BS2" s="166"/>
+      <c r="BT2" s="166"/>
+      <c r="BU2" s="166"/>
+      <c r="BV2" s="166"/>
+      <c r="BW2" s="166"/>
+      <c r="BX2" s="166"/>
+      <c r="BY2" s="168" t="s">
         <v>333</v>
       </c>
-      <c r="BZ2" s="169"/>
-      <c r="CA2" s="169"/>
-      <c r="CB2" s="169"/>
-      <c r="CC2" s="169"/>
-      <c r="CD2" s="169"/>
-      <c r="CE2" s="169"/>
-      <c r="CF2" s="169"/>
-      <c r="CG2" s="169"/>
-      <c r="CH2" s="169"/>
-      <c r="CI2" s="169"/>
-      <c r="CJ2" s="170" t="s">
+      <c r="BZ2" s="168"/>
+      <c r="CA2" s="168"/>
+      <c r="CB2" s="168"/>
+      <c r="CC2" s="168"/>
+      <c r="CD2" s="168"/>
+      <c r="CE2" s="168"/>
+      <c r="CF2" s="168"/>
+      <c r="CG2" s="168"/>
+      <c r="CH2" s="168"/>
+      <c r="CI2" s="168"/>
+      <c r="CJ2" s="169" t="s">
         <v>332</v>
       </c>
-      <c r="CK2" s="170"/>
-      <c r="CL2" s="170"/>
-      <c r="CM2" s="170"/>
-      <c r="CN2" s="170"/>
-      <c r="CO2" s="170"/>
-      <c r="CP2" s="170"/>
-      <c r="CQ2" s="170"/>
-      <c r="CR2" s="170"/>
-      <c r="CS2" s="170"/>
-      <c r="CT2" s="170"/>
-      <c r="CU2" s="170"/>
-      <c r="CV2" s="170"/>
-      <c r="CW2" s="170"/>
-      <c r="CX2" s="170"/>
-      <c r="CY2" s="170"/>
-      <c r="CZ2" s="170"/>
-      <c r="DA2" s="170"/>
-      <c r="DB2" s="170"/>
-      <c r="DC2" s="170"/>
-      <c r="DD2" s="170"/>
-      <c r="DE2" s="171" t="s">
+      <c r="CK2" s="169"/>
+      <c r="CL2" s="169"/>
+      <c r="CM2" s="169"/>
+      <c r="CN2" s="169"/>
+      <c r="CO2" s="169"/>
+      <c r="CP2" s="169"/>
+      <c r="CQ2" s="169"/>
+      <c r="CR2" s="169"/>
+      <c r="CS2" s="169"/>
+      <c r="CT2" s="169"/>
+      <c r="CU2" s="169"/>
+      <c r="CV2" s="169"/>
+      <c r="CW2" s="169"/>
+      <c r="CX2" s="169"/>
+      <c r="CY2" s="169"/>
+      <c r="CZ2" s="169"/>
+      <c r="DA2" s="169"/>
+      <c r="DB2" s="169"/>
+      <c r="DC2" s="169"/>
+      <c r="DD2" s="169"/>
+      <c r="DE2" s="170" t="s">
         <v>331</v>
       </c>
-      <c r="DF2" s="171"/>
-      <c r="DG2" s="171"/>
-      <c r="DH2" s="171"/>
-      <c r="DI2" s="171"/>
-      <c r="DJ2" s="158" t="s">
+      <c r="DF2" s="170"/>
+      <c r="DG2" s="170"/>
+      <c r="DH2" s="170"/>
+      <c r="DI2" s="170"/>
+      <c r="DJ2" s="157" t="s">
         <v>330</v>
       </c>
-      <c r="DK2" s="158"/>
-      <c r="DL2" s="158"/>
-      <c r="DM2" s="158"/>
-      <c r="DN2" s="159" t="s">
+      <c r="DK2" s="157"/>
+      <c r="DL2" s="157"/>
+      <c r="DM2" s="157"/>
+      <c r="DN2" s="158" t="s">
         <v>329</v>
       </c>
-      <c r="DO2" s="159"/>
-      <c r="DP2" s="159"/>
-      <c r="DQ2" s="159"/>
-      <c r="DR2" s="159"/>
-      <c r="DS2" s="159"/>
-      <c r="DT2" s="160" t="s">
+      <c r="DO2" s="158"/>
+      <c r="DP2" s="158"/>
+      <c r="DQ2" s="158"/>
+      <c r="DR2" s="158"/>
+      <c r="DS2" s="158"/>
+      <c r="DT2" s="159" t="s">
         <v>328</v>
       </c>
-      <c r="DU2" s="160"/>
-      <c r="DV2" s="160"/>
-      <c r="DW2" s="160"/>
-      <c r="DX2" s="160"/>
-      <c r="DY2" s="160"/>
-      <c r="DZ2" s="160"/>
-      <c r="EA2" s="160"/>
-      <c r="EB2" s="160"/>
-      <c r="EC2" s="160"/>
-      <c r="ED2" s="160"/>
-      <c r="EE2" s="160"/>
-      <c r="EF2" s="160"/>
-      <c r="EG2" s="160"/>
-      <c r="EH2" s="160"/>
-      <c r="EI2" s="160"/>
-      <c r="EJ2" s="160"/>
-      <c r="EK2" s="160"/>
-      <c r="EL2" s="160"/>
-      <c r="EM2" s="160"/>
-      <c r="EN2" s="160"/>
-      <c r="EO2" s="168" t="s">
+      <c r="DU2" s="159"/>
+      <c r="DV2" s="159"/>
+      <c r="DW2" s="159"/>
+      <c r="DX2" s="159"/>
+      <c r="DY2" s="159"/>
+      <c r="DZ2" s="159"/>
+      <c r="EA2" s="159"/>
+      <c r="EB2" s="159"/>
+      <c r="EC2" s="159"/>
+      <c r="ED2" s="159"/>
+      <c r="EE2" s="159"/>
+      <c r="EF2" s="159"/>
+      <c r="EG2" s="159"/>
+      <c r="EH2" s="159"/>
+      <c r="EI2" s="159"/>
+      <c r="EJ2" s="159"/>
+      <c r="EK2" s="159"/>
+      <c r="EL2" s="159"/>
+      <c r="EM2" s="159"/>
+      <c r="EN2" s="159"/>
+      <c r="EO2" s="167" t="s">
         <v>336</v>
       </c>
-      <c r="EP2" s="168"/>
-      <c r="EQ2" s="168"/>
-      <c r="ER2" s="168"/>
-      <c r="ES2" s="168"/>
-      <c r="ET2" s="168"/>
-      <c r="EU2" s="168"/>
-      <c r="EV2" s="168"/>
-      <c r="EW2" s="168"/>
-      <c r="EX2" s="168"/>
-      <c r="EY2" s="168"/>
-      <c r="EZ2" s="168"/>
-      <c r="FA2" s="168"/>
-      <c r="FB2" s="168"/>
-      <c r="FC2" s="168"/>
-      <c r="FD2" s="168"/>
-      <c r="FE2" s="168"/>
-      <c r="FF2" s="168"/>
-      <c r="FG2" s="168"/>
-      <c r="FH2" s="168"/>
-      <c r="FI2" s="168"/>
-      <c r="FJ2" s="168"/>
-      <c r="FK2" s="168"/>
-      <c r="FL2" s="168"/>
-      <c r="FM2" s="168"/>
-      <c r="FN2" s="168"/>
-      <c r="FO2" s="168"/>
-      <c r="FP2" s="168"/>
-      <c r="FQ2" s="168"/>
-      <c r="FR2" s="168"/>
-      <c r="FS2" s="168"/>
-      <c r="FT2" s="168"/>
-      <c r="FU2" s="168"/>
-      <c r="FV2" s="168"/>
-      <c r="FW2" s="168"/>
-      <c r="FX2" s="168"/>
-      <c r="FY2" s="168"/>
-      <c r="FZ2" s="168"/>
-      <c r="GA2" s="168"/>
-      <c r="GB2" s="168"/>
-      <c r="GC2" s="168"/>
-      <c r="GD2" s="168"/>
-      <c r="GE2" s="168"/>
-      <c r="GF2" s="168"/>
-      <c r="GG2" s="168"/>
-      <c r="GH2" s="168"/>
-      <c r="GI2" s="168"/>
-      <c r="GJ2" s="168"/>
-      <c r="GK2" s="168"/>
-      <c r="GL2" s="168"/>
-      <c r="GM2" s="168"/>
-      <c r="GN2" s="168"/>
-      <c r="GO2" s="168"/>
-      <c r="GP2" s="168"/>
-      <c r="GQ2" s="168"/>
-      <c r="GR2" s="168"/>
-      <c r="GS2" s="168"/>
-      <c r="GT2" s="168"/>
-      <c r="GU2" s="168"/>
-      <c r="GV2" s="168"/>
-      <c r="GW2" s="168"/>
-      <c r="GX2" s="168"/>
-      <c r="GY2" s="168"/>
-      <c r="GZ2" s="168"/>
-      <c r="HA2" s="168"/>
-      <c r="HB2" s="168"/>
-      <c r="HC2" s="168"/>
-      <c r="HD2" s="168"/>
-      <c r="HE2" s="168"/>
-      <c r="HF2" s="168"/>
-      <c r="HG2" s="168"/>
-      <c r="HH2" s="168"/>
-      <c r="HI2" s="168"/>
-      <c r="HJ2" s="168"/>
-      <c r="HK2" s="168"/>
-      <c r="HL2" s="168"/>
-      <c r="HM2" s="168"/>
-      <c r="HN2" s="168"/>
-      <c r="HO2" s="168"/>
-      <c r="HP2" s="168"/>
-      <c r="HQ2" s="168"/>
-      <c r="HR2" s="168"/>
-      <c r="HS2" s="168"/>
-      <c r="HT2" s="168"/>
-      <c r="HU2" s="168"/>
-      <c r="HV2" s="168"/>
-      <c r="HW2" s="168"/>
-      <c r="HX2" s="168"/>
-      <c r="HY2" s="168"/>
-      <c r="HZ2" s="168"/>
-      <c r="IA2" s="168"/>
-      <c r="IB2" s="168"/>
-      <c r="IC2" s="168"/>
-      <c r="ID2" s="168"/>
-      <c r="IE2" s="168"/>
-      <c r="IF2" s="168"/>
-      <c r="IG2" s="168"/>
-      <c r="IH2" s="168"/>
-      <c r="II2" s="168"/>
-      <c r="IJ2" s="168"/>
-      <c r="IK2" s="168"/>
-      <c r="IL2" s="168"/>
-      <c r="IM2" s="168"/>
-      <c r="IN2" s="168"/>
+      <c r="EP2" s="167"/>
+      <c r="EQ2" s="167"/>
+      <c r="ER2" s="167"/>
+      <c r="ES2" s="167"/>
+      <c r="ET2" s="167"/>
+      <c r="EU2" s="167"/>
+      <c r="EV2" s="167"/>
+      <c r="EW2" s="167"/>
+      <c r="EX2" s="167"/>
+      <c r="EY2" s="167"/>
+      <c r="EZ2" s="167"/>
+      <c r="FA2" s="167"/>
+      <c r="FB2" s="167"/>
+      <c r="FC2" s="167"/>
+      <c r="FD2" s="167"/>
+      <c r="FE2" s="167"/>
+      <c r="FF2" s="167"/>
+      <c r="FG2" s="167"/>
+      <c r="FH2" s="167"/>
+      <c r="FI2" s="167"/>
+      <c r="FJ2" s="167"/>
+      <c r="FK2" s="167"/>
+      <c r="FL2" s="167"/>
+      <c r="FM2" s="167"/>
+      <c r="FN2" s="167"/>
+      <c r="FO2" s="167"/>
+      <c r="FP2" s="167"/>
+      <c r="FQ2" s="167"/>
+      <c r="FR2" s="167"/>
+      <c r="FS2" s="167"/>
+      <c r="FT2" s="167"/>
+      <c r="FU2" s="167"/>
+      <c r="FV2" s="167"/>
+      <c r="FW2" s="167"/>
+      <c r="FX2" s="167"/>
+      <c r="FY2" s="167"/>
+      <c r="FZ2" s="167"/>
+      <c r="GA2" s="167"/>
+      <c r="GB2" s="167"/>
+      <c r="GC2" s="167"/>
+      <c r="GD2" s="167"/>
+      <c r="GE2" s="167"/>
+      <c r="GF2" s="167"/>
+      <c r="GG2" s="167"/>
+      <c r="GH2" s="167"/>
+      <c r="GI2" s="167"/>
+      <c r="GJ2" s="167"/>
+      <c r="GK2" s="167"/>
+      <c r="GL2" s="167"/>
+      <c r="GM2" s="167"/>
+      <c r="GN2" s="167"/>
+      <c r="GO2" s="167"/>
+      <c r="GP2" s="167"/>
+      <c r="GQ2" s="167"/>
+      <c r="GR2" s="167"/>
+      <c r="GS2" s="167"/>
+      <c r="GT2" s="167"/>
+      <c r="GU2" s="167"/>
+      <c r="GV2" s="167"/>
+      <c r="GW2" s="167"/>
+      <c r="GX2" s="167"/>
+      <c r="GY2" s="167"/>
+      <c r="GZ2" s="167"/>
+      <c r="HA2" s="167"/>
+      <c r="HB2" s="167"/>
+      <c r="HC2" s="167"/>
+      <c r="HD2" s="167"/>
+      <c r="HE2" s="167"/>
+      <c r="HF2" s="167"/>
+      <c r="HG2" s="167"/>
+      <c r="HH2" s="167"/>
+      <c r="HI2" s="167"/>
+      <c r="HJ2" s="167"/>
+      <c r="HK2" s="167"/>
+      <c r="HL2" s="167"/>
+      <c r="HM2" s="167"/>
+      <c r="HN2" s="167"/>
+      <c r="HO2" s="167"/>
+      <c r="HP2" s="167"/>
+      <c r="HQ2" s="167"/>
+      <c r="HR2" s="167"/>
+      <c r="HS2" s="167"/>
+      <c r="HT2" s="167"/>
+      <c r="HU2" s="167"/>
+      <c r="HV2" s="167"/>
+      <c r="HW2" s="167"/>
+      <c r="HX2" s="167"/>
+      <c r="HY2" s="167"/>
+      <c r="HZ2" s="167"/>
+      <c r="IA2" s="167"/>
+      <c r="IB2" s="167"/>
+      <c r="IC2" s="167"/>
+      <c r="ID2" s="167"/>
+      <c r="IE2" s="167"/>
+      <c r="IF2" s="167"/>
+      <c r="IG2" s="167"/>
+      <c r="IH2" s="167"/>
+      <c r="II2" s="167"/>
+      <c r="IJ2" s="167"/>
+      <c r="IK2" s="167"/>
+      <c r="IL2" s="167"/>
+      <c r="IM2" s="167"/>
+      <c r="IN2" s="167"/>
     </row>
     <row r="3" spans="1:248" s="58" customFormat="1" ht="64">
       <c r="A3" s="49" t="s">
@@ -11462,7 +11414,7 @@
   <dimension ref="F9:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11471,12 +11423,12 @@
   </cols>
   <sheetData>
     <row r="9" spans="6:6">
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="76" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="12" spans="6:6">
-      <c r="F12" s="76" t="s">
+      <c r="F12" s="75" t="s">
         <v>347</v>
       </c>
     </row>

</xml_diff>

<commit_message>
shiftRows with row height copied
</commit_message>
<xml_diff>
--- a/src/test/resources/ceping.xlsx
+++ b/src/test/resources/ceping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02AB9C1-0079-FF41-8F8F-714B5C76AD6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D50A436-8DA0-B340-8582-BC59A82246EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
   <sheets>
     <sheet name="有评语-模板" sheetId="5" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="357">
   <si>
     <t>大数据类候选人测评结论表</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1439,6 +1439,10 @@
   </si>
   <si>
     <t>{age}</t>
+  </si>
+  <si>
+    <t>素质项再谢谢</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2361,6 +2365,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2395,12 +2405,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6961,8 +6965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0B56D7-DA51-554E-86D1-0655EAEF35DF}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="125" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AM1048576"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="125" zoomScaleNormal="150" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -7074,7 +7078,7 @@
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="116" customHeight="1">
       <c r="A8" s="78" t="s">
         <v>9</v>
       </c>
@@ -7085,12 +7089,12 @@
       <c r="F8" s="81"/>
       <c r="G8" s="79"/>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:7" s="8" customFormat="1" ht="200" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="78" t="s">
-        <v>11</v>
+        <v>356</v>
       </c>
       <c r="C9" s="79"/>
       <c r="D9" s="80" t="s">
@@ -7321,7 +7325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6F288-1AD6-674A-831C-FFD9B35C5B5E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="125" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="125" zoomScaleNormal="135" zoomScaleSheetLayoutView="125" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -9835,262 +9839,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:248" s="48" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="161" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="163" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="162" t="s">
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="162"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="162"/>
-      <c r="AH1" s="162"/>
-      <c r="AI1" s="162"/>
-      <c r="AJ1" s="162"/>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="163" t="s">
+      <c r="J1" s="164"/>
+      <c r="K1" s="164"/>
+      <c r="L1" s="164"/>
+      <c r="M1" s="164"/>
+      <c r="N1" s="164"/>
+      <c r="O1" s="164"/>
+      <c r="P1" s="164"/>
+      <c r="Q1" s="164"/>
+      <c r="R1" s="164"/>
+      <c r="S1" s="164"/>
+      <c r="T1" s="164"/>
+      <c r="U1" s="164"/>
+      <c r="V1" s="164"/>
+      <c r="W1" s="164"/>
+      <c r="X1" s="164"/>
+      <c r="Y1" s="164"/>
+      <c r="Z1" s="164"/>
+      <c r="AA1" s="164"/>
+      <c r="AB1" s="164"/>
+      <c r="AC1" s="164"/>
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="163"/>
-      <c r="AP1" s="163"/>
-      <c r="AQ1" s="163"/>
-      <c r="AR1" s="163"/>
-      <c r="AS1" s="163"/>
-      <c r="AT1" s="163"/>
-      <c r="AU1" s="163"/>
-      <c r="AV1" s="163"/>
-      <c r="AW1" s="163"/>
-      <c r="AX1" s="163"/>
-      <c r="AY1" s="163"/>
-      <c r="AZ1" s="163"/>
-      <c r="BA1" s="163"/>
-      <c r="BB1" s="163"/>
-      <c r="BC1" s="163"/>
-      <c r="BD1" s="163"/>
-      <c r="BE1" s="163"/>
-      <c r="BF1" s="163"/>
-      <c r="BG1" s="163"/>
-      <c r="BH1" s="163"/>
-      <c r="BI1" s="163"/>
-      <c r="BJ1" s="163"/>
-      <c r="BK1" s="163"/>
-      <c r="BL1" s="163"/>
-      <c r="BM1" s="163"/>
-      <c r="BN1" s="163"/>
-      <c r="BO1" s="163"/>
-      <c r="BP1" s="163"/>
-      <c r="BQ1" s="163"/>
-      <c r="BR1" s="163"/>
-      <c r="BS1" s="163"/>
-      <c r="BT1" s="163"/>
-      <c r="BU1" s="163"/>
-      <c r="BV1" s="163"/>
-      <c r="BW1" s="163"/>
-      <c r="BX1" s="163"/>
-      <c r="BY1" s="163"/>
-      <c r="BZ1" s="163"/>
-      <c r="CA1" s="163"/>
-      <c r="CB1" s="163"/>
-      <c r="CC1" s="163"/>
-      <c r="CD1" s="163"/>
-      <c r="CE1" s="163"/>
-      <c r="CF1" s="163"/>
-      <c r="CG1" s="163"/>
-      <c r="CH1" s="163"/>
-      <c r="CI1" s="163"/>
-      <c r="CJ1" s="163"/>
-      <c r="CK1" s="163"/>
-      <c r="CL1" s="163"/>
-      <c r="CM1" s="163"/>
-      <c r="CN1" s="163"/>
-      <c r="CO1" s="163"/>
-      <c r="CP1" s="163"/>
-      <c r="CQ1" s="163"/>
-      <c r="CR1" s="163"/>
-      <c r="CS1" s="163"/>
-      <c r="CT1" s="163"/>
-      <c r="CU1" s="163"/>
-      <c r="CV1" s="163"/>
-      <c r="CW1" s="163"/>
-      <c r="CX1" s="163"/>
-      <c r="CY1" s="163"/>
-      <c r="CZ1" s="163"/>
-      <c r="DA1" s="163"/>
-      <c r="DB1" s="163"/>
-      <c r="DC1" s="163"/>
-      <c r="DD1" s="163"/>
-      <c r="DE1" s="163"/>
-      <c r="DF1" s="163"/>
-      <c r="DG1" s="163"/>
-      <c r="DH1" s="163"/>
-      <c r="DI1" s="163"/>
-      <c r="DJ1" s="163"/>
-      <c r="DK1" s="163"/>
-      <c r="DL1" s="163"/>
-      <c r="DM1" s="163"/>
-      <c r="DN1" s="163"/>
-      <c r="DO1" s="163"/>
-      <c r="DP1" s="163"/>
-      <c r="DQ1" s="163"/>
-      <c r="DR1" s="163"/>
-      <c r="DS1" s="163"/>
-      <c r="DT1" s="163"/>
-      <c r="DU1" s="163"/>
-      <c r="DV1" s="163"/>
-      <c r="DW1" s="163"/>
-      <c r="DX1" s="163"/>
-      <c r="DY1" s="163"/>
-      <c r="DZ1" s="163"/>
-      <c r="EA1" s="163"/>
-      <c r="EB1" s="163"/>
-      <c r="EC1" s="163"/>
-      <c r="ED1" s="163"/>
-      <c r="EE1" s="163"/>
-      <c r="EF1" s="163"/>
-      <c r="EG1" s="163"/>
-      <c r="EH1" s="163"/>
-      <c r="EI1" s="163"/>
-      <c r="EJ1" s="163"/>
-      <c r="EK1" s="163"/>
-      <c r="EL1" s="163"/>
-      <c r="EM1" s="163"/>
-      <c r="EN1" s="163"/>
-      <c r="EO1" s="163"/>
-      <c r="EP1" s="163"/>
-      <c r="EQ1" s="163"/>
-      <c r="ER1" s="163"/>
-      <c r="ES1" s="163"/>
-      <c r="ET1" s="163"/>
-      <c r="EU1" s="163"/>
-      <c r="EV1" s="163"/>
-      <c r="EW1" s="163"/>
-      <c r="EX1" s="163"/>
-      <c r="EY1" s="163"/>
-      <c r="EZ1" s="163"/>
-      <c r="FA1" s="163"/>
-      <c r="FB1" s="163"/>
-      <c r="FC1" s="163"/>
-      <c r="FD1" s="163"/>
-      <c r="FE1" s="163"/>
-      <c r="FF1" s="163"/>
-      <c r="FG1" s="163"/>
-      <c r="FH1" s="163"/>
-      <c r="FI1" s="163"/>
-      <c r="FJ1" s="163"/>
-      <c r="FK1" s="163"/>
-      <c r="FL1" s="163"/>
-      <c r="FM1" s="163"/>
-      <c r="FN1" s="163"/>
-      <c r="FO1" s="163"/>
-      <c r="FP1" s="163"/>
-      <c r="FQ1" s="163"/>
-      <c r="FR1" s="163"/>
-      <c r="FS1" s="163"/>
-      <c r="FT1" s="163"/>
-      <c r="FU1" s="163"/>
-      <c r="FV1" s="163"/>
-      <c r="FW1" s="163"/>
-      <c r="FX1" s="163"/>
-      <c r="FY1" s="163"/>
-      <c r="FZ1" s="163"/>
-      <c r="GA1" s="163"/>
-      <c r="GB1" s="163"/>
-      <c r="GC1" s="163"/>
-      <c r="GD1" s="163"/>
-      <c r="GE1" s="163"/>
-      <c r="GF1" s="163"/>
-      <c r="GG1" s="163"/>
-      <c r="GH1" s="163"/>
-      <c r="GI1" s="163"/>
-      <c r="GJ1" s="163"/>
-      <c r="GK1" s="163"/>
-      <c r="GL1" s="163"/>
-      <c r="GM1" s="163"/>
-      <c r="GN1" s="163"/>
-      <c r="GO1" s="163"/>
-      <c r="GP1" s="163"/>
-      <c r="GQ1" s="163"/>
-      <c r="GR1" s="163"/>
-      <c r="GS1" s="163"/>
-      <c r="GT1" s="163"/>
-      <c r="GU1" s="163"/>
-      <c r="GV1" s="163"/>
-      <c r="GW1" s="163"/>
-      <c r="GX1" s="163"/>
-      <c r="GY1" s="163"/>
-      <c r="GZ1" s="163"/>
-      <c r="HA1" s="163"/>
-      <c r="HB1" s="163"/>
-      <c r="HC1" s="163"/>
-      <c r="HD1" s="163"/>
-      <c r="HE1" s="163"/>
-      <c r="HF1" s="163"/>
-      <c r="HG1" s="163"/>
-      <c r="HH1" s="163"/>
-      <c r="HI1" s="163"/>
-      <c r="HJ1" s="163"/>
-      <c r="HK1" s="163"/>
-      <c r="HL1" s="163"/>
-      <c r="HM1" s="163"/>
-      <c r="HN1" s="163"/>
-      <c r="HO1" s="163"/>
-      <c r="HP1" s="163"/>
-      <c r="HQ1" s="163"/>
-      <c r="HR1" s="163"/>
-      <c r="HS1" s="163"/>
-      <c r="HT1" s="163"/>
-      <c r="HU1" s="163"/>
-      <c r="HV1" s="163"/>
-      <c r="HW1" s="163"/>
-      <c r="HX1" s="163"/>
-      <c r="HY1" s="163"/>
-      <c r="HZ1" s="163"/>
-      <c r="IA1" s="163"/>
-      <c r="IB1" s="163"/>
-      <c r="IC1" s="163"/>
-      <c r="ID1" s="163"/>
-      <c r="IE1" s="163"/>
-      <c r="IF1" s="163"/>
-      <c r="IG1" s="163"/>
-      <c r="IH1" s="163"/>
-      <c r="II1" s="163"/>
-      <c r="IJ1" s="163"/>
-      <c r="IK1" s="163"/>
-      <c r="IL1" s="163"/>
-      <c r="IM1" s="163"/>
-      <c r="IN1" s="163"/>
+      <c r="AO1" s="165"/>
+      <c r="AP1" s="165"/>
+      <c r="AQ1" s="165"/>
+      <c r="AR1" s="165"/>
+      <c r="AS1" s="165"/>
+      <c r="AT1" s="165"/>
+      <c r="AU1" s="165"/>
+      <c r="AV1" s="165"/>
+      <c r="AW1" s="165"/>
+      <c r="AX1" s="165"/>
+      <c r="AY1" s="165"/>
+      <c r="AZ1" s="165"/>
+      <c r="BA1" s="165"/>
+      <c r="BB1" s="165"/>
+      <c r="BC1" s="165"/>
+      <c r="BD1" s="165"/>
+      <c r="BE1" s="165"/>
+      <c r="BF1" s="165"/>
+      <c r="BG1" s="165"/>
+      <c r="BH1" s="165"/>
+      <c r="BI1" s="165"/>
+      <c r="BJ1" s="165"/>
+      <c r="BK1" s="165"/>
+      <c r="BL1" s="165"/>
+      <c r="BM1" s="165"/>
+      <c r="BN1" s="165"/>
+      <c r="BO1" s="165"/>
+      <c r="BP1" s="165"/>
+      <c r="BQ1" s="165"/>
+      <c r="BR1" s="165"/>
+      <c r="BS1" s="165"/>
+      <c r="BT1" s="165"/>
+      <c r="BU1" s="165"/>
+      <c r="BV1" s="165"/>
+      <c r="BW1" s="165"/>
+      <c r="BX1" s="165"/>
+      <c r="BY1" s="165"/>
+      <c r="BZ1" s="165"/>
+      <c r="CA1" s="165"/>
+      <c r="CB1" s="165"/>
+      <c r="CC1" s="165"/>
+      <c r="CD1" s="165"/>
+      <c r="CE1" s="165"/>
+      <c r="CF1" s="165"/>
+      <c r="CG1" s="165"/>
+      <c r="CH1" s="165"/>
+      <c r="CI1" s="165"/>
+      <c r="CJ1" s="165"/>
+      <c r="CK1" s="165"/>
+      <c r="CL1" s="165"/>
+      <c r="CM1" s="165"/>
+      <c r="CN1" s="165"/>
+      <c r="CO1" s="165"/>
+      <c r="CP1" s="165"/>
+      <c r="CQ1" s="165"/>
+      <c r="CR1" s="165"/>
+      <c r="CS1" s="165"/>
+      <c r="CT1" s="165"/>
+      <c r="CU1" s="165"/>
+      <c r="CV1" s="165"/>
+      <c r="CW1" s="165"/>
+      <c r="CX1" s="165"/>
+      <c r="CY1" s="165"/>
+      <c r="CZ1" s="165"/>
+      <c r="DA1" s="165"/>
+      <c r="DB1" s="165"/>
+      <c r="DC1" s="165"/>
+      <c r="DD1" s="165"/>
+      <c r="DE1" s="165"/>
+      <c r="DF1" s="165"/>
+      <c r="DG1" s="165"/>
+      <c r="DH1" s="165"/>
+      <c r="DI1" s="165"/>
+      <c r="DJ1" s="165"/>
+      <c r="DK1" s="165"/>
+      <c r="DL1" s="165"/>
+      <c r="DM1" s="165"/>
+      <c r="DN1" s="165"/>
+      <c r="DO1" s="165"/>
+      <c r="DP1" s="165"/>
+      <c r="DQ1" s="165"/>
+      <c r="DR1" s="165"/>
+      <c r="DS1" s="165"/>
+      <c r="DT1" s="165"/>
+      <c r="DU1" s="165"/>
+      <c r="DV1" s="165"/>
+      <c r="DW1" s="165"/>
+      <c r="DX1" s="165"/>
+      <c r="DY1" s="165"/>
+      <c r="DZ1" s="165"/>
+      <c r="EA1" s="165"/>
+      <c r="EB1" s="165"/>
+      <c r="EC1" s="165"/>
+      <c r="ED1" s="165"/>
+      <c r="EE1" s="165"/>
+      <c r="EF1" s="165"/>
+      <c r="EG1" s="165"/>
+      <c r="EH1" s="165"/>
+      <c r="EI1" s="165"/>
+      <c r="EJ1" s="165"/>
+      <c r="EK1" s="165"/>
+      <c r="EL1" s="165"/>
+      <c r="EM1" s="165"/>
+      <c r="EN1" s="165"/>
+      <c r="EO1" s="165"/>
+      <c r="EP1" s="165"/>
+      <c r="EQ1" s="165"/>
+      <c r="ER1" s="165"/>
+      <c r="ES1" s="165"/>
+      <c r="ET1" s="165"/>
+      <c r="EU1" s="165"/>
+      <c r="EV1" s="165"/>
+      <c r="EW1" s="165"/>
+      <c r="EX1" s="165"/>
+      <c r="EY1" s="165"/>
+      <c r="EZ1" s="165"/>
+      <c r="FA1" s="165"/>
+      <c r="FB1" s="165"/>
+      <c r="FC1" s="165"/>
+      <c r="FD1" s="165"/>
+      <c r="FE1" s="165"/>
+      <c r="FF1" s="165"/>
+      <c r="FG1" s="165"/>
+      <c r="FH1" s="165"/>
+      <c r="FI1" s="165"/>
+      <c r="FJ1" s="165"/>
+      <c r="FK1" s="165"/>
+      <c r="FL1" s="165"/>
+      <c r="FM1" s="165"/>
+      <c r="FN1" s="165"/>
+      <c r="FO1" s="165"/>
+      <c r="FP1" s="165"/>
+      <c r="FQ1" s="165"/>
+      <c r="FR1" s="165"/>
+      <c r="FS1" s="165"/>
+      <c r="FT1" s="165"/>
+      <c r="FU1" s="165"/>
+      <c r="FV1" s="165"/>
+      <c r="FW1" s="165"/>
+      <c r="FX1" s="165"/>
+      <c r="FY1" s="165"/>
+      <c r="FZ1" s="165"/>
+      <c r="GA1" s="165"/>
+      <c r="GB1" s="165"/>
+      <c r="GC1" s="165"/>
+      <c r="GD1" s="165"/>
+      <c r="GE1" s="165"/>
+      <c r="GF1" s="165"/>
+      <c r="GG1" s="165"/>
+      <c r="GH1" s="165"/>
+      <c r="GI1" s="165"/>
+      <c r="GJ1" s="165"/>
+      <c r="GK1" s="165"/>
+      <c r="GL1" s="165"/>
+      <c r="GM1" s="165"/>
+      <c r="GN1" s="165"/>
+      <c r="GO1" s="165"/>
+      <c r="GP1" s="165"/>
+      <c r="GQ1" s="165"/>
+      <c r="GR1" s="165"/>
+      <c r="GS1" s="165"/>
+      <c r="GT1" s="165"/>
+      <c r="GU1" s="165"/>
+      <c r="GV1" s="165"/>
+      <c r="GW1" s="165"/>
+      <c r="GX1" s="165"/>
+      <c r="GY1" s="165"/>
+      <c r="GZ1" s="165"/>
+      <c r="HA1" s="165"/>
+      <c r="HB1" s="165"/>
+      <c r="HC1" s="165"/>
+      <c r="HD1" s="165"/>
+      <c r="HE1" s="165"/>
+      <c r="HF1" s="165"/>
+      <c r="HG1" s="165"/>
+      <c r="HH1" s="165"/>
+      <c r="HI1" s="165"/>
+      <c r="HJ1" s="165"/>
+      <c r="HK1" s="165"/>
+      <c r="HL1" s="165"/>
+      <c r="HM1" s="165"/>
+      <c r="HN1" s="165"/>
+      <c r="HO1" s="165"/>
+      <c r="HP1" s="165"/>
+      <c r="HQ1" s="165"/>
+      <c r="HR1" s="165"/>
+      <c r="HS1" s="165"/>
+      <c r="HT1" s="165"/>
+      <c r="HU1" s="165"/>
+      <c r="HV1" s="165"/>
+      <c r="HW1" s="165"/>
+      <c r="HX1" s="165"/>
+      <c r="HY1" s="165"/>
+      <c r="HZ1" s="165"/>
+      <c r="IA1" s="165"/>
+      <c r="IB1" s="165"/>
+      <c r="IC1" s="165"/>
+      <c r="ID1" s="165"/>
+      <c r="IE1" s="165"/>
+      <c r="IF1" s="165"/>
+      <c r="IG1" s="165"/>
+      <c r="IH1" s="165"/>
+      <c r="II1" s="165"/>
+      <c r="IJ1" s="165"/>
+      <c r="IK1" s="165"/>
+      <c r="IL1" s="165"/>
+      <c r="IM1" s="165"/>
+      <c r="IN1" s="165"/>
     </row>
     <row r="2" spans="1:248" s="48" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="49"/>
@@ -10101,274 +10105,274 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
-      <c r="I2" s="164" t="s">
+      <c r="I2" s="166" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
-      <c r="L2" s="164"/>
-      <c r="M2" s="164"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="164"/>
-      <c r="Q2" s="164"/>
-      <c r="R2" s="164"/>
-      <c r="S2" s="164"/>
-      <c r="T2" s="164"/>
-      <c r="U2" s="164"/>
-      <c r="V2" s="164" t="s">
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="166"/>
+      <c r="R2" s="166"/>
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="166"/>
+      <c r="V2" s="166" t="s">
         <v>100</v>
       </c>
-      <c r="W2" s="164"/>
-      <c r="X2" s="164"/>
-      <c r="Y2" s="164"/>
-      <c r="Z2" s="164"/>
-      <c r="AA2" s="164"/>
-      <c r="AB2" s="164"/>
-      <c r="AC2" s="164" t="s">
+      <c r="W2" s="166"/>
+      <c r="X2" s="166"/>
+      <c r="Y2" s="166"/>
+      <c r="Z2" s="166"/>
+      <c r="AA2" s="166"/>
+      <c r="AB2" s="166"/>
+      <c r="AC2" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="164"/>
-      <c r="AE2" s="164"/>
-      <c r="AF2" s="164"/>
-      <c r="AG2" s="164"/>
-      <c r="AH2" s="164"/>
-      <c r="AI2" s="164" t="s">
+      <c r="AD2" s="166"/>
+      <c r="AE2" s="166"/>
+      <c r="AF2" s="166"/>
+      <c r="AG2" s="166"/>
+      <c r="AH2" s="166"/>
+      <c r="AI2" s="166" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="164"/>
-      <c r="AK2" s="164"/>
-      <c r="AL2" s="164"/>
-      <c r="AM2" s="164"/>
+      <c r="AJ2" s="166"/>
+      <c r="AK2" s="166"/>
+      <c r="AL2" s="166"/>
+      <c r="AM2" s="166"/>
       <c r="AN2" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="165" t="s">
+      <c r="AO2" s="167" t="s">
         <v>335</v>
       </c>
-      <c r="AP2" s="165"/>
-      <c r="AQ2" s="165"/>
-      <c r="AR2" s="165"/>
-      <c r="AS2" s="165"/>
-      <c r="AT2" s="165"/>
-      <c r="AU2" s="165"/>
-      <c r="AV2" s="165"/>
-      <c r="AW2" s="165"/>
-      <c r="AX2" s="165"/>
-      <c r="AY2" s="165"/>
-      <c r="AZ2" s="165"/>
-      <c r="BA2" s="165"/>
-      <c r="BB2" s="165"/>
-      <c r="BC2" s="165"/>
-      <c r="BD2" s="165"/>
-      <c r="BE2" s="165"/>
-      <c r="BF2" s="165"/>
-      <c r="BG2" s="165"/>
-      <c r="BH2" s="165"/>
-      <c r="BI2" s="166" t="s">
+      <c r="AP2" s="167"/>
+      <c r="AQ2" s="167"/>
+      <c r="AR2" s="167"/>
+      <c r="AS2" s="167"/>
+      <c r="AT2" s="167"/>
+      <c r="AU2" s="167"/>
+      <c r="AV2" s="167"/>
+      <c r="AW2" s="167"/>
+      <c r="AX2" s="167"/>
+      <c r="AY2" s="167"/>
+      <c r="AZ2" s="167"/>
+      <c r="BA2" s="167"/>
+      <c r="BB2" s="167"/>
+      <c r="BC2" s="167"/>
+      <c r="BD2" s="167"/>
+      <c r="BE2" s="167"/>
+      <c r="BF2" s="167"/>
+      <c r="BG2" s="167"/>
+      <c r="BH2" s="167"/>
+      <c r="BI2" s="168" t="s">
         <v>334</v>
       </c>
-      <c r="BJ2" s="166"/>
-      <c r="BK2" s="166"/>
-      <c r="BL2" s="166"/>
-      <c r="BM2" s="166"/>
-      <c r="BN2" s="166"/>
-      <c r="BO2" s="166"/>
-      <c r="BP2" s="166"/>
-      <c r="BQ2" s="166"/>
-      <c r="BR2" s="166"/>
-      <c r="BS2" s="166"/>
-      <c r="BT2" s="166"/>
-      <c r="BU2" s="166"/>
-      <c r="BV2" s="166"/>
-      <c r="BW2" s="166"/>
-      <c r="BX2" s="166"/>
-      <c r="BY2" s="168" t="s">
+      <c r="BJ2" s="168"/>
+      <c r="BK2" s="168"/>
+      <c r="BL2" s="168"/>
+      <c r="BM2" s="168"/>
+      <c r="BN2" s="168"/>
+      <c r="BO2" s="168"/>
+      <c r="BP2" s="168"/>
+      <c r="BQ2" s="168"/>
+      <c r="BR2" s="168"/>
+      <c r="BS2" s="168"/>
+      <c r="BT2" s="168"/>
+      <c r="BU2" s="168"/>
+      <c r="BV2" s="168"/>
+      <c r="BW2" s="168"/>
+      <c r="BX2" s="168"/>
+      <c r="BY2" s="170" t="s">
         <v>333</v>
       </c>
-      <c r="BZ2" s="168"/>
-      <c r="CA2" s="168"/>
-      <c r="CB2" s="168"/>
-      <c r="CC2" s="168"/>
-      <c r="CD2" s="168"/>
-      <c r="CE2" s="168"/>
-      <c r="CF2" s="168"/>
-      <c r="CG2" s="168"/>
-      <c r="CH2" s="168"/>
-      <c r="CI2" s="168"/>
-      <c r="CJ2" s="169" t="s">
+      <c r="BZ2" s="170"/>
+      <c r="CA2" s="170"/>
+      <c r="CB2" s="170"/>
+      <c r="CC2" s="170"/>
+      <c r="CD2" s="170"/>
+      <c r="CE2" s="170"/>
+      <c r="CF2" s="170"/>
+      <c r="CG2" s="170"/>
+      <c r="CH2" s="170"/>
+      <c r="CI2" s="170"/>
+      <c r="CJ2" s="157" t="s">
         <v>332</v>
       </c>
-      <c r="CK2" s="169"/>
-      <c r="CL2" s="169"/>
-      <c r="CM2" s="169"/>
-      <c r="CN2" s="169"/>
-      <c r="CO2" s="169"/>
-      <c r="CP2" s="169"/>
-      <c r="CQ2" s="169"/>
-      <c r="CR2" s="169"/>
-      <c r="CS2" s="169"/>
-      <c r="CT2" s="169"/>
-      <c r="CU2" s="169"/>
-      <c r="CV2" s="169"/>
-      <c r="CW2" s="169"/>
-      <c r="CX2" s="169"/>
-      <c r="CY2" s="169"/>
-      <c r="CZ2" s="169"/>
-      <c r="DA2" s="169"/>
-      <c r="DB2" s="169"/>
-      <c r="DC2" s="169"/>
-      <c r="DD2" s="169"/>
-      <c r="DE2" s="170" t="s">
+      <c r="CK2" s="157"/>
+      <c r="CL2" s="157"/>
+      <c r="CM2" s="157"/>
+      <c r="CN2" s="157"/>
+      <c r="CO2" s="157"/>
+      <c r="CP2" s="157"/>
+      <c r="CQ2" s="157"/>
+      <c r="CR2" s="157"/>
+      <c r="CS2" s="157"/>
+      <c r="CT2" s="157"/>
+      <c r="CU2" s="157"/>
+      <c r="CV2" s="157"/>
+      <c r="CW2" s="157"/>
+      <c r="CX2" s="157"/>
+      <c r="CY2" s="157"/>
+      <c r="CZ2" s="157"/>
+      <c r="DA2" s="157"/>
+      <c r="DB2" s="157"/>
+      <c r="DC2" s="157"/>
+      <c r="DD2" s="157"/>
+      <c r="DE2" s="158" t="s">
         <v>331</v>
       </c>
-      <c r="DF2" s="170"/>
-      <c r="DG2" s="170"/>
-      <c r="DH2" s="170"/>
-      <c r="DI2" s="170"/>
-      <c r="DJ2" s="157" t="s">
+      <c r="DF2" s="158"/>
+      <c r="DG2" s="158"/>
+      <c r="DH2" s="158"/>
+      <c r="DI2" s="158"/>
+      <c r="DJ2" s="159" t="s">
         <v>330</v>
       </c>
-      <c r="DK2" s="157"/>
-      <c r="DL2" s="157"/>
-      <c r="DM2" s="157"/>
-      <c r="DN2" s="158" t="s">
+      <c r="DK2" s="159"/>
+      <c r="DL2" s="159"/>
+      <c r="DM2" s="159"/>
+      <c r="DN2" s="160" t="s">
         <v>329</v>
       </c>
-      <c r="DO2" s="158"/>
-      <c r="DP2" s="158"/>
-      <c r="DQ2" s="158"/>
-      <c r="DR2" s="158"/>
-      <c r="DS2" s="158"/>
-      <c r="DT2" s="159" t="s">
+      <c r="DO2" s="160"/>
+      <c r="DP2" s="160"/>
+      <c r="DQ2" s="160"/>
+      <c r="DR2" s="160"/>
+      <c r="DS2" s="160"/>
+      <c r="DT2" s="161" t="s">
         <v>328</v>
       </c>
-      <c r="DU2" s="159"/>
-      <c r="DV2" s="159"/>
-      <c r="DW2" s="159"/>
-      <c r="DX2" s="159"/>
-      <c r="DY2" s="159"/>
-      <c r="DZ2" s="159"/>
-      <c r="EA2" s="159"/>
-      <c r="EB2" s="159"/>
-      <c r="EC2" s="159"/>
-      <c r="ED2" s="159"/>
-      <c r="EE2" s="159"/>
-      <c r="EF2" s="159"/>
-      <c r="EG2" s="159"/>
-      <c r="EH2" s="159"/>
-      <c r="EI2" s="159"/>
-      <c r="EJ2" s="159"/>
-      <c r="EK2" s="159"/>
-      <c r="EL2" s="159"/>
-      <c r="EM2" s="159"/>
-      <c r="EN2" s="159"/>
-      <c r="EO2" s="167" t="s">
+      <c r="DU2" s="161"/>
+      <c r="DV2" s="161"/>
+      <c r="DW2" s="161"/>
+      <c r="DX2" s="161"/>
+      <c r="DY2" s="161"/>
+      <c r="DZ2" s="161"/>
+      <c r="EA2" s="161"/>
+      <c r="EB2" s="161"/>
+      <c r="EC2" s="161"/>
+      <c r="ED2" s="161"/>
+      <c r="EE2" s="161"/>
+      <c r="EF2" s="161"/>
+      <c r="EG2" s="161"/>
+      <c r="EH2" s="161"/>
+      <c r="EI2" s="161"/>
+      <c r="EJ2" s="161"/>
+      <c r="EK2" s="161"/>
+      <c r="EL2" s="161"/>
+      <c r="EM2" s="161"/>
+      <c r="EN2" s="161"/>
+      <c r="EO2" s="169" t="s">
         <v>336</v>
       </c>
-      <c r="EP2" s="167"/>
-      <c r="EQ2" s="167"/>
-      <c r="ER2" s="167"/>
-      <c r="ES2" s="167"/>
-      <c r="ET2" s="167"/>
-      <c r="EU2" s="167"/>
-      <c r="EV2" s="167"/>
-      <c r="EW2" s="167"/>
-      <c r="EX2" s="167"/>
-      <c r="EY2" s="167"/>
-      <c r="EZ2" s="167"/>
-      <c r="FA2" s="167"/>
-      <c r="FB2" s="167"/>
-      <c r="FC2" s="167"/>
-      <c r="FD2" s="167"/>
-      <c r="FE2" s="167"/>
-      <c r="FF2" s="167"/>
-      <c r="FG2" s="167"/>
-      <c r="FH2" s="167"/>
-      <c r="FI2" s="167"/>
-      <c r="FJ2" s="167"/>
-      <c r="FK2" s="167"/>
-      <c r="FL2" s="167"/>
-      <c r="FM2" s="167"/>
-      <c r="FN2" s="167"/>
-      <c r="FO2" s="167"/>
-      <c r="FP2" s="167"/>
-      <c r="FQ2" s="167"/>
-      <c r="FR2" s="167"/>
-      <c r="FS2" s="167"/>
-      <c r="FT2" s="167"/>
-      <c r="FU2" s="167"/>
-      <c r="FV2" s="167"/>
-      <c r="FW2" s="167"/>
-      <c r="FX2" s="167"/>
-      <c r="FY2" s="167"/>
-      <c r="FZ2" s="167"/>
-      <c r="GA2" s="167"/>
-      <c r="GB2" s="167"/>
-      <c r="GC2" s="167"/>
-      <c r="GD2" s="167"/>
-      <c r="GE2" s="167"/>
-      <c r="GF2" s="167"/>
-      <c r="GG2" s="167"/>
-      <c r="GH2" s="167"/>
-      <c r="GI2" s="167"/>
-      <c r="GJ2" s="167"/>
-      <c r="GK2" s="167"/>
-      <c r="GL2" s="167"/>
-      <c r="GM2" s="167"/>
-      <c r="GN2" s="167"/>
-      <c r="GO2" s="167"/>
-      <c r="GP2" s="167"/>
-      <c r="GQ2" s="167"/>
-      <c r="GR2" s="167"/>
-      <c r="GS2" s="167"/>
-      <c r="GT2" s="167"/>
-      <c r="GU2" s="167"/>
-      <c r="GV2" s="167"/>
-      <c r="GW2" s="167"/>
-      <c r="GX2" s="167"/>
-      <c r="GY2" s="167"/>
-      <c r="GZ2" s="167"/>
-      <c r="HA2" s="167"/>
-      <c r="HB2" s="167"/>
-      <c r="HC2" s="167"/>
-      <c r="HD2" s="167"/>
-      <c r="HE2" s="167"/>
-      <c r="HF2" s="167"/>
-      <c r="HG2" s="167"/>
-      <c r="HH2" s="167"/>
-      <c r="HI2" s="167"/>
-      <c r="HJ2" s="167"/>
-      <c r="HK2" s="167"/>
-      <c r="HL2" s="167"/>
-      <c r="HM2" s="167"/>
-      <c r="HN2" s="167"/>
-      <c r="HO2" s="167"/>
-      <c r="HP2" s="167"/>
-      <c r="HQ2" s="167"/>
-      <c r="HR2" s="167"/>
-      <c r="HS2" s="167"/>
-      <c r="HT2" s="167"/>
-      <c r="HU2" s="167"/>
-      <c r="HV2" s="167"/>
-      <c r="HW2" s="167"/>
-      <c r="HX2" s="167"/>
-      <c r="HY2" s="167"/>
-      <c r="HZ2" s="167"/>
-      <c r="IA2" s="167"/>
-      <c r="IB2" s="167"/>
-      <c r="IC2" s="167"/>
-      <c r="ID2" s="167"/>
-      <c r="IE2" s="167"/>
-      <c r="IF2" s="167"/>
-      <c r="IG2" s="167"/>
-      <c r="IH2" s="167"/>
-      <c r="II2" s="167"/>
-      <c r="IJ2" s="167"/>
-      <c r="IK2" s="167"/>
-      <c r="IL2" s="167"/>
-      <c r="IM2" s="167"/>
-      <c r="IN2" s="167"/>
+      <c r="EP2" s="169"/>
+      <c r="EQ2" s="169"/>
+      <c r="ER2" s="169"/>
+      <c r="ES2" s="169"/>
+      <c r="ET2" s="169"/>
+      <c r="EU2" s="169"/>
+      <c r="EV2" s="169"/>
+      <c r="EW2" s="169"/>
+      <c r="EX2" s="169"/>
+      <c r="EY2" s="169"/>
+      <c r="EZ2" s="169"/>
+      <c r="FA2" s="169"/>
+      <c r="FB2" s="169"/>
+      <c r="FC2" s="169"/>
+      <c r="FD2" s="169"/>
+      <c r="FE2" s="169"/>
+      <c r="FF2" s="169"/>
+      <c r="FG2" s="169"/>
+      <c r="FH2" s="169"/>
+      <c r="FI2" s="169"/>
+      <c r="FJ2" s="169"/>
+      <c r="FK2" s="169"/>
+      <c r="FL2" s="169"/>
+      <c r="FM2" s="169"/>
+      <c r="FN2" s="169"/>
+      <c r="FO2" s="169"/>
+      <c r="FP2" s="169"/>
+      <c r="FQ2" s="169"/>
+      <c r="FR2" s="169"/>
+      <c r="FS2" s="169"/>
+      <c r="FT2" s="169"/>
+      <c r="FU2" s="169"/>
+      <c r="FV2" s="169"/>
+      <c r="FW2" s="169"/>
+      <c r="FX2" s="169"/>
+      <c r="FY2" s="169"/>
+      <c r="FZ2" s="169"/>
+      <c r="GA2" s="169"/>
+      <c r="GB2" s="169"/>
+      <c r="GC2" s="169"/>
+      <c r="GD2" s="169"/>
+      <c r="GE2" s="169"/>
+      <c r="GF2" s="169"/>
+      <c r="GG2" s="169"/>
+      <c r="GH2" s="169"/>
+      <c r="GI2" s="169"/>
+      <c r="GJ2" s="169"/>
+      <c r="GK2" s="169"/>
+      <c r="GL2" s="169"/>
+      <c r="GM2" s="169"/>
+      <c r="GN2" s="169"/>
+      <c r="GO2" s="169"/>
+      <c r="GP2" s="169"/>
+      <c r="GQ2" s="169"/>
+      <c r="GR2" s="169"/>
+      <c r="GS2" s="169"/>
+      <c r="GT2" s="169"/>
+      <c r="GU2" s="169"/>
+      <c r="GV2" s="169"/>
+      <c r="GW2" s="169"/>
+      <c r="GX2" s="169"/>
+      <c r="GY2" s="169"/>
+      <c r="GZ2" s="169"/>
+      <c r="HA2" s="169"/>
+      <c r="HB2" s="169"/>
+      <c r="HC2" s="169"/>
+      <c r="HD2" s="169"/>
+      <c r="HE2" s="169"/>
+      <c r="HF2" s="169"/>
+      <c r="HG2" s="169"/>
+      <c r="HH2" s="169"/>
+      <c r="HI2" s="169"/>
+      <c r="HJ2" s="169"/>
+      <c r="HK2" s="169"/>
+      <c r="HL2" s="169"/>
+      <c r="HM2" s="169"/>
+      <c r="HN2" s="169"/>
+      <c r="HO2" s="169"/>
+      <c r="HP2" s="169"/>
+      <c r="HQ2" s="169"/>
+      <c r="HR2" s="169"/>
+      <c r="HS2" s="169"/>
+      <c r="HT2" s="169"/>
+      <c r="HU2" s="169"/>
+      <c r="HV2" s="169"/>
+      <c r="HW2" s="169"/>
+      <c r="HX2" s="169"/>
+      <c r="HY2" s="169"/>
+      <c r="HZ2" s="169"/>
+      <c r="IA2" s="169"/>
+      <c r="IB2" s="169"/>
+      <c r="IC2" s="169"/>
+      <c r="ID2" s="169"/>
+      <c r="IE2" s="169"/>
+      <c r="IF2" s="169"/>
+      <c r="IG2" s="169"/>
+      <c r="IH2" s="169"/>
+      <c r="II2" s="169"/>
+      <c r="IJ2" s="169"/>
+      <c r="IK2" s="169"/>
+      <c r="IL2" s="169"/>
+      <c r="IM2" s="169"/>
+      <c r="IN2" s="169"/>
     </row>
     <row r="3" spans="1:248" s="58" customFormat="1" ht="64">
       <c r="A3" s="49" t="s">
@@ -11384,10 +11388,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="DE2:DI2"/>
-    <mergeCell ref="DJ2:DM2"/>
-    <mergeCell ref="DN2:DS2"/>
-    <mergeCell ref="DT2:EN2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:AM1"/>
@@ -11401,6 +11401,10 @@
     <mergeCell ref="EO2:IN2"/>
     <mergeCell ref="BY2:CI2"/>
     <mergeCell ref="CJ2:DD2"/>
+    <mergeCell ref="DE2:DI2"/>
+    <mergeCell ref="DJ2:DM2"/>
+    <mergeCell ref="DN2:DS2"/>
+    <mergeCell ref="DT2:EN2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>